<commit_message>
Now inserts the more detailed labours and removes the general type!
</commit_message>
<xml_diff>
--- a/excel_files/output.xlsx
+++ b/excel_files/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="83">
   <si>
     <t>C-AAGR</t>
   </si>
@@ -199,12 +199,60 @@
     <t>trade</t>
   </si>
   <si>
+    <t>Labour 112</t>
+  </si>
+  <si>
+    <t>Labour 113</t>
+  </si>
+  <si>
+    <t>Labour 121</t>
+  </si>
+  <si>
+    <t>Labour 122</t>
+  </si>
+  <si>
+    <t>Labour 123</t>
+  </si>
+  <si>
+    <t>Labour 131</t>
+  </si>
+  <si>
+    <t>Labour 132</t>
+  </si>
+  <si>
+    <t>Labour 133</t>
+  </si>
+  <si>
+    <t>Labour 211</t>
+  </si>
+  <si>
+    <t>Labour 212</t>
+  </si>
+  <si>
+    <t>Labour 213</t>
+  </si>
+  <si>
+    <t>Labour 221</t>
+  </si>
+  <si>
+    <t>Labour 222</t>
+  </si>
+  <si>
+    <t>Labour 223</t>
+  </si>
+  <si>
+    <t>Labour 231</t>
+  </si>
+  <si>
+    <t>Labour 232</t>
+  </si>
+  <si>
+    <t>Labour 233</t>
+  </si>
+  <si>
     <t>tmarg</t>
   </si>
   <si>
-    <t>Labour</t>
-  </si>
-  <si>
     <t>Capital</t>
   </si>
   <si>
@@ -215,57 +263,6 @@
   </si>
   <si>
     <t>Labour 111</t>
-  </si>
-  <si>
-    <t>Labour 112</t>
-  </si>
-  <si>
-    <t>Labour 113</t>
-  </si>
-  <si>
-    <t>Labour 121</t>
-  </si>
-  <si>
-    <t>Labour 122</t>
-  </si>
-  <si>
-    <t>Labour 123</t>
-  </si>
-  <si>
-    <t>Labour 131</t>
-  </si>
-  <si>
-    <t>Labour 132</t>
-  </si>
-  <si>
-    <t>Labour 133</t>
-  </si>
-  <si>
-    <t>Labour 211</t>
-  </si>
-  <si>
-    <t>Labour 212</t>
-  </si>
-  <si>
-    <t>Labour 213</t>
-  </si>
-  <si>
-    <t>Labour 221</t>
-  </si>
-  <si>
-    <t>Labour 222</t>
-  </si>
-  <si>
-    <t>Labour 223</t>
-  </si>
-  <si>
-    <t>Labour 231</t>
-  </si>
-  <si>
-    <t>Labour 232</t>
-  </si>
-  <si>
-    <t>Labour 233</t>
   </si>
 </sst>
 </file>
@@ -623,13 +620,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CG85"/>
+  <dimension ref="A1:CE84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:85">
+    <row r="1" spans="1:83">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -876,14 +873,8 @@
       <c r="CE1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="CF1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="CG1" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:85">
+    </row>
+    <row r="2" spans="1:83">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -975,7 +966,7 @@
         <v>932.17</v>
       </c>
     </row>
-    <row r="3" spans="1:85">
+    <row r="3" spans="1:83">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1067,7 +1058,7 @@
         <v>178.78</v>
       </c>
     </row>
-    <row r="4" spans="1:85">
+    <row r="4" spans="1:83">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1159,7 +1150,7 @@
         <v>74302.3</v>
       </c>
     </row>
-    <row r="5" spans="1:85">
+    <row r="5" spans="1:83">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1250,11 +1241,11 @@
       <c r="BJ5">
         <v>17.91</v>
       </c>
-      <c r="BK5">
+      <c r="CB5">
         <v>3864.9</v>
       </c>
     </row>
-    <row r="6" spans="1:85">
+    <row r="6" spans="1:83">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1346,7 +1337,7 @@
         <v>22.91</v>
       </c>
     </row>
-    <row r="7" spans="1:85">
+    <row r="7" spans="1:83">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1438,7 +1429,7 @@
         <v>779.75</v>
       </c>
     </row>
-    <row r="8" spans="1:85">
+    <row r="8" spans="1:83">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1530,7 +1521,7 @@
         <v>863.5599999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:85">
+    <row r="9" spans="1:83">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1621,11 +1612,11 @@
       <c r="BJ9">
         <v>20.63</v>
       </c>
-      <c r="BK9">
+      <c r="CB9">
         <v>12232.23</v>
       </c>
     </row>
-    <row r="10" spans="1:85">
+    <row r="10" spans="1:83">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1711,7 +1702,7 @@
         <v>1.42</v>
       </c>
     </row>
-    <row r="11" spans="1:85">
+    <row r="11" spans="1:83">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1802,11 +1793,11 @@
       <c r="BJ11">
         <v>1944.4</v>
       </c>
-      <c r="BK11">
+      <c r="CB11">
         <v>15632.6</v>
       </c>
     </row>
-    <row r="12" spans="1:85">
+    <row r="12" spans="1:83">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1895,7 +1886,7 @@
         <v>860.4400000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:85">
+    <row r="13" spans="1:83">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1987,7 +1978,7 @@
         <v>13353.97</v>
       </c>
     </row>
-    <row r="14" spans="1:85">
+    <row r="14" spans="1:83">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -2078,11 +2069,11 @@
       <c r="BJ14">
         <v>17170.96</v>
       </c>
-      <c r="BK14">
+      <c r="CB14">
         <v>84802.46000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:85">
+    <row r="15" spans="1:83">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -2173,11 +2164,11 @@
       <c r="BJ15">
         <v>348.75</v>
       </c>
-      <c r="BK15">
+      <c r="CB15">
         <v>2668.03</v>
       </c>
     </row>
-    <row r="16" spans="1:85">
+    <row r="16" spans="1:83">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -2268,11 +2259,11 @@
       <c r="BJ16">
         <v>2683.26</v>
       </c>
-      <c r="BK16">
+      <c r="CB16">
         <v>8239.969999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:63">
+    <row r="17" spans="1:80">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -2363,11 +2354,11 @@
       <c r="BJ17">
         <v>902.08</v>
       </c>
-      <c r="BK17">
+      <c r="CB17">
         <v>212.12</v>
       </c>
     </row>
-    <row r="18" spans="1:63">
+    <row r="18" spans="1:80">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -2456,7 +2447,7 @@
         <v>268.25</v>
       </c>
     </row>
-    <row r="19" spans="1:63">
+    <row r="19" spans="1:80">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -2548,7 +2539,7 @@
         <v>17.16</v>
       </c>
     </row>
-    <row r="20" spans="1:63">
+    <row r="20" spans="1:80">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -2640,7 +2631,7 @@
         <v>19.61</v>
       </c>
     </row>
-    <row r="21" spans="1:63">
+    <row r="21" spans="1:80">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -2723,7 +2714,7 @@
         <v>8.800000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:63">
+    <row r="22" spans="1:80">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -2800,7 +2791,7 @@
         <v>305.05</v>
       </c>
     </row>
-    <row r="23" spans="1:63">
+    <row r="23" spans="1:80">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -2892,7 +2883,7 @@
         <v>521.4400000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:63">
+    <row r="24" spans="1:80">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -2984,7 +2975,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="25" spans="1:63">
+    <row r="25" spans="1:80">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -3073,7 +3064,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="26" spans="1:63">
+    <row r="26" spans="1:80">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -3165,7 +3156,7 @@
         <v>886.08</v>
       </c>
     </row>
-    <row r="27" spans="1:63">
+    <row r="27" spans="1:80">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -3257,7 +3248,7 @@
         <v>42.01</v>
       </c>
     </row>
-    <row r="28" spans="1:63">
+    <row r="28" spans="1:80">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
@@ -3340,7 +3331,7 @@
         <v>36.54</v>
       </c>
     </row>
-    <row r="29" spans="1:63">
+    <row r="29" spans="1:80">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
@@ -3426,7 +3417,7 @@
         <v>8314.83</v>
       </c>
     </row>
-    <row r="30" spans="1:63">
+    <row r="30" spans="1:80">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
@@ -3514,11 +3505,11 @@
       <c r="BI30">
         <v>0.39</v>
       </c>
-      <c r="BK30">
+      <c r="CB30">
         <v>578.79</v>
       </c>
     </row>
-    <row r="31" spans="1:63">
+    <row r="31" spans="1:80">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
@@ -3609,11 +3600,11 @@
       <c r="BJ31">
         <v>64.92</v>
       </c>
-      <c r="BK31">
+      <c r="CB31">
         <v>138.26</v>
       </c>
     </row>
-    <row r="32" spans="1:63">
+    <row r="32" spans="1:80">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
@@ -3704,7 +3695,7 @@
       <c r="BJ32">
         <v>888.9299999999999</v>
       </c>
-      <c r="BK32">
+      <c r="CB32">
         <v>3303.91</v>
       </c>
     </row>
@@ -4520,7 +4511,7 @@
         <v>3.27</v>
       </c>
     </row>
-    <row r="49" spans="1:67">
+    <row r="49" spans="1:83">
       <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
@@ -4576,7 +4567,7 @@
         <v>6.15</v>
       </c>
     </row>
-    <row r="50" spans="1:67">
+    <row r="50" spans="1:83">
       <c r="A50" s="1" t="s">
         <v>48</v>
       </c>
@@ -4632,7 +4623,7 @@
         <v>18.06</v>
       </c>
     </row>
-    <row r="51" spans="1:67">
+    <row r="51" spans="1:83">
       <c r="A51" s="1" t="s">
         <v>49</v>
       </c>
@@ -4688,7 +4679,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="52" spans="1:67">
+    <row r="52" spans="1:83">
       <c r="A52" s="1" t="s">
         <v>50</v>
       </c>
@@ -4705,7 +4696,7 @@
         <v>12.62</v>
       </c>
     </row>
-    <row r="53" spans="1:67">
+    <row r="53" spans="1:83">
       <c r="A53" s="1" t="s">
         <v>51</v>
       </c>
@@ -4722,7 +4713,7 @@
         <v>86.53</v>
       </c>
     </row>
-    <row r="54" spans="1:67">
+    <row r="54" spans="1:83">
       <c r="A54" s="1" t="s">
         <v>52</v>
       </c>
@@ -4742,7 +4733,7 @@
         <v>3418.74</v>
       </c>
     </row>
-    <row r="55" spans="1:67">
+    <row r="55" spans="1:83">
       <c r="A55" s="1" t="s">
         <v>53</v>
       </c>
@@ -4777,7 +4768,7 @@
         <v>36500.62</v>
       </c>
     </row>
-    <row r="56" spans="1:67">
+    <row r="56" spans="1:83">
       <c r="A56" s="1" t="s">
         <v>54</v>
       </c>
@@ -4809,7 +4800,7 @@
         <v>3985.92</v>
       </c>
     </row>
-    <row r="57" spans="1:67">
+    <row r="57" spans="1:83">
       <c r="A57" s="1" t="s">
         <v>55</v>
       </c>
@@ -4838,32 +4829,29 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="58" spans="1:67">
+    <row r="58" spans="1:83">
       <c r="A58" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="BL58">
-        <v>131530.1</v>
-      </c>
-      <c r="BM58">
+      <c r="CC58">
         <v>112199.01</v>
       </c>
     </row>
-    <row r="59" spans="1:67">
+    <row r="59" spans="1:83">
       <c r="A59" s="1" t="s">
         <v>57</v>
       </c>
       <c r="BJ59">
         <v>36958.79</v>
       </c>
-      <c r="BN59">
+      <c r="CD59">
         <v>4774.3</v>
       </c>
-      <c r="BO59">
+      <c r="CE59">
         <v>9930.33</v>
       </c>
     </row>
-    <row r="60" spans="1:67">
+    <row r="60" spans="1:83">
       <c r="A60" s="1" t="s">
         <v>58</v>
       </c>
@@ -4871,7 +4859,7 @@
         <v>60156.74</v>
       </c>
     </row>
-    <row r="61" spans="1:67">
+    <row r="61" spans="1:83">
       <c r="A61" s="1" t="s">
         <v>59</v>
       </c>
@@ -4879,7 +4867,7 @@
         <v>3839.16</v>
       </c>
     </row>
-    <row r="62" spans="1:67">
+    <row r="62" spans="1:83">
       <c r="A62" s="1" t="s">
         <v>60</v>
       </c>
@@ -4977,9 +4965,9 @@
         <v>51297.1</v>
       </c>
     </row>
-    <row r="63" spans="1:67">
+    <row r="63" spans="1:83">
       <c r="A63" s="1" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="B63">
         <v>1653.21</v>
@@ -5078,1722 +5066,1645 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="64" spans="1:67">
+    <row r="64" spans="1:83">
       <c r="A64" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH64">
+        <v>9.414114025598392</v>
+      </c>
+      <c r="AI64">
+        <v>4.98343871824909</v>
+      </c>
+      <c r="AJ64">
+        <v>200.4209536320157</v>
+      </c>
+      <c r="AK64">
+        <v>4.98343871824909</v>
+      </c>
+      <c r="AL64">
+        <v>200.4209536320157</v>
+      </c>
+      <c r="AN64">
+        <v>3.583830243987031</v>
+      </c>
+      <c r="AO64">
+        <v>3.583830243987031</v>
+      </c>
+      <c r="AP64">
+        <v>11.83001546522602</v>
+      </c>
+      <c r="AQ64">
+        <v>0.882314035994932</v>
+      </c>
+      <c r="AR64">
+        <v>0.882314035994932</v>
+      </c>
+      <c r="AS64">
+        <v>73.19743904368953</v>
+      </c>
+      <c r="AT64">
+        <v>192.0036300258339</v>
+      </c>
+      <c r="AU64">
+        <v>192.0036300258339</v>
+      </c>
+      <c r="AV64">
+        <v>192.0036300258339</v>
+      </c>
+      <c r="AW64">
+        <v>8.166333993524313</v>
+      </c>
+      <c r="AX64">
+        <v>22.61657591545954</v>
+      </c>
+      <c r="AY64">
+        <v>0.6143333348818123</v>
+      </c>
+      <c r="AZ64">
+        <v>38.40820165850223</v>
+      </c>
+      <c r="BA64">
+        <v>38.40820165850223</v>
+      </c>
+      <c r="BB64">
+        <v>38.40820165850223</v>
+      </c>
+      <c r="BC64">
+        <v>38.40820165850223</v>
+      </c>
+      <c r="BD64">
+        <v>38.40820165850223</v>
+      </c>
+      <c r="BE64">
+        <v>0.6143333348818123</v>
+      </c>
+    </row>
+    <row r="65" spans="1:57">
+      <c r="A65" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH65">
+        <v>59.33229717329145</v>
+      </c>
+      <c r="AI65">
+        <v>52.88727739527822</v>
+      </c>
+      <c r="AJ65">
+        <v>2386.627410095036</v>
+      </c>
+      <c r="AK65">
+        <v>52.88727739527822</v>
+      </c>
+      <c r="AL65">
+        <v>2386.627410095036</v>
+      </c>
+      <c r="AN65">
+        <v>16.82216917671263</v>
+      </c>
+      <c r="AO65">
+        <v>16.82216917671263</v>
+      </c>
+      <c r="AP65">
+        <v>75.89979358144105</v>
+      </c>
+      <c r="AQ65">
+        <v>9.907512448914348</v>
+      </c>
+      <c r="AR65">
+        <v>9.907512448914348</v>
+      </c>
+      <c r="AS65">
+        <v>168.617042367179</v>
+      </c>
+      <c r="AT65">
+        <v>337.3299611688592</v>
+      </c>
+      <c r="AU65">
+        <v>337.3299611688592</v>
+      </c>
+      <c r="AV65">
+        <v>337.3299611688592</v>
+      </c>
+      <c r="AW65">
+        <v>15.90577829927206</v>
+      </c>
+      <c r="AX65">
+        <v>164.5034938763827</v>
+      </c>
+      <c r="AY65">
+        <v>2.83422336127609</v>
+      </c>
+      <c r="AZ65">
+        <v>111.1287621074915</v>
+      </c>
+      <c r="BA65">
+        <v>111.1287621074915</v>
+      </c>
+      <c r="BB65">
+        <v>111.1287621074915</v>
+      </c>
+      <c r="BC65">
+        <v>111.1287621074915</v>
+      </c>
+      <c r="BD65">
+        <v>111.1287621074915</v>
+      </c>
+      <c r="BE65">
+        <v>2.83422336127609</v>
+      </c>
+    </row>
+    <row r="66" spans="1:57">
+      <c r="A66" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AH64">
-        <v>606.71</v>
-      </c>
-      <c r="AI64">
-        <v>2.48</v>
-      </c>
-      <c r="AJ64">
-        <v>288.04</v>
-      </c>
-      <c r="AK64">
-        <v>1467.42</v>
-      </c>
-      <c r="AL64">
-        <v>25315.67</v>
-      </c>
-      <c r="AM64">
-        <v>496.89</v>
-      </c>
-      <c r="AN64">
-        <v>115.12</v>
-      </c>
-      <c r="AO64">
-        <v>464.11</v>
-      </c>
-      <c r="AP64">
-        <v>1077.97</v>
-      </c>
-      <c r="AQ64">
-        <v>238.76</v>
-      </c>
-      <c r="AR64">
-        <v>10.19</v>
-      </c>
-      <c r="AS64">
-        <v>6546.59</v>
-      </c>
-      <c r="AT64">
-        <v>9171.24</v>
-      </c>
-      <c r="AU64">
-        <v>16888.18</v>
-      </c>
-      <c r="AV64">
-        <v>39974.96</v>
-      </c>
-      <c r="AW64">
-        <v>350.8</v>
-      </c>
-      <c r="AX64">
-        <v>3612.7</v>
-      </c>
-      <c r="AY64">
-        <v>172.44</v>
-      </c>
-      <c r="AZ64">
-        <v>1.93</v>
-      </c>
-      <c r="BA64">
-        <v>14.36</v>
-      </c>
-      <c r="BB64">
-        <v>507.79</v>
-      </c>
-      <c r="BC64">
-        <v>23024.77</v>
-      </c>
-      <c r="BD64">
-        <v>1162.91</v>
-      </c>
-      <c r="BE64">
-        <v>18.08</v>
-      </c>
-    </row>
-    <row r="65" spans="1:65">
-      <c r="A65" s="1" t="s">
+      <c r="AH66">
+        <v>7.205654163155705</v>
+      </c>
+      <c r="AI66">
+        <v>4.216897656582296</v>
+      </c>
+      <c r="AJ66">
+        <v>424.28795445811</v>
+      </c>
+      <c r="AK66">
+        <v>4.216897656582296</v>
+      </c>
+      <c r="AL66">
+        <v>424.28795445811</v>
+      </c>
+      <c r="AN66">
+        <v>3.524966271901503</v>
+      </c>
+      <c r="AO66">
+        <v>3.524966271901503</v>
+      </c>
+      <c r="AP66">
+        <v>14.83037091043778</v>
+      </c>
+      <c r="AQ66">
+        <v>2.587943928549066</v>
+      </c>
+      <c r="AR66">
+        <v>2.587943928549066</v>
+      </c>
+      <c r="AS66">
+        <v>15.87995030975901</v>
+      </c>
+      <c r="AT66">
+        <v>95.40936142164284</v>
+      </c>
+      <c r="AU66">
+        <v>95.40936142164284</v>
+      </c>
+      <c r="AV66">
+        <v>95.40936142164284</v>
+      </c>
+      <c r="AW66">
+        <v>4.508362703770399</v>
+      </c>
+      <c r="AX66">
+        <v>20.73699029148556</v>
+      </c>
+      <c r="AY66">
+        <v>0.6809700198937206</v>
+      </c>
+      <c r="AZ66">
+        <v>24.04094541568309</v>
+      </c>
+      <c r="BA66">
+        <v>24.04094541568309</v>
+      </c>
+      <c r="BB66">
+        <v>24.04094541568309</v>
+      </c>
+      <c r="BC66">
+        <v>24.04094541568309</v>
+      </c>
+      <c r="BD66">
+        <v>24.04094541568309</v>
+      </c>
+      <c r="BE66">
+        <v>0.6809700198937206</v>
+      </c>
+    </row>
+    <row r="67" spans="1:57">
+      <c r="A67" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AH65">
+      <c r="AH67">
+        <v>85.96996595606208</v>
+      </c>
+      <c r="AI67">
+        <v>45.81034803465009</v>
+      </c>
+      <c r="AJ67">
+        <v>1067.650717165209</v>
+      </c>
+      <c r="AK67">
+        <v>45.81034803465009</v>
+      </c>
+      <c r="AL67">
+        <v>1067.650717165209</v>
+      </c>
+      <c r="AN67">
+        <v>21.2452943026647</v>
+      </c>
+      <c r="AO67">
+        <v>21.2452943026647</v>
+      </c>
+      <c r="AP67">
+        <v>67.45605026192963</v>
+      </c>
+      <c r="AQ67">
+        <v>3.648380930209532</v>
+      </c>
+      <c r="AR67">
+        <v>3.648380930209532</v>
+      </c>
+      <c r="AS67">
+        <v>1017.25321948424</v>
+      </c>
+      <c r="AT67">
+        <v>2296.914724432677</v>
+      </c>
+      <c r="AU67">
+        <v>2296.914724432677</v>
+      </c>
+      <c r="AV67">
+        <v>2296.914724432677</v>
+      </c>
+      <c r="AW67">
+        <v>57.67828812599182</v>
+      </c>
+      <c r="AX67">
+        <v>253.528219165653</v>
+      </c>
+      <c r="AY67">
+        <v>6.298046703189611</v>
+      </c>
+      <c r="AZ67">
+        <v>533.8607489335537</v>
+      </c>
+      <c r="BA67">
+        <v>533.8607489335537</v>
+      </c>
+      <c r="BB67">
+        <v>533.8607489335537</v>
+      </c>
+      <c r="BC67">
+        <v>533.8607489335537</v>
+      </c>
+      <c r="BD67">
+        <v>533.8607489335537</v>
+      </c>
+      <c r="BE67">
+        <v>6.298046703189611</v>
+      </c>
+    </row>
+    <row r="68" spans="1:57">
+      <c r="A68" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AH68">
+        <v>210.7794315168262</v>
+      </c>
+      <c r="AI68">
+        <v>300.8081789076329</v>
+      </c>
+      <c r="AJ68">
+        <v>4553.744405761063</v>
+      </c>
+      <c r="AK68">
+        <v>300.8081789076329</v>
+      </c>
+      <c r="AL68">
+        <v>4553.744405761063</v>
+      </c>
+      <c r="AN68">
+        <v>71.71276636935771</v>
+      </c>
+      <c r="AO68">
+        <v>71.71276636935771</v>
+      </c>
+      <c r="AP68">
+        <v>425.0448387694359</v>
+      </c>
+      <c r="AQ68">
+        <v>24.91756613589823</v>
+      </c>
+      <c r="AR68">
+        <v>24.91756613589823</v>
+      </c>
+      <c r="AS68">
+        <v>1199.389830690175</v>
+      </c>
+      <c r="AT68">
+        <v>3500.822733426095</v>
+      </c>
+      <c r="AU68">
+        <v>3500.822733426095</v>
+      </c>
+      <c r="AV68">
+        <v>3500.822733426095</v>
+      </c>
+      <c r="AW68">
+        <v>55.08900470733643</v>
+      </c>
+      <c r="AX68">
+        <v>787.1122351065278</v>
+      </c>
+      <c r="AY68">
+        <v>7.304603953659534</v>
+      </c>
+      <c r="AZ68">
+        <v>521.6428579665424</v>
+      </c>
+      <c r="BA68">
+        <v>521.6428579665424</v>
+      </c>
+      <c r="BB68">
+        <v>521.6428579665424</v>
+      </c>
+      <c r="BC68">
+        <v>521.6428579665424</v>
+      </c>
+      <c r="BD68">
+        <v>521.6428579665424</v>
+      </c>
+      <c r="BE68">
+        <v>7.304603953659534</v>
+      </c>
+    </row>
+    <row r="69" spans="1:57">
+      <c r="A69" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH69">
+        <v>17.85041145477444</v>
+      </c>
+      <c r="AI69">
+        <v>28.15027438197285</v>
+      </c>
+      <c r="AJ69">
+        <v>377.6822184351739</v>
+      </c>
+      <c r="AK69">
+        <v>28.15027438197285</v>
+      </c>
+      <c r="AL69">
+        <v>377.6822184351739</v>
+      </c>
+      <c r="AN69">
+        <v>4.714462637193501</v>
+      </c>
+      <c r="AO69">
+        <v>4.714462637193501</v>
+      </c>
+      <c r="AP69">
+        <v>49.16584968741984</v>
+      </c>
+      <c r="AQ69">
+        <v>2.893772782757878</v>
+      </c>
+      <c r="AR69">
+        <v>2.893772782757878</v>
+      </c>
+      <c r="AS69">
+        <v>33.3963167022774</v>
+      </c>
+      <c r="AT69">
+        <v>255.6969061620534</v>
+      </c>
+      <c r="AU69">
+        <v>255.6969061620534</v>
+      </c>
+      <c r="AV69">
+        <v>255.6969061620534</v>
+      </c>
+      <c r="AW69">
+        <v>5.374387093633413</v>
+      </c>
+      <c r="AX69">
+        <v>25.69650055831298</v>
+      </c>
+      <c r="AY69">
+        <v>0.2742241334868595</v>
+      </c>
+      <c r="AZ69">
+        <v>44.71875981566311</v>
+      </c>
+      <c r="BA69">
+        <v>44.71875981566311</v>
+      </c>
+      <c r="BB69">
+        <v>44.71875981566311</v>
+      </c>
+      <c r="BC69">
+        <v>44.71875981566311</v>
+      </c>
+      <c r="BD69">
+        <v>44.71875981566311</v>
+      </c>
+      <c r="BE69">
+        <v>0.2742241334868595</v>
+      </c>
+    </row>
+    <row r="70" spans="1:57">
+      <c r="A70" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH70">
+        <v>22.72248552095145</v>
+      </c>
+      <c r="AI70">
+        <v>26.40249624270946</v>
+      </c>
+      <c r="AJ70">
+        <v>551.2811292873323</v>
+      </c>
+      <c r="AK70">
+        <v>26.40249624270946</v>
+      </c>
+      <c r="AL70">
+        <v>551.2811292873323</v>
+      </c>
+      <c r="AN70">
+        <v>4.544429623456672</v>
+      </c>
+      <c r="AO70">
+        <v>4.544429623456672</v>
+      </c>
+      <c r="AP70">
+        <v>15.6135156785883</v>
+      </c>
+      <c r="AQ70">
+        <v>1.124677603738382</v>
+      </c>
+      <c r="AR70">
+        <v>1.124677603738382</v>
+      </c>
+      <c r="AS70">
+        <v>224.3877803584561</v>
+      </c>
+      <c r="AT70">
+        <v>1211.574020833299</v>
+      </c>
+      <c r="AU70">
+        <v>1211.574020833299</v>
+      </c>
+      <c r="AV70">
+        <v>1211.574020833299</v>
+      </c>
+      <c r="AW70">
+        <v>13.75366018712521</v>
+      </c>
+      <c r="AX70">
+        <v>151.1198314923793</v>
+      </c>
+      <c r="AY70">
+        <v>4.972760506421327</v>
+      </c>
+      <c r="AZ70">
+        <v>185.2030471046567</v>
+      </c>
+      <c r="BA70">
+        <v>185.2030471046567</v>
+      </c>
+      <c r="BB70">
+        <v>185.2030471046567</v>
+      </c>
+      <c r="BC70">
+        <v>185.2030471046567</v>
+      </c>
+      <c r="BD70">
+        <v>185.2030471046567</v>
+      </c>
+      <c r="BE70">
+        <v>4.972760506421327</v>
+      </c>
+    </row>
+    <row r="71" spans="1:57">
+      <c r="A71" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH71">
+        <v>86.79474751248956</v>
+      </c>
+      <c r="AI71">
+        <v>139.8593661420047</v>
+      </c>
+      <c r="AJ71">
+        <v>1530.035279196426</v>
+      </c>
+      <c r="AK71">
+        <v>139.8593661420047</v>
+      </c>
+      <c r="AL71">
+        <v>1530.035279196426</v>
+      </c>
+      <c r="AN71">
+        <v>27.99167295109481</v>
+      </c>
+      <c r="AO71">
+        <v>27.99167295109481</v>
+      </c>
+      <c r="AP71">
+        <v>188.5514367929101</v>
+      </c>
+      <c r="AQ71">
+        <v>9.954080538451672</v>
+      </c>
+      <c r="AR71">
+        <v>9.954080538451672</v>
+      </c>
+      <c r="AS71">
+        <v>898.22598473683</v>
+      </c>
+      <c r="AT71">
+        <v>3174.076085808873</v>
+      </c>
+      <c r="AU71">
+        <v>3174.076085808873</v>
+      </c>
+      <c r="AV71">
+        <v>3174.076085808873</v>
+      </c>
+      <c r="AW71">
+        <v>25.92668635845184</v>
+      </c>
+      <c r="AX71">
+        <v>885.2735020026564</v>
+      </c>
+      <c r="AY71">
+        <v>4.723041579052805</v>
+      </c>
+      <c r="AZ71">
+        <v>223.8124471736551</v>
+      </c>
+      <c r="BA71">
+        <v>223.8124471736551</v>
+      </c>
+      <c r="BB71">
+        <v>223.8124471736551</v>
+      </c>
+      <c r="BC71">
+        <v>223.8124471736551</v>
+      </c>
+      <c r="BD71">
+        <v>223.8124471736551</v>
+      </c>
+      <c r="BE71">
+        <v>4.723041579052805</v>
+      </c>
+    </row>
+    <row r="72" spans="1:57">
+      <c r="A72" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AH72">
+        <v>13.98811280122027</v>
+      </c>
+      <c r="AI72">
+        <v>15.2970779588446</v>
+      </c>
+      <c r="AJ72">
+        <v>153.0186887697224</v>
+      </c>
+      <c r="AK72">
+        <v>15.2970779588446</v>
+      </c>
+      <c r="AL72">
+        <v>153.0186887697224</v>
+      </c>
+      <c r="AN72">
+        <v>3.391067505558021</v>
+      </c>
+      <c r="AO72">
+        <v>3.391067505558021</v>
+      </c>
+      <c r="AP72">
+        <v>36.30120203226805</v>
+      </c>
+      <c r="AQ72">
+        <v>1.918124681361951</v>
+      </c>
+      <c r="AR72">
+        <v>1.918124681361951</v>
+      </c>
+      <c r="AS72">
+        <v>89.16462504421361</v>
+      </c>
+      <c r="AT72">
+        <v>210.5832067055814</v>
+      </c>
+      <c r="AU72">
+        <v>210.5832067055814</v>
+      </c>
+      <c r="AV72">
+        <v>210.5832067055814</v>
+      </c>
+      <c r="AW72">
+        <v>5.622723040729761</v>
+      </c>
+      <c r="AX72">
+        <v>36.43868462974206</v>
+      </c>
+      <c r="AY72">
+        <v>0.2696506427740678</v>
+      </c>
+      <c r="AZ72">
+        <v>61.94066436254979</v>
+      </c>
+      <c r="BA72">
+        <v>61.94066436254979</v>
+      </c>
+      <c r="BB72">
+        <v>61.94066436254979</v>
+      </c>
+      <c r="BC72">
+        <v>61.94066436254979</v>
+      </c>
+      <c r="BD72">
+        <v>61.94066436254979</v>
+      </c>
+      <c r="BE72">
+        <v>0.2696506427740678</v>
+      </c>
+    </row>
+    <row r="73" spans="1:57">
+      <c r="A73" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AH73">
+        <v>20.77479004822672</v>
+      </c>
+      <c r="AI73">
+        <v>4.852747014700435</v>
+      </c>
+      <c r="AJ73">
+        <v>48.24235908871516</v>
+      </c>
+      <c r="AK73">
+        <v>4.852747014700435</v>
+      </c>
+      <c r="AL73">
+        <v>48.24235908871516</v>
+      </c>
+      <c r="AN73">
+        <v>4.100118934209458</v>
+      </c>
+      <c r="AO73">
+        <v>4.100118934209458</v>
+      </c>
+      <c r="AP73">
+        <v>5.887614787886851</v>
+      </c>
+      <c r="AQ73">
+        <v>1.975540813524276</v>
+      </c>
+      <c r="AR73">
+        <v>1.975540813524276</v>
+      </c>
+      <c r="AS73">
+        <v>94.09361228807829</v>
+      </c>
+      <c r="AT73">
+        <v>432.1870895471797</v>
+      </c>
+      <c r="AU73">
+        <v>432.1870895471797</v>
+      </c>
+      <c r="AV73">
+        <v>432.1870895471797</v>
+      </c>
+      <c r="AW73">
+        <v>7.274246802926064</v>
+      </c>
+      <c r="AX73">
+        <v>48.43849489577114</v>
+      </c>
+      <c r="AY73">
+        <v>2.568719942420721</v>
+      </c>
+      <c r="AZ73">
+        <v>96.82042559319736</v>
+      </c>
+      <c r="BA73">
+        <v>96.82042559319736</v>
+      </c>
+      <c r="BB73">
+        <v>96.82042559319736</v>
+      </c>
+      <c r="BC73">
+        <v>96.82042559319736</v>
+      </c>
+      <c r="BD73">
+        <v>96.82042559319736</v>
+      </c>
+      <c r="BE73">
+        <v>2.568719942420721</v>
+      </c>
+    </row>
+    <row r="74" spans="1:57">
+      <c r="A74" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AH74">
+        <v>6.972353674806655</v>
+      </c>
+      <c r="AI74">
+        <v>12.21744870962575</v>
+      </c>
+      <c r="AJ74">
+        <v>199.71937682949</v>
+      </c>
+      <c r="AK74">
+        <v>12.21744870962575</v>
+      </c>
+      <c r="AL74">
+        <v>199.71937682949</v>
+      </c>
+      <c r="AN74">
+        <v>18.19257926173508</v>
+      </c>
+      <c r="AO74">
+        <v>18.19257926173508</v>
+      </c>
+      <c r="AP74">
+        <v>18.15562672873959</v>
+      </c>
+      <c r="AQ74">
+        <v>11.11295016352087</v>
+      </c>
+      <c r="AR74">
+        <v>11.11295016352087</v>
+      </c>
+      <c r="AS74">
+        <v>263.5501914815977</v>
+      </c>
+      <c r="AT74">
+        <v>908.7285465851427</v>
+      </c>
+      <c r="AU74">
+        <v>908.7285465851427</v>
+      </c>
+      <c r="AV74">
+        <v>908.7285465851427</v>
+      </c>
+      <c r="AW74">
+        <v>15.00309596955776</v>
+      </c>
+      <c r="AX74">
+        <v>157.2740013517439</v>
+      </c>
+      <c r="AY74">
+        <v>10.54452222824097</v>
+      </c>
+      <c r="AZ74">
+        <v>341.338813333869</v>
+      </c>
+      <c r="BA74">
+        <v>341.338813333869</v>
+      </c>
+      <c r="BB74">
+        <v>341.338813333869</v>
+      </c>
+      <c r="BC74">
+        <v>341.338813333869</v>
+      </c>
+      <c r="BD74">
+        <v>341.338813333869</v>
+      </c>
+      <c r="BE74">
+        <v>10.54452222824097</v>
+      </c>
+    </row>
+    <row r="75" spans="1:57">
+      <c r="A75" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AH75">
+        <v>0.5680094407271827</v>
+      </c>
+      <c r="AI75">
+        <v>0.6389008355734405</v>
+      </c>
+      <c r="AJ75">
+        <v>21.40426394213398</v>
+      </c>
+      <c r="AK75">
+        <v>0.6389008355734405</v>
+      </c>
+      <c r="AL75">
+        <v>21.40426394213398</v>
+      </c>
+      <c r="AN75">
+        <v>3.499278473271989</v>
+      </c>
+      <c r="AO75">
+        <v>3.499278473271989</v>
+      </c>
+      <c r="AP75">
+        <v>2.967877806534525</v>
+      </c>
+      <c r="AQ75">
+        <v>2.793893166305497</v>
+      </c>
+      <c r="AR75">
+        <v>2.793893166305497</v>
+      </c>
+      <c r="AS75">
+        <v>14.40585431333166</v>
+      </c>
+      <c r="AT75">
+        <v>100.455687204795</v>
+      </c>
+      <c r="AU75">
+        <v>100.455687204795</v>
+      </c>
+      <c r="AV75">
+        <v>100.455687204795</v>
+      </c>
+      <c r="AW75">
+        <v>2.471739122271538</v>
+      </c>
+      <c r="AX75">
+        <v>3.190947880822932</v>
+      </c>
+      <c r="AY75">
+        <v>0.3704864161368459</v>
+      </c>
+      <c r="AZ75">
+        <v>79.33680799412728</v>
+      </c>
+      <c r="BA75">
+        <v>79.33680799412728</v>
+      </c>
+      <c r="BB75">
+        <v>79.33680799412728</v>
+      </c>
+      <c r="BC75">
+        <v>79.33680799412728</v>
+      </c>
+      <c r="BD75">
+        <v>79.33680799412728</v>
+      </c>
+      <c r="BE75">
+        <v>0.3704864161368459</v>
+      </c>
+    </row>
+    <row r="76" spans="1:57">
+      <c r="A76" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AH76">
+        <v>14.58600710416213</v>
+      </c>
+      <c r="AI76">
+        <v>20.80613398961723</v>
+      </c>
+      <c r="AJ76">
+        <v>203.2207749169506</v>
+      </c>
+      <c r="AK76">
+        <v>20.80613398961723</v>
+      </c>
+      <c r="AL76">
+        <v>203.2207749169506</v>
+      </c>
+      <c r="AN76">
+        <v>15.73506095610559</v>
+      </c>
+      <c r="AO76">
+        <v>15.73506095610559</v>
+      </c>
+      <c r="AP76">
+        <v>25.33586614327505</v>
+      </c>
+      <c r="AQ76">
+        <v>4.656144000031054</v>
+      </c>
+      <c r="AR76">
+        <v>4.656144000031054</v>
+      </c>
+      <c r="AS76">
+        <v>629.8837321466208</v>
+      </c>
+      <c r="AT76">
+        <v>2327.148932623268</v>
+      </c>
+      <c r="AU76">
+        <v>2327.148932623268</v>
+      </c>
+      <c r="AV76">
+        <v>2327.148932623268</v>
+      </c>
+      <c r="AW76">
+        <v>40.31813014149666</v>
+      </c>
+      <c r="AX76">
+        <v>221.5278009824455</v>
+      </c>
+      <c r="AY76">
+        <v>11.62228437572718</v>
+      </c>
+      <c r="AZ76">
+        <v>658.5692046878339</v>
+      </c>
+      <c r="BA76">
+        <v>658.5692046878339</v>
+      </c>
+      <c r="BB76">
+        <v>658.5692046878339</v>
+      </c>
+      <c r="BC76">
+        <v>658.5692046878339</v>
+      </c>
+      <c r="BD76">
+        <v>658.5692046878339</v>
+      </c>
+      <c r="BE76">
+        <v>11.62228437572718</v>
+      </c>
+    </row>
+    <row r="77" spans="1:57">
+      <c r="A77" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AH77">
+        <v>22.16415098886937</v>
+      </c>
+      <c r="AI77">
+        <v>49.84443322978914</v>
+      </c>
+      <c r="AJ77">
+        <v>674.1897927421331</v>
+      </c>
+      <c r="AK77">
+        <v>49.84443322978914</v>
+      </c>
+      <c r="AL77">
+        <v>674.1897927421331</v>
+      </c>
+      <c r="AN77">
+        <v>58.49801138035953</v>
+      </c>
+      <c r="AO77">
+        <v>58.49801138035953</v>
+      </c>
+      <c r="AP77">
+        <v>90.24182404957712</v>
+      </c>
+      <c r="AQ77">
+        <v>24.82541301250458</v>
+      </c>
+      <c r="AR77">
+        <v>24.82541301250458</v>
+      </c>
+      <c r="AS77">
+        <v>1220.66968123287</v>
+      </c>
+      <c r="AT77">
+        <v>3909.166663952172</v>
+      </c>
+      <c r="AU77">
+        <v>3909.166663952172</v>
+      </c>
+      <c r="AV77">
+        <v>3909.166663952172</v>
+      </c>
+      <c r="AW77">
+        <v>51.75319621562958</v>
+      </c>
+      <c r="AX77">
+        <v>509.3750439479947</v>
+      </c>
+      <c r="AY77">
+        <v>25.97905255854129</v>
+      </c>
+      <c r="AZ77">
+        <v>1172.28277120328</v>
+      </c>
+      <c r="BA77">
+        <v>1172.28277120328</v>
+      </c>
+      <c r="BB77">
+        <v>1172.28277120328</v>
+      </c>
+      <c r="BC77">
+        <v>1172.28277120328</v>
+      </c>
+      <c r="BD77">
+        <v>1172.28277120328</v>
+      </c>
+      <c r="BE77">
+        <v>25.97905255854129</v>
+      </c>
+    </row>
+    <row r="78" spans="1:57">
+      <c r="A78" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AH78">
+        <v>0.4406759691750631</v>
+      </c>
+      <c r="AI78">
+        <v>7.213819674542174</v>
+      </c>
+      <c r="AJ78">
+        <v>74.40975860358914</v>
+      </c>
+      <c r="AK78">
+        <v>7.213819674542174</v>
+      </c>
+      <c r="AL78">
+        <v>74.40975860358914</v>
+      </c>
+      <c r="AN78">
+        <v>5.620547629725189</v>
+      </c>
+      <c r="AO78">
+        <v>5.620547629725189</v>
+      </c>
+      <c r="AP78">
+        <v>11.42237053900957</v>
+      </c>
+      <c r="AQ78">
+        <v>6.340353480260819</v>
+      </c>
+      <c r="AR78">
+        <v>6.340353480260819</v>
+      </c>
+      <c r="AS78">
+        <v>47.1778669777466</v>
+      </c>
+      <c r="AT78">
+        <v>121.1692079006415</v>
+      </c>
+      <c r="AU78">
+        <v>121.1692079006415</v>
+      </c>
+      <c r="AV78">
+        <v>121.1692079006415</v>
+      </c>
+      <c r="AW78">
+        <v>9.171287022531033</v>
+      </c>
+      <c r="AX78">
+        <v>30.8258233175613</v>
+      </c>
+      <c r="AY78">
+        <v>2.15244241643697</v>
+      </c>
+      <c r="AZ78">
+        <v>94.26668654054404</v>
+      </c>
+      <c r="BA78">
+        <v>94.26668654054404</v>
+      </c>
+      <c r="BB78">
+        <v>94.26668654054404</v>
+      </c>
+      <c r="BC78">
+        <v>94.26668654054404</v>
+      </c>
+      <c r="BD78">
+        <v>94.26668654054404</v>
+      </c>
+      <c r="BE78">
+        <v>2.15244241643697</v>
+      </c>
+    </row>
+    <row r="79" spans="1:57">
+      <c r="A79" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH79">
+        <v>10.65145417792723</v>
+      </c>
+      <c r="AI79">
+        <v>4.660319383302704</v>
+      </c>
+      <c r="AJ79">
+        <v>39.81580099688144</v>
+      </c>
+      <c r="AK79">
+        <v>4.660319383302704</v>
+      </c>
+      <c r="AL79">
+        <v>39.81580099688144</v>
+      </c>
+      <c r="AN79">
+        <v>2.638983073509298</v>
+      </c>
+      <c r="AO79">
+        <v>2.638983073509298</v>
+      </c>
+      <c r="AP79">
+        <v>2.937615607588086</v>
+      </c>
+      <c r="AQ79">
+        <v>1.239205213543028</v>
+      </c>
+      <c r="AR79">
+        <v>1.239205213543028</v>
+      </c>
+      <c r="AS79">
+        <v>64.8387075754907</v>
+      </c>
+      <c r="AT79">
+        <v>415.808921625279</v>
+      </c>
+      <c r="AU79">
+        <v>415.808921625279</v>
+      </c>
+      <c r="AV79">
+        <v>415.808921625279</v>
+      </c>
+      <c r="AW79">
+        <v>7.183363182842732</v>
+      </c>
+      <c r="AX79">
+        <v>100.2953584484756</v>
+      </c>
+      <c r="AY79">
+        <v>4.522884311899542</v>
+      </c>
+      <c r="AZ79">
+        <v>203.228815502882</v>
+      </c>
+      <c r="BA79">
+        <v>203.228815502882</v>
+      </c>
+      <c r="BB79">
+        <v>203.228815502882</v>
+      </c>
+      <c r="BC79">
+        <v>203.228815502882</v>
+      </c>
+      <c r="BD79">
+        <v>203.228815502882</v>
+      </c>
+      <c r="BE79">
+        <v>4.522884311899542</v>
+      </c>
+    </row>
+    <row r="80" spans="1:57">
+      <c r="A80" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AH80">
+        <v>13.45798746185377</v>
+      </c>
+      <c r="AI80">
+        <v>14.08343166541308</v>
+      </c>
+      <c r="AJ80">
+        <v>243.6396059985738</v>
+      </c>
+      <c r="AK80">
+        <v>14.08343166541308</v>
+      </c>
+      <c r="AL80">
+        <v>243.6396059985738</v>
+      </c>
+      <c r="AN80">
+        <v>21.23328398842365</v>
+      </c>
+      <c r="AO80">
+        <v>21.23328398842365</v>
+      </c>
+      <c r="AP80">
+        <v>29.97947199227288</v>
+      </c>
+      <c r="AQ80">
+        <v>10.14648030120879</v>
+      </c>
+      <c r="AR80">
+        <v>10.14648030120879</v>
+      </c>
+      <c r="AS80">
+        <v>456.9800567036122</v>
+      </c>
+      <c r="AT80">
+        <v>2217.601935847849</v>
+      </c>
+      <c r="AU80">
+        <v>2217.601935847849</v>
+      </c>
+      <c r="AV80">
+        <v>2217.601935847849</v>
+      </c>
+      <c r="AW80">
+        <v>20.47749817073345</v>
+      </c>
+      <c r="AX80">
+        <v>158.8606877215207</v>
+      </c>
+      <c r="AY80">
+        <v>7.524771695435047</v>
+      </c>
+      <c r="AZ80">
+        <v>471.0361390480996</v>
+      </c>
+      <c r="BA80">
+        <v>471.0361390480996</v>
+      </c>
+      <c r="BB80">
+        <v>471.0361390480996</v>
+      </c>
+      <c r="BC80">
+        <v>471.0361390480996</v>
+      </c>
+      <c r="BD80">
+        <v>471.0361390480996</v>
+      </c>
+      <c r="BE80">
+        <v>7.524771695435047</v>
+      </c>
+    </row>
+    <row r="81" spans="1:81">
+      <c r="A81" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AH81">
+        <v>3.037352387174033</v>
+      </c>
+      <c r="AI81">
+        <v>2.217408262763638</v>
+      </c>
+      <c r="AJ81">
+        <v>52.46461887568468</v>
+      </c>
+      <c r="AK81">
+        <v>2.217408262763638</v>
+      </c>
+      <c r="AL81">
+        <v>52.46461887568468</v>
+      </c>
+      <c r="AN81">
+        <v>2.566478029908613</v>
+      </c>
+      <c r="AO81">
+        <v>2.566478029908613</v>
+      </c>
+      <c r="AP81">
+        <v>6.34865314183291</v>
+      </c>
+      <c r="AQ81">
+        <v>3.550646647298708</v>
+      </c>
+      <c r="AR81">
+        <v>3.550646647298708</v>
+      </c>
+      <c r="AS81">
+        <v>35.47821828959975</v>
+      </c>
+      <c r="AT81">
+        <v>304.7823744788766</v>
+      </c>
+      <c r="AU81">
+        <v>304.7823744788766</v>
+      </c>
+      <c r="AV81">
+        <v>304.7823744788766</v>
+      </c>
+      <c r="AW81">
+        <v>5.122214941680432</v>
+      </c>
+      <c r="AX81">
+        <v>35.88583554206416</v>
+      </c>
+      <c r="AY81">
+        <v>2.002981155142188</v>
+      </c>
+      <c r="AZ81">
+        <v>80.71584402132035</v>
+      </c>
+      <c r="BA81">
+        <v>80.71584402132035</v>
+      </c>
+      <c r="BB81">
+        <v>80.71584402132035</v>
+      </c>
+      <c r="BC81">
+        <v>80.71584402132035</v>
+      </c>
+      <c r="BD81">
+        <v>80.71584402132035</v>
+      </c>
+      <c r="BE81">
+        <v>2.002981155142188</v>
+      </c>
+    </row>
+    <row r="82" spans="1:81">
+      <c r="A82" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH82">
         <v>5167.79</v>
       </c>
-      <c r="AI65">
+      <c r="AI82">
         <v>7.13</v>
       </c>
-      <c r="AJ65">
+      <c r="AJ82">
         <v>673.79</v>
       </c>
-      <c r="AK65">
+      <c r="AK82">
         <v>1611.53</v>
       </c>
-      <c r="AL65">
+      <c r="AL82">
         <v>19997.65</v>
       </c>
-      <c r="AM65">
+      <c r="AM82">
         <v>723.73</v>
       </c>
-      <c r="AN65">
+      <c r="AN82">
         <v>67.78</v>
       </c>
-      <c r="AO65">
+      <c r="AO82">
         <v>703.41</v>
       </c>
-      <c r="AP65">
+      <c r="AP82">
         <v>2397.43</v>
       </c>
-      <c r="AQ65">
+      <c r="AQ82">
         <v>79.59999999999999</v>
       </c>
-      <c r="AR65">
+      <c r="AR82">
         <v>6.37</v>
       </c>
-      <c r="AS65">
+      <c r="AS82">
         <v>5650.28</v>
       </c>
-      <c r="AT65">
+      <c r="AT82">
         <v>7547.66</v>
       </c>
-      <c r="AU65">
+      <c r="AU82">
         <v>13791.83</v>
       </c>
-      <c r="AV65">
+      <c r="AV82">
         <v>47294.49</v>
       </c>
-      <c r="AW65">
+      <c r="AW82">
         <v>941.97</v>
       </c>
-      <c r="AX65">
+      <c r="AX82">
         <v>1072.71</v>
       </c>
-      <c r="AY65">
+      <c r="AY82">
         <v>208.05</v>
       </c>
-      <c r="AZ65">
+      <c r="AZ82">
         <v>2.61</v>
       </c>
-      <c r="BA65">
+      <c r="BA82">
         <v>20.59</v>
       </c>
-      <c r="BB65">
+      <c r="BB82">
         <v>397.37</v>
       </c>
-      <c r="BC65">
+      <c r="BC82">
         <v>2884.17</v>
       </c>
-      <c r="BD65">
+      <c r="BD82">
         <v>936.51</v>
       </c>
-      <c r="BE65">
+      <c r="BE82">
         <v>14.56</v>
       </c>
     </row>
-    <row r="66" spans="1:65">
-      <c r="A66" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="AH66">
+    <row r="83" spans="1:81">
+      <c r="A83" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AH83">
         <v>7.28</v>
       </c>
-      <c r="AJ66">
+      <c r="AJ83">
         <v>0.16</v>
       </c>
-      <c r="AK66">
+      <c r="AK83">
         <v>50.76</v>
       </c>
-      <c r="AL66">
+      <c r="AL83">
         <v>660.9299999999999</v>
       </c>
-      <c r="AM66">
+      <c r="AM83">
         <v>15.33</v>
       </c>
-      <c r="AN66">
+      <c r="AN83">
         <v>7.13</v>
       </c>
-      <c r="AO66">
+      <c r="AO83">
         <v>30.73</v>
       </c>
-      <c r="AP66">
+      <c r="AP83">
         <v>96.58</v>
       </c>
-      <c r="AQ66">
+      <c r="AQ83">
         <v>13.3</v>
       </c>
-      <c r="AR66">
+      <c r="AR83">
         <v>0.71</v>
       </c>
-      <c r="AS66">
+      <c r="AS83">
         <v>268.63</v>
       </c>
-      <c r="AT66">
+      <c r="AT83">
         <v>397.03</v>
       </c>
-      <c r="AU66">
+      <c r="AU83">
         <v>664.72</v>
       </c>
-      <c r="AV66">
+      <c r="AV83">
         <v>1652.9</v>
       </c>
-      <c r="AZ66">
+      <c r="AZ83">
         <v>0.09</v>
       </c>
-      <c r="BA66">
+      <c r="BA83">
         <v>0.63</v>
       </c>
-      <c r="BB66">
+      <c r="BB83">
         <v>27.2</v>
       </c>
-      <c r="BC66">
+      <c r="BC83">
         <v>820.11</v>
       </c>
-      <c r="BD66">
+      <c r="BD83">
         <v>59.18</v>
       </c>
-      <c r="BE66">
+      <c r="BE83">
         <v>0.91</v>
       </c>
     </row>
-    <row r="67" spans="1:65">
-      <c r="A67" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B67">
+    <row r="84" spans="1:81">
+      <c r="A84" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B84">
         <v>227.52</v>
       </c>
-      <c r="C67">
+      <c r="C84">
         <v>74.33</v>
       </c>
-      <c r="D67">
+      <c r="D84">
         <v>2319.47</v>
       </c>
-      <c r="E67">
+      <c r="E84">
         <v>186.97</v>
       </c>
-      <c r="F67">
+      <c r="F84">
         <v>5.96</v>
       </c>
-      <c r="G67">
+      <c r="G84">
         <v>109.87</v>
       </c>
-      <c r="H67">
+      <c r="H84">
         <v>99.19</v>
       </c>
-      <c r="I67">
+      <c r="I84">
         <v>558.99</v>
       </c>
-      <c r="J67">
+      <c r="J84">
         <v>41.54</v>
       </c>
-      <c r="K67">
+      <c r="K84">
         <v>433.29</v>
       </c>
-      <c r="L67">
+      <c r="L84">
         <v>580.78</v>
       </c>
-      <c r="M67">
+      <c r="M84">
         <v>765.54</v>
       </c>
-      <c r="N67">
+      <c r="N84">
         <v>3251.01</v>
       </c>
-      <c r="O67">
+      <c r="O84">
         <v>53.1</v>
       </c>
-      <c r="P67">
+      <c r="P84">
         <v>216.04</v>
       </c>
-      <c r="Q67">
+      <c r="Q84">
         <v>5.88</v>
       </c>
-      <c r="R67">
+      <c r="R84">
         <v>76.8</v>
       </c>
-      <c r="S67">
+      <c r="S84">
         <v>174.74</v>
       </c>
-      <c r="T67">
+      <c r="T84">
         <v>21.43</v>
       </c>
-      <c r="U67">
+      <c r="U84">
         <v>42.26</v>
       </c>
-      <c r="V67">
+      <c r="V84">
         <v>51.85</v>
       </c>
-      <c r="W67">
+      <c r="W84">
         <v>19.07</v>
       </c>
-      <c r="X67">
+      <c r="X84">
         <v>19.84</v>
       </c>
-      <c r="Y67">
+      <c r="Y84">
         <v>0.44</v>
       </c>
-      <c r="Z67">
+      <c r="Z84">
         <v>117.44</v>
       </c>
-      <c r="AA67">
+      <c r="AA84">
         <v>12.27</v>
       </c>
-      <c r="AB67">
+      <c r="AB84">
         <v>4.69</v>
       </c>
-      <c r="AC67">
+      <c r="AC84">
         <v>330.19</v>
       </c>
-      <c r="AD67">
+      <c r="AD84">
         <v>33.42</v>
       </c>
-      <c r="AE67">
+      <c r="AE84">
         <v>4.14</v>
       </c>
-      <c r="AF67">
+      <c r="AF84">
         <v>92.26000000000001</v>
       </c>
-      <c r="AG67">
-        <v>0</v>
-      </c>
-      <c r="AH67">
-        <v>0</v>
-      </c>
-      <c r="AI67">
-        <v>0</v>
-      </c>
-      <c r="AJ67">
-        <v>0</v>
-      </c>
-      <c r="AN67">
-        <v>0</v>
-      </c>
-      <c r="AP67">
-        <v>0</v>
-      </c>
-      <c r="AQ67">
-        <v>0</v>
-      </c>
-      <c r="AR67">
-        <v>0</v>
-      </c>
-      <c r="AS67">
-        <v>0</v>
-      </c>
-      <c r="AU67">
-        <v>0</v>
-      </c>
-      <c r="AV67">
-        <v>0</v>
-      </c>
-      <c r="AW67">
-        <v>0</v>
-      </c>
-      <c r="AX67">
-        <v>0</v>
-      </c>
-      <c r="BB67">
-        <v>0</v>
-      </c>
-      <c r="BD67">
-        <v>0</v>
-      </c>
-      <c r="BE67">
-        <v>0</v>
-      </c>
-      <c r="BF67">
-        <v>0</v>
-      </c>
-      <c r="BG67">
-        <v>0</v>
-      </c>
-      <c r="BH67">
-        <v>0</v>
-      </c>
-      <c r="BI67">
-        <v>0</v>
-      </c>
-      <c r="BJ67">
-        <v>0</v>
-      </c>
-      <c r="BK67">
-        <v>0</v>
-      </c>
-      <c r="BM67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:65">
-      <c r="A68" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AH68">
-        <v>9.414114025598392</v>
-      </c>
-      <c r="AI68">
-        <v>4.98343871824909</v>
-      </c>
-      <c r="AJ68">
-        <v>200.4209536320157</v>
-      </c>
-      <c r="AK68">
-        <v>4.98343871824909</v>
-      </c>
-      <c r="AL68">
-        <v>200.4209536320157</v>
-      </c>
-      <c r="AN68">
-        <v>3.583830243987031</v>
-      </c>
-      <c r="AO68">
-        <v>3.583830243987031</v>
-      </c>
-      <c r="AP68">
-        <v>11.83001546522602</v>
-      </c>
-      <c r="AQ68">
-        <v>0.882314035994932</v>
-      </c>
-      <c r="AR68">
-        <v>0.882314035994932</v>
-      </c>
-      <c r="AS68">
-        <v>73.19743904368953</v>
-      </c>
-      <c r="AT68">
-        <v>192.0036300258339</v>
-      </c>
-      <c r="AU68">
-        <v>192.0036300258339</v>
-      </c>
-      <c r="AV68">
-        <v>192.0036300258339</v>
-      </c>
-      <c r="AW68">
-        <v>8.166333993524313</v>
-      </c>
-      <c r="AX68">
-        <v>22.61657591545954</v>
-      </c>
-      <c r="AY68">
-        <v>0.6143333348818123</v>
-      </c>
-      <c r="AZ68">
-        <v>38.40820165850223</v>
-      </c>
-      <c r="BA68">
-        <v>38.40820165850223</v>
-      </c>
-      <c r="BB68">
-        <v>38.40820165850223</v>
-      </c>
-      <c r="BC68">
-        <v>38.40820165850223</v>
-      </c>
-      <c r="BD68">
-        <v>38.40820165850223</v>
-      </c>
-      <c r="BE68">
-        <v>0.6143333348818123</v>
-      </c>
-    </row>
-    <row r="69" spans="1:65">
-      <c r="A69" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AH69">
-        <v>59.33229717329145</v>
-      </c>
-      <c r="AI69">
-        <v>52.88727739527822</v>
-      </c>
-      <c r="AJ69">
-        <v>2386.627410095036</v>
-      </c>
-      <c r="AK69">
-        <v>52.88727739527822</v>
-      </c>
-      <c r="AL69">
-        <v>2386.627410095036</v>
-      </c>
-      <c r="AN69">
-        <v>16.82216917671263</v>
-      </c>
-      <c r="AO69">
-        <v>16.82216917671263</v>
-      </c>
-      <c r="AP69">
-        <v>75.89979358144105</v>
-      </c>
-      <c r="AQ69">
-        <v>9.907512448914348</v>
-      </c>
-      <c r="AR69">
-        <v>9.907512448914348</v>
-      </c>
-      <c r="AS69">
-        <v>168.617042367179</v>
-      </c>
-      <c r="AT69">
-        <v>337.3299611688592</v>
-      </c>
-      <c r="AU69">
-        <v>337.3299611688592</v>
-      </c>
-      <c r="AV69">
-        <v>337.3299611688592</v>
-      </c>
-      <c r="AW69">
-        <v>15.90577829927206</v>
-      </c>
-      <c r="AX69">
-        <v>164.5034938763827</v>
-      </c>
-      <c r="AY69">
-        <v>2.83422336127609</v>
-      </c>
-      <c r="AZ69">
-        <v>111.1287621074915</v>
-      </c>
-      <c r="BA69">
-        <v>111.1287621074915</v>
-      </c>
-      <c r="BB69">
-        <v>111.1287621074915</v>
-      </c>
-      <c r="BC69">
-        <v>111.1287621074915</v>
-      </c>
-      <c r="BD69">
-        <v>111.1287621074915</v>
-      </c>
-      <c r="BE69">
-        <v>2.83422336127609</v>
-      </c>
-    </row>
-    <row r="70" spans="1:65">
-      <c r="A70" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AH70">
-        <v>7.205654163155705</v>
-      </c>
-      <c r="AI70">
-        <v>4.216897656582296</v>
-      </c>
-      <c r="AJ70">
-        <v>424.28795445811</v>
-      </c>
-      <c r="AK70">
-        <v>4.216897656582296</v>
-      </c>
-      <c r="AL70">
-        <v>424.28795445811</v>
-      </c>
-      <c r="AN70">
-        <v>3.524966271901503</v>
-      </c>
-      <c r="AO70">
-        <v>3.524966271901503</v>
-      </c>
-      <c r="AP70">
-        <v>14.83037091043778</v>
-      </c>
-      <c r="AQ70">
-        <v>2.587943928549066</v>
-      </c>
-      <c r="AR70">
-        <v>2.587943928549066</v>
-      </c>
-      <c r="AS70">
-        <v>15.87995030975901</v>
-      </c>
-      <c r="AT70">
-        <v>95.40936142164284</v>
-      </c>
-      <c r="AU70">
-        <v>95.40936142164284</v>
-      </c>
-      <c r="AV70">
-        <v>95.40936142164284</v>
-      </c>
-      <c r="AW70">
-        <v>4.508362703770399</v>
-      </c>
-      <c r="AX70">
-        <v>20.73699029148556</v>
-      </c>
-      <c r="AY70">
-        <v>0.6809700198937206</v>
-      </c>
-      <c r="AZ70">
-        <v>24.04094541568309</v>
-      </c>
-      <c r="BA70">
-        <v>24.04094541568309</v>
-      </c>
-      <c r="BB70">
-        <v>24.04094541568309</v>
-      </c>
-      <c r="BC70">
-        <v>24.04094541568309</v>
-      </c>
-      <c r="BD70">
-        <v>24.04094541568309</v>
-      </c>
-      <c r="BE70">
-        <v>0.6809700198937206</v>
-      </c>
-    </row>
-    <row r="71" spans="1:65">
-      <c r="A71" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AH71">
-        <v>85.96996595606208</v>
-      </c>
-      <c r="AI71">
-        <v>45.81034803465009</v>
-      </c>
-      <c r="AJ71">
-        <v>1067.650717165209</v>
-      </c>
-      <c r="AK71">
-        <v>45.81034803465009</v>
-      </c>
-      <c r="AL71">
-        <v>1067.650717165209</v>
-      </c>
-      <c r="AN71">
-        <v>21.2452943026647</v>
-      </c>
-      <c r="AO71">
-        <v>21.2452943026647</v>
-      </c>
-      <c r="AP71">
-        <v>67.45605026192963</v>
-      </c>
-      <c r="AQ71">
-        <v>3.648380930209532</v>
-      </c>
-      <c r="AR71">
-        <v>3.648380930209532</v>
-      </c>
-      <c r="AS71">
-        <v>1017.25321948424</v>
-      </c>
-      <c r="AT71">
-        <v>2296.914724432677</v>
-      </c>
-      <c r="AU71">
-        <v>2296.914724432677</v>
-      </c>
-      <c r="AV71">
-        <v>2296.914724432677</v>
-      </c>
-      <c r="AW71">
-        <v>57.67828812599182</v>
-      </c>
-      <c r="AX71">
-        <v>253.528219165653</v>
-      </c>
-      <c r="AY71">
-        <v>6.298046703189611</v>
-      </c>
-      <c r="AZ71">
-        <v>533.8607489335537</v>
-      </c>
-      <c r="BA71">
-        <v>533.8607489335537</v>
-      </c>
-      <c r="BB71">
-        <v>533.8607489335537</v>
-      </c>
-      <c r="BC71">
-        <v>533.8607489335537</v>
-      </c>
-      <c r="BD71">
-        <v>533.8607489335537</v>
-      </c>
-      <c r="BE71">
-        <v>6.298046703189611</v>
-      </c>
-    </row>
-    <row r="72" spans="1:65">
-      <c r="A72" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="AH72">
-        <v>210.7794315168262</v>
-      </c>
-      <c r="AI72">
-        <v>300.8081789076329</v>
-      </c>
-      <c r="AJ72">
-        <v>4553.744405761063</v>
-      </c>
-      <c r="AK72">
-        <v>300.8081789076329</v>
-      </c>
-      <c r="AL72">
-        <v>4553.744405761063</v>
-      </c>
-      <c r="AN72">
-        <v>71.71276636935771</v>
-      </c>
-      <c r="AO72">
-        <v>71.71276636935771</v>
-      </c>
-      <c r="AP72">
-        <v>425.0448387694359</v>
-      </c>
-      <c r="AQ72">
-        <v>24.91756613589823</v>
-      </c>
-      <c r="AR72">
-        <v>24.91756613589823</v>
-      </c>
-      <c r="AS72">
-        <v>1199.389830690175</v>
-      </c>
-      <c r="AT72">
-        <v>3500.822733426095</v>
-      </c>
-      <c r="AU72">
-        <v>3500.822733426095</v>
-      </c>
-      <c r="AV72">
-        <v>3500.822733426095</v>
-      </c>
-      <c r="AW72">
-        <v>55.08900470733643</v>
-      </c>
-      <c r="AX72">
-        <v>787.1122351065278</v>
-      </c>
-      <c r="AY72">
-        <v>7.304603953659534</v>
-      </c>
-      <c r="AZ72">
-        <v>521.6428579665424</v>
-      </c>
-      <c r="BA72">
-        <v>521.6428579665424</v>
-      </c>
-      <c r="BB72">
-        <v>521.6428579665424</v>
-      </c>
-      <c r="BC72">
-        <v>521.6428579665424</v>
-      </c>
-      <c r="BD72">
-        <v>521.6428579665424</v>
-      </c>
-      <c r="BE72">
-        <v>7.304603953659534</v>
-      </c>
-    </row>
-    <row r="73" spans="1:65">
-      <c r="A73" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AH73">
-        <v>17.85041145477444</v>
-      </c>
-      <c r="AI73">
-        <v>28.15027438197285</v>
-      </c>
-      <c r="AJ73">
-        <v>377.6822184351739</v>
-      </c>
-      <c r="AK73">
-        <v>28.15027438197285</v>
-      </c>
-      <c r="AL73">
-        <v>377.6822184351739</v>
-      </c>
-      <c r="AN73">
-        <v>4.714462637193501</v>
-      </c>
-      <c r="AO73">
-        <v>4.714462637193501</v>
-      </c>
-      <c r="AP73">
-        <v>49.16584968741984</v>
-      </c>
-      <c r="AQ73">
-        <v>2.893772782757878</v>
-      </c>
-      <c r="AR73">
-        <v>2.893772782757878</v>
-      </c>
-      <c r="AS73">
-        <v>33.3963167022774</v>
-      </c>
-      <c r="AT73">
-        <v>255.6969061620534</v>
-      </c>
-      <c r="AU73">
-        <v>255.6969061620534</v>
-      </c>
-      <c r="AV73">
-        <v>255.6969061620534</v>
-      </c>
-      <c r="AW73">
-        <v>5.374387093633413</v>
-      </c>
-      <c r="AX73">
-        <v>25.69650055831298</v>
-      </c>
-      <c r="AY73">
-        <v>0.2742241334868595</v>
-      </c>
-      <c r="AZ73">
-        <v>44.71875981566311</v>
-      </c>
-      <c r="BA73">
-        <v>44.71875981566311</v>
-      </c>
-      <c r="BB73">
-        <v>44.71875981566311</v>
-      </c>
-      <c r="BC73">
-        <v>44.71875981566311</v>
-      </c>
-      <c r="BD73">
-        <v>44.71875981566311</v>
-      </c>
-      <c r="BE73">
-        <v>0.2742241334868595</v>
-      </c>
-    </row>
-    <row r="74" spans="1:65">
-      <c r="A74" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AH74">
-        <v>22.72248552095145</v>
-      </c>
-      <c r="AI74">
-        <v>26.40249624270946</v>
-      </c>
-      <c r="AJ74">
-        <v>551.2811292873323</v>
-      </c>
-      <c r="AK74">
-        <v>26.40249624270946</v>
-      </c>
-      <c r="AL74">
-        <v>551.2811292873323</v>
-      </c>
-      <c r="AN74">
-        <v>4.544429623456672</v>
-      </c>
-      <c r="AO74">
-        <v>4.544429623456672</v>
-      </c>
-      <c r="AP74">
-        <v>15.6135156785883</v>
-      </c>
-      <c r="AQ74">
-        <v>1.124677603738382</v>
-      </c>
-      <c r="AR74">
-        <v>1.124677603738382</v>
-      </c>
-      <c r="AS74">
-        <v>224.3877803584561</v>
-      </c>
-      <c r="AT74">
-        <v>1211.574020833299</v>
-      </c>
-      <c r="AU74">
-        <v>1211.574020833299</v>
-      </c>
-      <c r="AV74">
-        <v>1211.574020833299</v>
-      </c>
-      <c r="AW74">
-        <v>13.75366018712521</v>
-      </c>
-      <c r="AX74">
-        <v>151.1198314923793</v>
-      </c>
-      <c r="AY74">
-        <v>4.972760506421327</v>
-      </c>
-      <c r="AZ74">
-        <v>185.2030471046567</v>
-      </c>
-      <c r="BA74">
-        <v>185.2030471046567</v>
-      </c>
-      <c r="BB74">
-        <v>185.2030471046567</v>
-      </c>
-      <c r="BC74">
-        <v>185.2030471046567</v>
-      </c>
-      <c r="BD74">
-        <v>185.2030471046567</v>
-      </c>
-      <c r="BE74">
-        <v>4.972760506421327</v>
-      </c>
-    </row>
-    <row r="75" spans="1:65">
-      <c r="A75" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AH75">
-        <v>86.79474751248956</v>
-      </c>
-      <c r="AI75">
-        <v>139.8593661420047</v>
-      </c>
-      <c r="AJ75">
-        <v>1530.035279196426</v>
-      </c>
-      <c r="AK75">
-        <v>139.8593661420047</v>
-      </c>
-      <c r="AL75">
-        <v>1530.035279196426</v>
-      </c>
-      <c r="AN75">
-        <v>27.99167295109481</v>
-      </c>
-      <c r="AO75">
-        <v>27.99167295109481</v>
-      </c>
-      <c r="AP75">
-        <v>188.5514367929101</v>
-      </c>
-      <c r="AQ75">
-        <v>9.954080538451672</v>
-      </c>
-      <c r="AR75">
-        <v>9.954080538451672</v>
-      </c>
-      <c r="AS75">
-        <v>898.22598473683</v>
-      </c>
-      <c r="AT75">
-        <v>3174.076085808873</v>
-      </c>
-      <c r="AU75">
-        <v>3174.076085808873</v>
-      </c>
-      <c r="AV75">
-        <v>3174.076085808873</v>
-      </c>
-      <c r="AW75">
-        <v>25.92668635845184</v>
-      </c>
-      <c r="AX75">
-        <v>885.2735020026564</v>
-      </c>
-      <c r="AY75">
-        <v>4.723041579052805</v>
-      </c>
-      <c r="AZ75">
-        <v>223.8124471736551</v>
-      </c>
-      <c r="BA75">
-        <v>223.8124471736551</v>
-      </c>
-      <c r="BB75">
-        <v>223.8124471736551</v>
-      </c>
-      <c r="BC75">
-        <v>223.8124471736551</v>
-      </c>
-      <c r="BD75">
-        <v>223.8124471736551</v>
-      </c>
-      <c r="BE75">
-        <v>4.723041579052805</v>
-      </c>
-    </row>
-    <row r="76" spans="1:65">
-      <c r="A76" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AH76">
-        <v>13.98811280122027</v>
-      </c>
-      <c r="AI76">
-        <v>15.2970779588446</v>
-      </c>
-      <c r="AJ76">
-        <v>153.0186887697224</v>
-      </c>
-      <c r="AK76">
-        <v>15.2970779588446</v>
-      </c>
-      <c r="AL76">
-        <v>153.0186887697224</v>
-      </c>
-      <c r="AN76">
-        <v>3.391067505558021</v>
-      </c>
-      <c r="AO76">
-        <v>3.391067505558021</v>
-      </c>
-      <c r="AP76">
-        <v>36.30120203226805</v>
-      </c>
-      <c r="AQ76">
-        <v>1.918124681361951</v>
-      </c>
-      <c r="AR76">
-        <v>1.918124681361951</v>
-      </c>
-      <c r="AS76">
-        <v>89.16462504421361</v>
-      </c>
-      <c r="AT76">
-        <v>210.5832067055814</v>
-      </c>
-      <c r="AU76">
-        <v>210.5832067055814</v>
-      </c>
-      <c r="AV76">
-        <v>210.5832067055814</v>
-      </c>
-      <c r="AW76">
-        <v>5.622723040729761</v>
-      </c>
-      <c r="AX76">
-        <v>36.43868462974206</v>
-      </c>
-      <c r="AY76">
-        <v>0.2696506427740678</v>
-      </c>
-      <c r="AZ76">
-        <v>61.94066436254979</v>
-      </c>
-      <c r="BA76">
-        <v>61.94066436254979</v>
-      </c>
-      <c r="BB76">
-        <v>61.94066436254979</v>
-      </c>
-      <c r="BC76">
-        <v>61.94066436254979</v>
-      </c>
-      <c r="BD76">
-        <v>61.94066436254979</v>
-      </c>
-      <c r="BE76">
-        <v>0.2696506427740678</v>
-      </c>
-    </row>
-    <row r="77" spans="1:65">
-      <c r="A77" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AH77">
-        <v>20.77479004822672</v>
-      </c>
-      <c r="AI77">
-        <v>4.852747014700435</v>
-      </c>
-      <c r="AJ77">
-        <v>48.24235908871516</v>
-      </c>
-      <c r="AK77">
-        <v>4.852747014700435</v>
-      </c>
-      <c r="AL77">
-        <v>48.24235908871516</v>
-      </c>
-      <c r="AN77">
-        <v>4.100118934209458</v>
-      </c>
-      <c r="AO77">
-        <v>4.100118934209458</v>
-      </c>
-      <c r="AP77">
-        <v>5.887614787886851</v>
-      </c>
-      <c r="AQ77">
-        <v>1.975540813524276</v>
-      </c>
-      <c r="AR77">
-        <v>1.975540813524276</v>
-      </c>
-      <c r="AS77">
-        <v>94.09361228807829</v>
-      </c>
-      <c r="AT77">
-        <v>432.1870895471797</v>
-      </c>
-      <c r="AU77">
-        <v>432.1870895471797</v>
-      </c>
-      <c r="AV77">
-        <v>432.1870895471797</v>
-      </c>
-      <c r="AW77">
-        <v>7.274246802926064</v>
-      </c>
-      <c r="AX77">
-        <v>48.43849489577114</v>
-      </c>
-      <c r="AY77">
-        <v>2.568719942420721</v>
-      </c>
-      <c r="AZ77">
-        <v>96.82042559319736</v>
-      </c>
-      <c r="BA77">
-        <v>96.82042559319736</v>
-      </c>
-      <c r="BB77">
-        <v>96.82042559319736</v>
-      </c>
-      <c r="BC77">
-        <v>96.82042559319736</v>
-      </c>
-      <c r="BD77">
-        <v>96.82042559319736</v>
-      </c>
-      <c r="BE77">
-        <v>2.568719942420721</v>
-      </c>
-    </row>
-    <row r="78" spans="1:65">
-      <c r="A78" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="AH78">
-        <v>6.972353674806655</v>
-      </c>
-      <c r="AI78">
-        <v>12.21744870962575</v>
-      </c>
-      <c r="AJ78">
-        <v>199.71937682949</v>
-      </c>
-      <c r="AK78">
-        <v>12.21744870962575</v>
-      </c>
-      <c r="AL78">
-        <v>199.71937682949</v>
-      </c>
-      <c r="AN78">
-        <v>18.19257926173508</v>
-      </c>
-      <c r="AO78">
-        <v>18.19257926173508</v>
-      </c>
-      <c r="AP78">
-        <v>18.15562672873959</v>
-      </c>
-      <c r="AQ78">
-        <v>11.11295016352087</v>
-      </c>
-      <c r="AR78">
-        <v>11.11295016352087</v>
-      </c>
-      <c r="AS78">
-        <v>263.5501914815977</v>
-      </c>
-      <c r="AT78">
-        <v>908.7285465851427</v>
-      </c>
-      <c r="AU78">
-        <v>908.7285465851427</v>
-      </c>
-      <c r="AV78">
-        <v>908.7285465851427</v>
-      </c>
-      <c r="AW78">
-        <v>15.00309596955776</v>
-      </c>
-      <c r="AX78">
-        <v>157.2740013517439</v>
-      </c>
-      <c r="AY78">
-        <v>10.54452222824097</v>
-      </c>
-      <c r="AZ78">
-        <v>341.338813333869</v>
-      </c>
-      <c r="BA78">
-        <v>341.338813333869</v>
-      </c>
-      <c r="BB78">
-        <v>341.338813333869</v>
-      </c>
-      <c r="BC78">
-        <v>341.338813333869</v>
-      </c>
-      <c r="BD78">
-        <v>341.338813333869</v>
-      </c>
-      <c r="BE78">
-        <v>10.54452222824097</v>
-      </c>
-    </row>
-    <row r="79" spans="1:65">
-      <c r="A79" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="AH79">
-        <v>0.5680094407271827</v>
-      </c>
-      <c r="AI79">
-        <v>0.6389008355734405</v>
-      </c>
-      <c r="AJ79">
-        <v>21.40426394213398</v>
-      </c>
-      <c r="AK79">
-        <v>0.6389008355734405</v>
-      </c>
-      <c r="AL79">
-        <v>21.40426394213398</v>
-      </c>
-      <c r="AN79">
-        <v>3.499278473271989</v>
-      </c>
-      <c r="AO79">
-        <v>3.499278473271989</v>
-      </c>
-      <c r="AP79">
-        <v>2.967877806534525</v>
-      </c>
-      <c r="AQ79">
-        <v>2.793893166305497</v>
-      </c>
-      <c r="AR79">
-        <v>2.793893166305497</v>
-      </c>
-      <c r="AS79">
-        <v>14.40585431333166</v>
-      </c>
-      <c r="AT79">
-        <v>100.455687204795</v>
-      </c>
-      <c r="AU79">
-        <v>100.455687204795</v>
-      </c>
-      <c r="AV79">
-        <v>100.455687204795</v>
-      </c>
-      <c r="AW79">
-        <v>2.471739122271538</v>
-      </c>
-      <c r="AX79">
-        <v>3.190947880822932</v>
-      </c>
-      <c r="AY79">
-        <v>0.3704864161368459</v>
-      </c>
-      <c r="AZ79">
-        <v>79.33680799412728</v>
-      </c>
-      <c r="BA79">
-        <v>79.33680799412728</v>
-      </c>
-      <c r="BB79">
-        <v>79.33680799412728</v>
-      </c>
-      <c r="BC79">
-        <v>79.33680799412728</v>
-      </c>
-      <c r="BD79">
-        <v>79.33680799412728</v>
-      </c>
-      <c r="BE79">
-        <v>0.3704864161368459</v>
-      </c>
-    </row>
-    <row r="80" spans="1:65">
-      <c r="A80" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AH80">
-        <v>14.58600710416213</v>
-      </c>
-      <c r="AI80">
-        <v>20.80613398961723</v>
-      </c>
-      <c r="AJ80">
-        <v>203.2207749169506</v>
-      </c>
-      <c r="AK80">
-        <v>20.80613398961723</v>
-      </c>
-      <c r="AL80">
-        <v>203.2207749169506</v>
-      </c>
-      <c r="AN80">
-        <v>15.73506095610559</v>
-      </c>
-      <c r="AO80">
-        <v>15.73506095610559</v>
-      </c>
-      <c r="AP80">
-        <v>25.33586614327505</v>
-      </c>
-      <c r="AQ80">
-        <v>4.656144000031054</v>
-      </c>
-      <c r="AR80">
-        <v>4.656144000031054</v>
-      </c>
-      <c r="AS80">
-        <v>629.8837321466208</v>
-      </c>
-      <c r="AT80">
-        <v>2327.148932623268</v>
-      </c>
-      <c r="AU80">
-        <v>2327.148932623268</v>
-      </c>
-      <c r="AV80">
-        <v>2327.148932623268</v>
-      </c>
-      <c r="AW80">
-        <v>40.31813014149666</v>
-      </c>
-      <c r="AX80">
-        <v>221.5278009824455</v>
-      </c>
-      <c r="AY80">
-        <v>11.62228437572718</v>
-      </c>
-      <c r="AZ80">
-        <v>658.5692046878339</v>
-      </c>
-      <c r="BA80">
-        <v>658.5692046878339</v>
-      </c>
-      <c r="BB80">
-        <v>658.5692046878339</v>
-      </c>
-      <c r="BC80">
-        <v>658.5692046878339</v>
-      </c>
-      <c r="BD80">
-        <v>658.5692046878339</v>
-      </c>
-      <c r="BE80">
-        <v>11.62228437572718</v>
-      </c>
-    </row>
-    <row r="81" spans="1:57">
-      <c r="A81" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AH81">
-        <v>22.16415098886937</v>
-      </c>
-      <c r="AI81">
-        <v>49.84443322978914</v>
-      </c>
-      <c r="AJ81">
-        <v>674.1897927421331</v>
-      </c>
-      <c r="AK81">
-        <v>49.84443322978914</v>
-      </c>
-      <c r="AL81">
-        <v>674.1897927421331</v>
-      </c>
-      <c r="AN81">
-        <v>58.49801138035953</v>
-      </c>
-      <c r="AO81">
-        <v>58.49801138035953</v>
-      </c>
-      <c r="AP81">
-        <v>90.24182404957712</v>
-      </c>
-      <c r="AQ81">
-        <v>24.82541301250458</v>
-      </c>
-      <c r="AR81">
-        <v>24.82541301250458</v>
-      </c>
-      <c r="AS81">
-        <v>1220.66968123287</v>
-      </c>
-      <c r="AT81">
-        <v>3909.166663952172</v>
-      </c>
-      <c r="AU81">
-        <v>3909.166663952172</v>
-      </c>
-      <c r="AV81">
-        <v>3909.166663952172</v>
-      </c>
-      <c r="AW81">
-        <v>51.75319621562958</v>
-      </c>
-      <c r="AX81">
-        <v>509.3750439479947</v>
-      </c>
-      <c r="AY81">
-        <v>25.97905255854129</v>
-      </c>
-      <c r="AZ81">
-        <v>1172.28277120328</v>
-      </c>
-      <c r="BA81">
-        <v>1172.28277120328</v>
-      </c>
-      <c r="BB81">
-        <v>1172.28277120328</v>
-      </c>
-      <c r="BC81">
-        <v>1172.28277120328</v>
-      </c>
-      <c r="BD81">
-        <v>1172.28277120328</v>
-      </c>
-      <c r="BE81">
-        <v>25.97905255854129</v>
-      </c>
-    </row>
-    <row r="82" spans="1:57">
-      <c r="A82" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AH82">
-        <v>0.4406759691750631</v>
-      </c>
-      <c r="AI82">
-        <v>7.213819674542174</v>
-      </c>
-      <c r="AJ82">
-        <v>74.40975860358914</v>
-      </c>
-      <c r="AK82">
-        <v>7.213819674542174</v>
-      </c>
-      <c r="AL82">
-        <v>74.40975860358914</v>
-      </c>
-      <c r="AN82">
-        <v>5.620547629725189</v>
-      </c>
-      <c r="AO82">
-        <v>5.620547629725189</v>
-      </c>
-      <c r="AP82">
-        <v>11.42237053900957</v>
-      </c>
-      <c r="AQ82">
-        <v>6.340353480260819</v>
-      </c>
-      <c r="AR82">
-        <v>6.340353480260819</v>
-      </c>
-      <c r="AS82">
-        <v>47.1778669777466</v>
-      </c>
-      <c r="AT82">
-        <v>121.1692079006415</v>
-      </c>
-      <c r="AU82">
-        <v>121.1692079006415</v>
-      </c>
-      <c r="AV82">
-        <v>121.1692079006415</v>
-      </c>
-      <c r="AW82">
-        <v>9.171287022531033</v>
-      </c>
-      <c r="AX82">
-        <v>30.8258233175613</v>
-      </c>
-      <c r="AY82">
-        <v>2.15244241643697</v>
-      </c>
-      <c r="AZ82">
-        <v>94.26668654054404</v>
-      </c>
-      <c r="BA82">
-        <v>94.26668654054404</v>
-      </c>
-      <c r="BB82">
-        <v>94.26668654054404</v>
-      </c>
-      <c r="BC82">
-        <v>94.26668654054404</v>
-      </c>
-      <c r="BD82">
-        <v>94.26668654054404</v>
-      </c>
-      <c r="BE82">
-        <v>2.15244241643697</v>
-      </c>
-    </row>
-    <row r="83" spans="1:57">
-      <c r="A83" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AH83">
-        <v>10.65145417792723</v>
-      </c>
-      <c r="AI83">
-        <v>4.660319383302704</v>
-      </c>
-      <c r="AJ83">
-        <v>39.81580099688144</v>
-      </c>
-      <c r="AK83">
-        <v>4.660319383302704</v>
-      </c>
-      <c r="AL83">
-        <v>39.81580099688144</v>
-      </c>
-      <c r="AN83">
-        <v>2.638983073509298</v>
-      </c>
-      <c r="AO83">
-        <v>2.638983073509298</v>
-      </c>
-      <c r="AP83">
-        <v>2.937615607588086</v>
-      </c>
-      <c r="AQ83">
-        <v>1.239205213543028</v>
-      </c>
-      <c r="AR83">
-        <v>1.239205213543028</v>
-      </c>
-      <c r="AS83">
-        <v>64.8387075754907</v>
-      </c>
-      <c r="AT83">
-        <v>415.808921625279</v>
-      </c>
-      <c r="AU83">
-        <v>415.808921625279</v>
-      </c>
-      <c r="AV83">
-        <v>415.808921625279</v>
-      </c>
-      <c r="AW83">
-        <v>7.183363182842732</v>
-      </c>
-      <c r="AX83">
-        <v>100.2953584484756</v>
-      </c>
-      <c r="AY83">
-        <v>4.522884311899542</v>
-      </c>
-      <c r="AZ83">
-        <v>203.228815502882</v>
-      </c>
-      <c r="BA83">
-        <v>203.228815502882</v>
-      </c>
-      <c r="BB83">
-        <v>203.228815502882</v>
-      </c>
-      <c r="BC83">
-        <v>203.228815502882</v>
-      </c>
-      <c r="BD83">
-        <v>203.228815502882</v>
-      </c>
-      <c r="BE83">
-        <v>4.522884311899542</v>
-      </c>
-    </row>
-    <row r="84" spans="1:57">
-      <c r="A84" s="1" t="s">
-        <v>82</v>
+      <c r="AG84">
+        <v>0</v>
       </c>
       <c r="AH84">
-        <v>13.45798746185377</v>
+        <v>0</v>
       </c>
       <c r="AI84">
-        <v>14.08343166541308</v>
+        <v>0</v>
       </c>
       <c r="AJ84">
-        <v>243.6396059985738</v>
-      </c>
-      <c r="AK84">
-        <v>14.08343166541308</v>
-      </c>
-      <c r="AL84">
-        <v>243.6396059985738</v>
+        <v>0</v>
       </c>
       <c r="AN84">
-        <v>21.23328398842365</v>
-      </c>
-      <c r="AO84">
-        <v>21.23328398842365</v>
+        <v>0</v>
       </c>
       <c r="AP84">
-        <v>29.97947199227288</v>
+        <v>0</v>
       </c>
       <c r="AQ84">
-        <v>10.14648030120879</v>
+        <v>0</v>
       </c>
       <c r="AR84">
-        <v>10.14648030120879</v>
+        <v>0</v>
       </c>
       <c r="AS84">
-        <v>456.9800567036122</v>
-      </c>
-      <c r="AT84">
-        <v>2217.601935847849</v>
+        <v>0</v>
       </c>
       <c r="AU84">
-        <v>2217.601935847849</v>
+        <v>0</v>
       </c>
       <c r="AV84">
-        <v>2217.601935847849</v>
+        <v>0</v>
       </c>
       <c r="AW84">
-        <v>20.47749817073345</v>
+        <v>0</v>
       </c>
       <c r="AX84">
-        <v>158.8606877215207</v>
-      </c>
-      <c r="AY84">
-        <v>7.524771695435047</v>
-      </c>
-      <c r="AZ84">
-        <v>471.0361390480996</v>
-      </c>
-      <c r="BA84">
-        <v>471.0361390480996</v>
+        <v>0</v>
       </c>
       <c r="BB84">
-        <v>471.0361390480996</v>
-      </c>
-      <c r="BC84">
-        <v>471.0361390480996</v>
+        <v>0</v>
       </c>
       <c r="BD84">
-        <v>471.0361390480996</v>
+        <v>0</v>
       </c>
       <c r="BE84">
-        <v>7.524771695435047</v>
-      </c>
-    </row>
-    <row r="85" spans="1:57">
-      <c r="A85" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AH85">
-        <v>3.037352387174033</v>
-      </c>
-      <c r="AI85">
-        <v>2.217408262763638</v>
-      </c>
-      <c r="AJ85">
-        <v>52.46461887568468</v>
-      </c>
-      <c r="AK85">
-        <v>2.217408262763638</v>
-      </c>
-      <c r="AL85">
-        <v>52.46461887568468</v>
-      </c>
-      <c r="AN85">
-        <v>2.566478029908613</v>
-      </c>
-      <c r="AO85">
-        <v>2.566478029908613</v>
-      </c>
-      <c r="AP85">
-        <v>6.34865314183291</v>
-      </c>
-      <c r="AQ85">
-        <v>3.550646647298708</v>
-      </c>
-      <c r="AR85">
-        <v>3.550646647298708</v>
-      </c>
-      <c r="AS85">
-        <v>35.47821828959975</v>
-      </c>
-      <c r="AT85">
-        <v>304.7823744788766</v>
-      </c>
-      <c r="AU85">
-        <v>304.7823744788766</v>
-      </c>
-      <c r="AV85">
-        <v>304.7823744788766</v>
-      </c>
-      <c r="AW85">
-        <v>5.122214941680432</v>
-      </c>
-      <c r="AX85">
-        <v>35.88583554206416</v>
-      </c>
-      <c r="AY85">
-        <v>2.002981155142188</v>
-      </c>
-      <c r="AZ85">
-        <v>80.71584402132035</v>
-      </c>
-      <c r="BA85">
-        <v>80.71584402132035</v>
-      </c>
-      <c r="BB85">
-        <v>80.71584402132035</v>
-      </c>
-      <c r="BC85">
-        <v>80.71584402132035</v>
-      </c>
-      <c r="BD85">
-        <v>80.71584402132035</v>
-      </c>
-      <c r="BE85">
-        <v>2.002981155142188</v>
+        <v>0</v>
+      </c>
+      <c r="BF84">
+        <v>0</v>
+      </c>
+      <c r="BG84">
+        <v>0</v>
+      </c>
+      <c r="BH84">
+        <v>0</v>
+      </c>
+      <c r="BI84">
+        <v>0</v>
+      </c>
+      <c r="BJ84">
+        <v>0</v>
+      </c>
+      <c r="CB84">
+        <v>0</v>
+      </c>
+      <c r="CC84">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Now sums total value of each type of labour to HOUS
</commit_message>
<xml_diff>
--- a/excel_files/output.xlsx
+++ b/excel_files/output.xlsx
@@ -5139,8 +5139,11 @@
       <c r="BE64">
         <v>0.6143333348818123</v>
       </c>
-    </row>
-    <row r="65" spans="1:57">
+      <c r="BF64">
+        <v>1314.246116743768</v>
+      </c>
+    </row>
+    <row r="65" spans="1:58">
       <c r="A65" s="1" t="s">
         <v>61</v>
       </c>
@@ -5213,8 +5216,11 @@
       <c r="BE65">
         <v>2.83422336127609</v>
       </c>
-    </row>
-    <row r="66" spans="1:57">
+      <c r="BF65">
+        <v>6990.049284296037</v>
+      </c>
+    </row>
+    <row r="66" spans="1:58">
       <c r="A66" s="1" t="s">
         <v>62</v>
       </c>
@@ -5287,8 +5293,11 @@
       <c r="BE66">
         <v>0.6809700198937206</v>
       </c>
-    </row>
-    <row r="67" spans="1:57">
+      <c r="BF66">
+        <v>1340.191604392026</v>
+      </c>
+    </row>
+    <row r="67" spans="1:58">
       <c r="A67" s="1" t="s">
         <v>63</v>
       </c>
@@ -5361,8 +5370,11 @@
       <c r="BE67">
         <v>6.298046703189611</v>
       </c>
-    </row>
-    <row r="68" spans="1:57">
+      <c r="BF67">
+        <v>13331.23923523152</v>
+      </c>
+    </row>
+    <row r="68" spans="1:58">
       <c r="A68" s="1" t="s">
         <v>64</v>
       </c>
@@ -5435,8 +5447,11 @@
       <c r="BE68">
         <v>7.304603953659534</v>
       </c>
-    </row>
-    <row r="69" spans="1:57">
+      <c r="BF68">
+        <v>25705.07287315651</v>
+      </c>
+    </row>
+    <row r="69" spans="1:58">
       <c r="A69" s="1" t="s">
         <v>65</v>
       </c>
@@ -5509,8 +5524,11 @@
       <c r="BE69">
         <v>0.2742241334868595</v>
       </c>
-    </row>
-    <row r="70" spans="1:57">
+      <c r="BF69">
+        <v>1949.597887802064</v>
+      </c>
+    </row>
+    <row r="70" spans="1:58">
       <c r="A70" s="1" t="s">
         <v>66</v>
       </c>
@@ -5583,8 +5601,11 @@
       <c r="BE70">
         <v>4.972760506421327</v>
       </c>
-    </row>
-    <row r="71" spans="1:57">
+      <c r="BF70">
+        <v>6164.985557787995</v>
+      </c>
+    </row>
+    <row r="71" spans="1:58">
       <c r="A71" s="1" t="s">
         <v>67</v>
       </c>
@@ -5657,8 +5678,11 @@
       <c r="BE71">
         <v>4.723041579052805</v>
       </c>
-    </row>
-    <row r="72" spans="1:57">
+      <c r="BF71">
+        <v>16151.1897315123</v>
+      </c>
+    </row>
+    <row r="72" spans="1:58">
       <c r="A72" s="1" t="s">
         <v>68</v>
       </c>
@@ -5731,8 +5755,11 @@
       <c r="BE72">
         <v>0.2696506427740678</v>
       </c>
-    </row>
-    <row r="73" spans="1:57">
+      <c r="BF72">
+        <v>1470.757508594189</v>
+      </c>
+    </row>
+    <row r="73" spans="1:58">
       <c r="A73" s="1" t="s">
         <v>69</v>
       </c>
@@ -5805,8 +5832,11 @@
       <c r="BE73">
         <v>2.568719942420721</v>
       </c>
-    </row>
-    <row r="74" spans="1:57">
+      <c r="BF73">
+        <v>2080.611127017555</v>
+      </c>
+    </row>
+    <row r="74" spans="1:58">
       <c r="A74" s="1" t="s">
         <v>70</v>
       </c>
@@ -5879,8 +5909,11 @@
       <c r="BE74">
         <v>10.54452222824097</v>
       </c>
-    </row>
-    <row r="75" spans="1:57">
+      <c r="BF74">
+        <v>5397.408730016446</v>
+      </c>
+    </row>
+    <row r="75" spans="1:58">
       <c r="A75" s="1" t="s">
         <v>71</v>
       </c>
@@ -5953,8 +5986,11 @@
       <c r="BE75">
         <v>0.3704864161368459</v>
       </c>
-    </row>
-    <row r="76" spans="1:57">
+      <c r="BF75">
+        <v>779.0691758155526</v>
+      </c>
+    </row>
+    <row r="76" spans="1:58">
       <c r="A76" s="1" t="s">
         <v>72</v>
       </c>
@@ -6027,8 +6063,11 @@
       <c r="BE76">
         <v>11.62228437572718</v>
       </c>
-    </row>
-    <row r="77" spans="1:57">
+      <c r="BF76">
+        <v>11718.02515430384</v>
+      </c>
+    </row>
+    <row r="77" spans="1:58">
       <c r="A77" s="1" t="s">
         <v>73</v>
       </c>
@@ -6101,8 +6140,11 @@
       <c r="BE77">
         <v>25.97905255854129</v>
       </c>
-    </row>
-    <row r="78" spans="1:57">
+      <c r="BF77">
+        <v>21149.79115015452</v>
+      </c>
+    </row>
+    <row r="78" spans="1:58">
       <c r="A78" s="1" t="s">
         <v>74</v>
       </c>
@@ -6175,8 +6217,11 @@
       <c r="BE78">
         <v>2.15244241643697</v>
       </c>
-    </row>
-    <row r="79" spans="1:57">
+      <c r="BF78">
+        <v>1125.352923839777</v>
+      </c>
+    </row>
+    <row r="79" spans="1:58">
       <c r="A79" s="1" t="s">
         <v>75</v>
       </c>
@@ -6249,8 +6294,11 @@
       <c r="BE79">
         <v>4.522884311899542</v>
       </c>
-    </row>
-    <row r="80" spans="1:57">
+      <c r="BF79">
+        <v>2555.231727340843</v>
+      </c>
+    </row>
+    <row r="80" spans="1:58">
       <c r="A80" s="1" t="s">
         <v>76</v>
       </c>
@@ -6322,6 +6370,9 @@
       </c>
       <c r="BE80">
         <v>7.524771695435047</v>
+      </c>
+      <c r="BF80">
+        <v>10280.99735213215</v>
       </c>
     </row>
     <row r="81" spans="1:81">
@@ -6396,6 +6447,9 @@
       </c>
       <c r="BE81">
         <v>2.002981155142188</v>
+      </c>
+      <c r="BF81">
+        <v>1529.402883787179</v>
       </c>
     </row>
     <row r="82" spans="1:81">

</xml_diff>

<commit_message>
updated design and minor imporvements
</commit_message>
<xml_diff>
--- a/excel_files/output.xlsx
+++ b/excel_files/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="83">
   <si>
     <t>C-AAGR</t>
   </si>
@@ -620,13 +620,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CE84"/>
+  <dimension ref="A1:CF84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:83">
+    <row r="1" spans="1:84">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -873,8 +873,11 @@
       <c r="CE1" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="2" spans="1:83">
+      <c r="CF1" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:84">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -966,7 +969,7 @@
         <v>932.17</v>
       </c>
     </row>
-    <row r="3" spans="1:83">
+    <row r="3" spans="1:84">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1058,7 +1061,7 @@
         <v>178.78</v>
       </c>
     </row>
-    <row r="4" spans="1:83">
+    <row r="4" spans="1:84">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1150,7 +1153,7 @@
         <v>74302.3</v>
       </c>
     </row>
-    <row r="5" spans="1:83">
+    <row r="5" spans="1:84">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1245,7 +1248,7 @@
         <v>3864.9</v>
       </c>
     </row>
-    <row r="6" spans="1:83">
+    <row r="6" spans="1:84">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1337,7 +1340,7 @@
         <v>22.91</v>
       </c>
     </row>
-    <row r="7" spans="1:83">
+    <row r="7" spans="1:84">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1429,7 +1432,7 @@
         <v>779.75</v>
       </c>
     </row>
-    <row r="8" spans="1:83">
+    <row r="8" spans="1:84">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1521,7 +1524,7 @@
         <v>863.5599999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:83">
+    <row r="9" spans="1:84">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1616,7 +1619,7 @@
         <v>12232.23</v>
       </c>
     </row>
-    <row r="10" spans="1:83">
+    <row r="10" spans="1:84">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1702,7 +1705,7 @@
         <v>1.42</v>
       </c>
     </row>
-    <row r="11" spans="1:83">
+    <row r="11" spans="1:84">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1797,7 +1800,7 @@
         <v>15632.6</v>
       </c>
     </row>
-    <row r="12" spans="1:83">
+    <row r="12" spans="1:84">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1886,7 +1889,7 @@
         <v>860.4400000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:83">
+    <row r="13" spans="1:84">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1978,7 +1981,7 @@
         <v>13353.97</v>
       </c>
     </row>
-    <row r="14" spans="1:83">
+    <row r="14" spans="1:84">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -2073,7 +2076,7 @@
         <v>84802.46000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:83">
+    <row r="15" spans="1:84">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -2168,7 +2171,7 @@
         <v>2668.03</v>
       </c>
     </row>
-    <row r="16" spans="1:83">
+    <row r="16" spans="1:84">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -4511,7 +4514,7 @@
         <v>3.27</v>
       </c>
     </row>
-    <row r="49" spans="1:83">
+    <row r="49" spans="1:84">
       <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
@@ -4567,7 +4570,7 @@
         <v>6.15</v>
       </c>
     </row>
-    <row r="50" spans="1:83">
+    <row r="50" spans="1:84">
       <c r="A50" s="1" t="s">
         <v>48</v>
       </c>
@@ -4623,7 +4626,7 @@
         <v>18.06</v>
       </c>
     </row>
-    <row r="51" spans="1:83">
+    <row r="51" spans="1:84">
       <c r="A51" s="1" t="s">
         <v>49</v>
       </c>
@@ -4679,7 +4682,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="52" spans="1:83">
+    <row r="52" spans="1:84">
       <c r="A52" s="1" t="s">
         <v>50</v>
       </c>
@@ -4696,7 +4699,7 @@
         <v>12.62</v>
       </c>
     </row>
-    <row r="53" spans="1:83">
+    <row r="53" spans="1:84">
       <c r="A53" s="1" t="s">
         <v>51</v>
       </c>
@@ -4713,7 +4716,7 @@
         <v>86.53</v>
       </c>
     </row>
-    <row r="54" spans="1:83">
+    <row r="54" spans="1:84">
       <c r="A54" s="1" t="s">
         <v>52</v>
       </c>
@@ -4733,7 +4736,7 @@
         <v>3418.74</v>
       </c>
     </row>
-    <row r="55" spans="1:83">
+    <row r="55" spans="1:84">
       <c r="A55" s="1" t="s">
         <v>53</v>
       </c>
@@ -4768,7 +4771,7 @@
         <v>36500.62</v>
       </c>
     </row>
-    <row r="56" spans="1:83">
+    <row r="56" spans="1:84">
       <c r="A56" s="1" t="s">
         <v>54</v>
       </c>
@@ -4800,7 +4803,7 @@
         <v>3985.92</v>
       </c>
     </row>
-    <row r="57" spans="1:83">
+    <row r="57" spans="1:84">
       <c r="A57" s="1" t="s">
         <v>55</v>
       </c>
@@ -4829,15 +4832,69 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="58" spans="1:83">
+    <row r="58" spans="1:84">
       <c r="A58" s="1" t="s">
         <v>56</v>
       </c>
+      <c r="BK58">
+        <v>6990.049284296037</v>
+      </c>
+      <c r="BL58">
+        <v>1340.191604392026</v>
+      </c>
+      <c r="BM58">
+        <v>13331.23923523152</v>
+      </c>
+      <c r="BN58">
+        <v>25705.07287315651</v>
+      </c>
+      <c r="BO58">
+        <v>1949.597887802064</v>
+      </c>
+      <c r="BP58">
+        <v>6164.985557787995</v>
+      </c>
+      <c r="BQ58">
+        <v>16151.1897315123</v>
+      </c>
+      <c r="BR58">
+        <v>1470.757508594189</v>
+      </c>
+      <c r="BS58">
+        <v>2080.611127017555</v>
+      </c>
+      <c r="BT58">
+        <v>5397.408730016446</v>
+      </c>
+      <c r="BU58">
+        <v>779.0691758155526</v>
+      </c>
+      <c r="BV58">
+        <v>11718.02515430384</v>
+      </c>
+      <c r="BW58">
+        <v>21149.79115015452</v>
+      </c>
+      <c r="BX58">
+        <v>1125.352923839777</v>
+      </c>
+      <c r="BY58">
+        <v>2555.231727340843</v>
+      </c>
+      <c r="BZ58">
+        <v>10280.99735213215</v>
+      </c>
+      <c r="CA58">
+        <v>1529.402883787179</v>
+      </c>
       <c r="CC58">
         <v>112199.01</v>
       </c>
-    </row>
-    <row r="59" spans="1:83">
+      <c r="CF58">
+        <v>1314.246116743768</v>
+      </c>
+    </row>
+    <row r="59" spans="1:84">
       <c r="A59" s="1" t="s">
         <v>57</v>
       </c>
@@ -4851,7 +4908,7 @@
         <v>9930.33</v>
       </c>
     </row>
-    <row r="60" spans="1:83">
+    <row r="60" spans="1:84">
       <c r="A60" s="1" t="s">
         <v>58</v>
       </c>
@@ -4859,7 +4916,7 @@
         <v>60156.74</v>
       </c>
     </row>
-    <row r="61" spans="1:83">
+    <row r="61" spans="1:84">
       <c r="A61" s="1" t="s">
         <v>59</v>
       </c>
@@ -4867,7 +4924,7 @@
         <v>3839.16</v>
       </c>
     </row>
-    <row r="62" spans="1:83">
+    <row r="62" spans="1:84">
       <c r="A62" s="1" t="s">
         <v>60</v>
       </c>
@@ -4965,7 +5022,7 @@
         <v>51297.1</v>
       </c>
     </row>
-    <row r="63" spans="1:83">
+    <row r="63" spans="1:84">
       <c r="A63" s="1" t="s">
         <v>78</v>
       </c>
@@ -5066,7 +5123,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="64" spans="1:83">
+    <row r="64" spans="1:84">
       <c r="A64" s="1" t="s">
         <v>82</v>
       </c>
@@ -5139,11 +5196,8 @@
       <c r="BE64">
         <v>0.6143333348818123</v>
       </c>
-      <c r="BF64">
-        <v>1314.246116743768</v>
-      </c>
-    </row>
-    <row r="65" spans="1:58">
+    </row>
+    <row r="65" spans="1:57">
       <c r="A65" s="1" t="s">
         <v>61</v>
       </c>
@@ -5216,11 +5270,8 @@
       <c r="BE65">
         <v>2.83422336127609</v>
       </c>
-      <c r="BF65">
-        <v>6990.049284296037</v>
-      </c>
-    </row>
-    <row r="66" spans="1:58">
+    </row>
+    <row r="66" spans="1:57">
       <c r="A66" s="1" t="s">
         <v>62</v>
       </c>
@@ -5293,11 +5344,8 @@
       <c r="BE66">
         <v>0.6809700198937206</v>
       </c>
-      <c r="BF66">
-        <v>1340.191604392026</v>
-      </c>
-    </row>
-    <row r="67" spans="1:58">
+    </row>
+    <row r="67" spans="1:57">
       <c r="A67" s="1" t="s">
         <v>63</v>
       </c>
@@ -5370,11 +5418,8 @@
       <c r="BE67">
         <v>6.298046703189611</v>
       </c>
-      <c r="BF67">
-        <v>13331.23923523152</v>
-      </c>
-    </row>
-    <row r="68" spans="1:58">
+    </row>
+    <row r="68" spans="1:57">
       <c r="A68" s="1" t="s">
         <v>64</v>
       </c>
@@ -5447,11 +5492,8 @@
       <c r="BE68">
         <v>7.304603953659534</v>
       </c>
-      <c r="BF68">
-        <v>25705.07287315651</v>
-      </c>
-    </row>
-    <row r="69" spans="1:58">
+    </row>
+    <row r="69" spans="1:57">
       <c r="A69" s="1" t="s">
         <v>65</v>
       </c>
@@ -5524,11 +5566,8 @@
       <c r="BE69">
         <v>0.2742241334868595</v>
       </c>
-      <c r="BF69">
-        <v>1949.597887802064</v>
-      </c>
-    </row>
-    <row r="70" spans="1:58">
+    </row>
+    <row r="70" spans="1:57">
       <c r="A70" s="1" t="s">
         <v>66</v>
       </c>
@@ -5601,11 +5640,8 @@
       <c r="BE70">
         <v>4.972760506421327</v>
       </c>
-      <c r="BF70">
-        <v>6164.985557787995</v>
-      </c>
-    </row>
-    <row r="71" spans="1:58">
+    </row>
+    <row r="71" spans="1:57">
       <c r="A71" s="1" t="s">
         <v>67</v>
       </c>
@@ -5678,11 +5714,8 @@
       <c r="BE71">
         <v>4.723041579052805</v>
       </c>
-      <c r="BF71">
-        <v>16151.1897315123</v>
-      </c>
-    </row>
-    <row r="72" spans="1:58">
+    </row>
+    <row r="72" spans="1:57">
       <c r="A72" s="1" t="s">
         <v>68</v>
       </c>
@@ -5755,11 +5788,8 @@
       <c r="BE72">
         <v>0.2696506427740678</v>
       </c>
-      <c r="BF72">
-        <v>1470.757508594189</v>
-      </c>
-    </row>
-    <row r="73" spans="1:58">
+    </row>
+    <row r="73" spans="1:57">
       <c r="A73" s="1" t="s">
         <v>69</v>
       </c>
@@ -5832,11 +5862,8 @@
       <c r="BE73">
         <v>2.568719942420721</v>
       </c>
-      <c r="BF73">
-        <v>2080.611127017555</v>
-      </c>
-    </row>
-    <row r="74" spans="1:58">
+    </row>
+    <row r="74" spans="1:57">
       <c r="A74" s="1" t="s">
         <v>70</v>
       </c>
@@ -5909,11 +5936,8 @@
       <c r="BE74">
         <v>10.54452222824097</v>
       </c>
-      <c r="BF74">
-        <v>5397.408730016446</v>
-      </c>
-    </row>
-    <row r="75" spans="1:58">
+    </row>
+    <row r="75" spans="1:57">
       <c r="A75" s="1" t="s">
         <v>71</v>
       </c>
@@ -5986,11 +6010,8 @@
       <c r="BE75">
         <v>0.3704864161368459</v>
       </c>
-      <c r="BF75">
-        <v>779.0691758155526</v>
-      </c>
-    </row>
-    <row r="76" spans="1:58">
+    </row>
+    <row r="76" spans="1:57">
       <c r="A76" s="1" t="s">
         <v>72</v>
       </c>
@@ -6063,11 +6084,8 @@
       <c r="BE76">
         <v>11.62228437572718</v>
       </c>
-      <c r="BF76">
-        <v>11718.02515430384</v>
-      </c>
-    </row>
-    <row r="77" spans="1:58">
+    </row>
+    <row r="77" spans="1:57">
       <c r="A77" s="1" t="s">
         <v>73</v>
       </c>
@@ -6140,11 +6158,8 @@
       <c r="BE77">
         <v>25.97905255854129</v>
       </c>
-      <c r="BF77">
-        <v>21149.79115015452</v>
-      </c>
-    </row>
-    <row r="78" spans="1:58">
+    </row>
+    <row r="78" spans="1:57">
       <c r="A78" s="1" t="s">
         <v>74</v>
       </c>
@@ -6217,11 +6232,8 @@
       <c r="BE78">
         <v>2.15244241643697</v>
       </c>
-      <c r="BF78">
-        <v>1125.352923839777</v>
-      </c>
-    </row>
-    <row r="79" spans="1:58">
+    </row>
+    <row r="79" spans="1:57">
       <c r="A79" s="1" t="s">
         <v>75</v>
       </c>
@@ -6294,11 +6306,8 @@
       <c r="BE79">
         <v>4.522884311899542</v>
       </c>
-      <c r="BF79">
-        <v>2555.231727340843</v>
-      </c>
-    </row>
-    <row r="80" spans="1:58">
+    </row>
+    <row r="80" spans="1:57">
       <c r="A80" s="1" t="s">
         <v>76</v>
       </c>
@@ -6370,9 +6379,6 @@
       </c>
       <c r="BE80">
         <v>7.524771695435047</v>
-      </c>
-      <c r="BF80">
-        <v>10280.99735213215</v>
       </c>
     </row>
     <row r="81" spans="1:81">
@@ -6447,9 +6453,6 @@
       </c>
       <c r="BE81">
         <v>2.002981155142188</v>
-      </c>
-      <c r="BF81">
-        <v>1529.402883787179</v>
       </c>
     </row>
     <row r="82" spans="1:81">

</xml_diff>

<commit_message>
moved most settings apart from mapping to UI
</commit_message>
<xml_diff>
--- a/excel_files/output.xlsx
+++ b/excel_files/output.xlsx
@@ -4837,61 +4837,61 @@
         <v>56</v>
       </c>
       <c r="BK58">
-        <v>6990.049284296037</v>
+        <v>7078.174746093063</v>
       </c>
       <c r="BL58">
-        <v>1340.191604392026</v>
+        <v>1444.393869164158</v>
       </c>
       <c r="BM58">
-        <v>13331.23923523152</v>
+        <v>12838.60618591949</v>
       </c>
       <c r="BN58">
-        <v>25705.07287315651</v>
+        <v>25756.04642876922</v>
       </c>
       <c r="BO58">
-        <v>1949.597887802064</v>
+        <v>1995.628295730427</v>
       </c>
       <c r="BP58">
-        <v>6164.985557787995</v>
+        <v>5869.649075423349</v>
       </c>
       <c r="BQ58">
-        <v>16151.1897315123</v>
+        <v>15978.87289030425</v>
       </c>
       <c r="BR58">
-        <v>1470.757508594189</v>
+        <v>1723.667646666086</v>
       </c>
       <c r="BS58">
-        <v>2080.611127017555</v>
+        <v>1949.314980610249</v>
       </c>
       <c r="BT58">
-        <v>5397.408730016446</v>
+        <v>5630.730755461873</v>
       </c>
       <c r="BU58">
-        <v>779.0691758155526</v>
+        <v>764.6444049755133</v>
       </c>
       <c r="BV58">
-        <v>11718.02515430384</v>
+        <v>10806.28559654408</v>
       </c>
       <c r="BW58">
-        <v>21149.79115015452</v>
+        <v>22094.55055163287</v>
       </c>
       <c r="BX58">
-        <v>1125.352923839777</v>
+        <v>1261.475488687794</v>
       </c>
       <c r="BY58">
-        <v>2555.231727340843</v>
+        <v>2425.322495755267</v>
       </c>
       <c r="BZ58">
-        <v>10280.99735213215</v>
+        <v>10659.60169516933</v>
       </c>
       <c r="CA58">
-        <v>1529.402883787179</v>
+        <v>1524.323987165695</v>
       </c>
       <c r="CC58">
         <v>112199.01</v>
       </c>
       <c r="CF58">
-        <v>1314.246116743768</v>
+        <v>1231.931639694078</v>
       </c>
     </row>
     <row r="59" spans="1:84">
@@ -5128,73 +5128,73 @@
         <v>82</v>
       </c>
       <c r="AH64">
-        <v>9.414114025598392</v>
+        <v>10.32749597553164</v>
       </c>
       <c r="AI64">
-        <v>4.98343871824909</v>
+        <v>4.572988519864158</v>
       </c>
       <c r="AJ64">
-        <v>200.4209536320157</v>
+        <v>181.3535974402819</v>
       </c>
       <c r="AK64">
-        <v>4.98343871824909</v>
+        <v>4.572988519864158</v>
       </c>
       <c r="AL64">
-        <v>200.4209536320157</v>
+        <v>181.3535974402819</v>
       </c>
       <c r="AN64">
-        <v>3.583830243987031</v>
+        <v>3.242894353428856</v>
       </c>
       <c r="AO64">
-        <v>3.583830243987031</v>
+        <v>3.242894353428856</v>
       </c>
       <c r="AP64">
-        <v>11.83001546522602</v>
+        <v>10.59236898211762</v>
       </c>
       <c r="AQ64">
-        <v>0.882314035994932</v>
+        <v>0.8428759983042254</v>
       </c>
       <c r="AR64">
-        <v>0.882314035994932</v>
+        <v>0.8428759983042254</v>
       </c>
       <c r="AS64">
-        <v>73.19743904368953</v>
+        <v>67.1392593125347</v>
       </c>
       <c r="AT64">
-        <v>192.0036300258339</v>
+        <v>187.1088795390912</v>
       </c>
       <c r="AU64">
-        <v>192.0036300258339</v>
+        <v>187.1088795390912</v>
       </c>
       <c r="AV64">
-        <v>192.0036300258339</v>
+        <v>187.1088795390912</v>
       </c>
       <c r="AW64">
-        <v>8.166333993524313</v>
+        <v>7.32389857172966</v>
       </c>
       <c r="AX64">
-        <v>22.61657591545954</v>
+        <v>21.63126105456613</v>
       </c>
       <c r="AY64">
-        <v>0.6143333348818123</v>
+        <v>0.576311818435788</v>
       </c>
       <c r="AZ64">
-        <v>38.40820165850223</v>
+        <v>34.48267618393898</v>
       </c>
       <c r="BA64">
-        <v>38.40820165850223</v>
+        <v>34.48267618393898</v>
       </c>
       <c r="BB64">
-        <v>38.40820165850223</v>
+        <v>34.48267618393898</v>
       </c>
       <c r="BC64">
-        <v>38.40820165850223</v>
+        <v>34.48267618393898</v>
       </c>
       <c r="BD64">
-        <v>38.40820165850223</v>
+        <v>34.48267618393898</v>
       </c>
       <c r="BE64">
-        <v>0.6143333348818123</v>
+        <v>0.576311818435788</v>
       </c>
     </row>
     <row r="65" spans="1:57">
@@ -5202,73 +5202,73 @@
         <v>61</v>
       </c>
       <c r="AH65">
-        <v>59.33229717329145</v>
+        <v>55.62435575969518</v>
       </c>
       <c r="AI65">
-        <v>52.88727739527822</v>
+        <v>51.37581306248904</v>
       </c>
       <c r="AJ65">
-        <v>2386.627410095036</v>
+        <v>2374.258369275034</v>
       </c>
       <c r="AK65">
-        <v>52.88727739527822</v>
+        <v>51.37581306248904</v>
       </c>
       <c r="AL65">
-        <v>2386.627410095036</v>
+        <v>2374.258369275034</v>
       </c>
       <c r="AN65">
-        <v>16.82216917671263</v>
+        <v>17.37251496220007</v>
       </c>
       <c r="AO65">
-        <v>16.82216917671263</v>
+        <v>17.37251496220007</v>
       </c>
       <c r="AP65">
-        <v>75.89979358144105</v>
+        <v>76.32228273190559</v>
       </c>
       <c r="AQ65">
-        <v>9.907512448914348</v>
+        <v>10.02416591662914</v>
       </c>
       <c r="AR65">
-        <v>9.907512448914348</v>
+        <v>10.02416591662914</v>
       </c>
       <c r="AS65">
-        <v>168.617042367179</v>
+        <v>189.7119347106106</v>
       </c>
       <c r="AT65">
-        <v>337.3299611688592</v>
+        <v>383.2473745921999</v>
       </c>
       <c r="AU65">
-        <v>337.3299611688592</v>
+        <v>383.2473745921999</v>
       </c>
       <c r="AV65">
-        <v>337.3299611688592</v>
+        <v>383.2473745921999</v>
       </c>
       <c r="AW65">
-        <v>15.90577829927206</v>
+        <v>16.16081960052252</v>
       </c>
       <c r="AX65">
-        <v>164.5034938763827</v>
+        <v>159.3026870578528</v>
       </c>
       <c r="AY65">
-        <v>2.83422336127609</v>
+        <v>2.813445122912526</v>
       </c>
       <c r="AZ65">
-        <v>111.1287621074915</v>
+        <v>103.9243851554692</v>
       </c>
       <c r="BA65">
-        <v>111.1287621074915</v>
+        <v>103.9243851554692</v>
       </c>
       <c r="BB65">
-        <v>111.1287621074915</v>
+        <v>103.9243851554692</v>
       </c>
       <c r="BC65">
-        <v>111.1287621074915</v>
+        <v>103.9243851554692</v>
       </c>
       <c r="BD65">
-        <v>111.1287621074915</v>
+        <v>103.9243851554692</v>
       </c>
       <c r="BE65">
-        <v>2.83422336127609</v>
+        <v>2.813445122912526</v>
       </c>
     </row>
     <row r="66" spans="1:57">
@@ -5276,73 +5276,73 @@
         <v>62</v>
       </c>
       <c r="AH66">
-        <v>7.205654163155705</v>
+        <v>7.047710597058758</v>
       </c>
       <c r="AI66">
-        <v>4.216897656582296</v>
+        <v>3.990203469153494</v>
       </c>
       <c r="AJ66">
-        <v>424.28795445811</v>
+        <v>458.6134734524042</v>
       </c>
       <c r="AK66">
-        <v>4.216897656582296</v>
+        <v>3.990203469153494</v>
       </c>
       <c r="AL66">
-        <v>424.28795445811</v>
+        <v>458.6134734524042</v>
       </c>
       <c r="AN66">
-        <v>3.524966271901503</v>
+        <v>3.954541075909511</v>
       </c>
       <c r="AO66">
-        <v>3.524966271901503</v>
+        <v>3.954541075909511</v>
       </c>
       <c r="AP66">
-        <v>14.83037091043778</v>
+        <v>15.17512013768777</v>
       </c>
       <c r="AQ66">
-        <v>2.587943928549066</v>
+        <v>2.719587604282424</v>
       </c>
       <c r="AR66">
-        <v>2.587943928549066</v>
+        <v>2.719587604282424</v>
       </c>
       <c r="AS66">
-        <v>15.87995030975901</v>
+        <v>15.26135000328533</v>
       </c>
       <c r="AT66">
-        <v>95.40936142164284</v>
+        <v>104.1169870545808</v>
       </c>
       <c r="AU66">
-        <v>95.40936142164284</v>
+        <v>104.1169870545808</v>
       </c>
       <c r="AV66">
-        <v>95.40936142164284</v>
+        <v>104.1169870545808</v>
       </c>
       <c r="AW66">
-        <v>4.508362703770399</v>
+        <v>4.574907561019063</v>
       </c>
       <c r="AX66">
-        <v>20.73699029148556</v>
+        <v>22.23482795781456</v>
       </c>
       <c r="AY66">
-        <v>0.6809700198937206</v>
+        <v>0.7343764872662722</v>
       </c>
       <c r="AZ66">
-        <v>24.04094541568309</v>
+        <v>25.54492551310361</v>
       </c>
       <c r="BA66">
-        <v>24.04094541568309</v>
+        <v>25.54492551310361</v>
       </c>
       <c r="BB66">
-        <v>24.04094541568309</v>
+        <v>25.54492551310361</v>
       </c>
       <c r="BC66">
-        <v>24.04094541568309</v>
+        <v>25.54492551310361</v>
       </c>
       <c r="BD66">
-        <v>24.04094541568309</v>
+        <v>25.54492551310361</v>
       </c>
       <c r="BE66">
-        <v>0.6809700198937206</v>
+        <v>0.7343764872662722</v>
       </c>
     </row>
     <row r="67" spans="1:57">
@@ -5350,73 +5350,73 @@
         <v>63</v>
       </c>
       <c r="AH67">
-        <v>85.96996595606208</v>
+        <v>88.13898866191506</v>
       </c>
       <c r="AI67">
-        <v>45.81034803465009</v>
+        <v>46.80938113369048</v>
       </c>
       <c r="AJ67">
-        <v>1067.650717165209</v>
+        <v>1055.319351939931</v>
       </c>
       <c r="AK67">
-        <v>45.81034803465009</v>
+        <v>46.80938113369048</v>
       </c>
       <c r="AL67">
-        <v>1067.650717165209</v>
+        <v>1055.319351939931</v>
       </c>
       <c r="AN67">
-        <v>21.2452943026647</v>
+        <v>20.47571496848017</v>
       </c>
       <c r="AO67">
-        <v>21.2452943026647</v>
+        <v>20.47571496848017</v>
       </c>
       <c r="AP67">
-        <v>67.45605026192963</v>
+        <v>64.813621731475</v>
       </c>
       <c r="AQ67">
-        <v>3.648380930209532</v>
+        <v>3.584853507205844</v>
       </c>
       <c r="AR67">
-        <v>3.648380930209532</v>
+        <v>3.584853507205844</v>
       </c>
       <c r="AS67">
-        <v>1017.25321948424</v>
+        <v>983.8413402225077</v>
       </c>
       <c r="AT67">
-        <v>2296.914724432677</v>
+        <v>2134.991636324525</v>
       </c>
       <c r="AU67">
-        <v>2296.914724432677</v>
+        <v>2134.991636324525</v>
       </c>
       <c r="AV67">
-        <v>2296.914724432677</v>
+        <v>2134.991636324525</v>
       </c>
       <c r="AW67">
-        <v>57.67828812599182</v>
+        <v>56.55622662901879</v>
       </c>
       <c r="AX67">
-        <v>253.528219165653</v>
+        <v>256.5261487729848</v>
       </c>
       <c r="AY67">
-        <v>6.298046703189611</v>
+        <v>6.381567758470773</v>
       </c>
       <c r="AZ67">
-        <v>533.8607489335537</v>
+        <v>543.7226424624921</v>
       </c>
       <c r="BA67">
-        <v>533.8607489335537</v>
+        <v>543.7226424624921</v>
       </c>
       <c r="BB67">
-        <v>533.8607489335537</v>
+        <v>543.7226424624921</v>
       </c>
       <c r="BC67">
-        <v>533.8607489335537</v>
+        <v>543.7226424624921</v>
       </c>
       <c r="BD67">
-        <v>533.8607489335537</v>
+        <v>543.7226424624921</v>
       </c>
       <c r="BE67">
-        <v>6.298046703189611</v>
+        <v>6.381567758470773</v>
       </c>
     </row>
     <row r="68" spans="1:57">
@@ -5424,73 +5424,73 @@
         <v>64</v>
       </c>
       <c r="AH68">
-        <v>210.7794315168262</v>
+        <v>219.239612736702</v>
       </c>
       <c r="AI68">
-        <v>300.8081789076329</v>
+        <v>307.289012221992</v>
       </c>
       <c r="AJ68">
-        <v>4553.744405761063</v>
+        <v>4580.026900641024</v>
       </c>
       <c r="AK68">
-        <v>300.8081789076329</v>
+        <v>307.289012221992</v>
       </c>
       <c r="AL68">
-        <v>4553.744405761063</v>
+        <v>4580.026900641024</v>
       </c>
       <c r="AN68">
-        <v>71.71276636935771</v>
+        <v>71.96046021983028</v>
       </c>
       <c r="AO68">
-        <v>71.71276636935771</v>
+        <v>71.96046021983028</v>
       </c>
       <c r="AP68">
-        <v>425.0448387694359</v>
+        <v>427.6999570736289</v>
       </c>
       <c r="AQ68">
-        <v>24.91756613589823</v>
+        <v>24.70265532545745</v>
       </c>
       <c r="AR68">
-        <v>24.91756613589823</v>
+        <v>24.70265532545745</v>
       </c>
       <c r="AS68">
-        <v>1199.389830690175</v>
+        <v>1274.942523638755</v>
       </c>
       <c r="AT68">
-        <v>3500.822733426095</v>
+        <v>3465.241693329811</v>
       </c>
       <c r="AU68">
-        <v>3500.822733426095</v>
+        <v>3465.241693329811</v>
       </c>
       <c r="AV68">
-        <v>3500.822733426095</v>
+        <v>3465.241693329811</v>
       </c>
       <c r="AW68">
-        <v>55.08900470733643</v>
+        <v>55.81736481785774</v>
       </c>
       <c r="AX68">
-        <v>787.1122351065278</v>
+        <v>815.0322411715983</v>
       </c>
       <c r="AY68">
-        <v>7.304603953659534</v>
+        <v>7.278745202422141</v>
       </c>
       <c r="AZ68">
-        <v>521.6428579665424</v>
+        <v>517.0148204239607</v>
       </c>
       <c r="BA68">
-        <v>521.6428579665424</v>
+        <v>517.0148204239607</v>
       </c>
       <c r="BB68">
-        <v>521.6428579665424</v>
+        <v>517.0148204239607</v>
       </c>
       <c r="BC68">
-        <v>521.6428579665424</v>
+        <v>517.0148204239607</v>
       </c>
       <c r="BD68">
-        <v>521.6428579665424</v>
+        <v>517.0148204239607</v>
       </c>
       <c r="BE68">
-        <v>7.304603953659534</v>
+        <v>7.278745202422141</v>
       </c>
     </row>
     <row r="69" spans="1:57">
@@ -5498,73 +5498,73 @@
         <v>65</v>
       </c>
       <c r="AH69">
-        <v>17.85041145477444</v>
+        <v>18.53883464202285</v>
       </c>
       <c r="AI69">
-        <v>28.15027438197285</v>
+        <v>29.33736850079149</v>
       </c>
       <c r="AJ69">
-        <v>377.6822184351739</v>
+        <v>418.786363815777</v>
       </c>
       <c r="AK69">
-        <v>28.15027438197285</v>
+        <v>29.33736850079149</v>
       </c>
       <c r="AL69">
-        <v>377.6822184351739</v>
+        <v>418.786363815777</v>
       </c>
       <c r="AN69">
-        <v>4.714462637193501</v>
+        <v>4.858426191443577</v>
       </c>
       <c r="AO69">
-        <v>4.714462637193501</v>
+        <v>4.858426191443577</v>
       </c>
       <c r="AP69">
-        <v>49.16584968741984</v>
+        <v>50.61843925260008</v>
       </c>
       <c r="AQ69">
-        <v>2.893772782757878</v>
+        <v>2.979895184142515</v>
       </c>
       <c r="AR69">
-        <v>2.893772782757878</v>
+        <v>2.979895184142515</v>
       </c>
       <c r="AS69">
-        <v>33.3963167022774</v>
+        <v>36.33592108886689</v>
       </c>
       <c r="AT69">
-        <v>255.6969061620534</v>
+        <v>240.4236348219589</v>
       </c>
       <c r="AU69">
-        <v>255.6969061620534</v>
+        <v>240.4236348219589</v>
       </c>
       <c r="AV69">
-        <v>255.6969061620534</v>
+        <v>240.4236348219589</v>
       </c>
       <c r="AW69">
-        <v>5.374387093633413</v>
+        <v>5.169273956120015</v>
       </c>
       <c r="AX69">
-        <v>25.69650055831298</v>
+        <v>27.46067404816858</v>
       </c>
       <c r="AY69">
-        <v>0.2742241334868595</v>
+        <v>0.2682642942527309</v>
       </c>
       <c r="AZ69">
-        <v>44.71875981566311</v>
+        <v>44.75472246079148</v>
       </c>
       <c r="BA69">
-        <v>44.71875981566311</v>
+        <v>44.75472246079148</v>
       </c>
       <c r="BB69">
-        <v>44.71875981566311</v>
+        <v>44.75472246079148</v>
       </c>
       <c r="BC69">
-        <v>44.71875981566311</v>
+        <v>44.75472246079148</v>
       </c>
       <c r="BD69">
-        <v>44.71875981566311</v>
+        <v>44.75472246079148</v>
       </c>
       <c r="BE69">
-        <v>0.2742241334868595</v>
+        <v>0.2682642942527309</v>
       </c>
     </row>
     <row r="70" spans="1:57">
@@ -5572,73 +5572,73 @@
         <v>66</v>
       </c>
       <c r="AH70">
-        <v>22.72248552095145</v>
+        <v>19.97223727237433</v>
       </c>
       <c r="AI70">
-        <v>26.40249624270946</v>
+        <v>25.96263036634773</v>
       </c>
       <c r="AJ70">
-        <v>551.2811292873323</v>
+        <v>526.1549890216626</v>
       </c>
       <c r="AK70">
-        <v>26.40249624270946</v>
+        <v>25.96263036634773</v>
       </c>
       <c r="AL70">
-        <v>551.2811292873323</v>
+        <v>526.1549890216626</v>
       </c>
       <c r="AN70">
-        <v>4.544429623456672</v>
+        <v>4.432074601035565</v>
       </c>
       <c r="AO70">
-        <v>4.544429623456672</v>
+        <v>4.432074601035565</v>
       </c>
       <c r="AP70">
-        <v>15.6135156785883</v>
+        <v>14.37950947392732</v>
       </c>
       <c r="AQ70">
-        <v>1.124677603738382</v>
+        <v>1.066733890632168</v>
       </c>
       <c r="AR70">
-        <v>1.124677603738382</v>
+        <v>1.066733890632168</v>
       </c>
       <c r="AS70">
-        <v>224.3877803584561</v>
+        <v>208.6571391646564</v>
       </c>
       <c r="AT70">
-        <v>1211.574020833299</v>
+        <v>1132.170541267768</v>
       </c>
       <c r="AU70">
-        <v>1211.574020833299</v>
+        <v>1132.170541267768</v>
       </c>
       <c r="AV70">
-        <v>1211.574020833299</v>
+        <v>1132.170541267768</v>
       </c>
       <c r="AW70">
-        <v>13.75366018712521</v>
+        <v>13.81265972405672</v>
       </c>
       <c r="AX70">
-        <v>151.1198314923793</v>
+        <v>150.4025145620108</v>
       </c>
       <c r="AY70">
-        <v>4.972760506421327</v>
+        <v>5.01814355880022</v>
       </c>
       <c r="AZ70">
-        <v>185.2030471046567</v>
+        <v>188.1288497092128</v>
       </c>
       <c r="BA70">
-        <v>185.2030471046567</v>
+        <v>188.1288497092128</v>
       </c>
       <c r="BB70">
-        <v>185.2030471046567</v>
+        <v>188.1288497092128</v>
       </c>
       <c r="BC70">
-        <v>185.2030471046567</v>
+        <v>188.1288497092128</v>
       </c>
       <c r="BD70">
-        <v>185.2030471046567</v>
+        <v>188.1288497092128</v>
       </c>
       <c r="BE70">
-        <v>4.972760506421327</v>
+        <v>5.01814355880022</v>
       </c>
     </row>
     <row r="71" spans="1:57">
@@ -5646,73 +5646,73 @@
         <v>67</v>
       </c>
       <c r="AH71">
-        <v>86.79474751248956</v>
+        <v>82.58001702383162</v>
       </c>
       <c r="AI71">
-        <v>139.8593661420047</v>
+        <v>127.9566214829683</v>
       </c>
       <c r="AJ71">
-        <v>1530.035279196426</v>
+        <v>1489.914490683451</v>
       </c>
       <c r="AK71">
-        <v>139.8593661420047</v>
+        <v>127.9566214829683</v>
       </c>
       <c r="AL71">
-        <v>1530.035279196426</v>
+        <v>1489.914490683451</v>
       </c>
       <c r="AN71">
-        <v>27.99167295109481</v>
+        <v>27.35663459844887</v>
       </c>
       <c r="AO71">
-        <v>27.99167295109481</v>
+        <v>27.35663459844887</v>
       </c>
       <c r="AP71">
-        <v>188.5514367929101</v>
+        <v>182.8487649159133</v>
       </c>
       <c r="AQ71">
-        <v>9.954080538451672</v>
+        <v>9.322926331870258</v>
       </c>
       <c r="AR71">
-        <v>9.954080538451672</v>
+        <v>9.322926331870258</v>
       </c>
       <c r="AS71">
-        <v>898.22598473683</v>
+        <v>908.189632204175</v>
       </c>
       <c r="AT71">
-        <v>3174.076085808873</v>
+        <v>3165.645268564821</v>
       </c>
       <c r="AU71">
-        <v>3174.076085808873</v>
+        <v>3165.645268564821</v>
       </c>
       <c r="AV71">
-        <v>3174.076085808873</v>
+        <v>3165.645268564821</v>
       </c>
       <c r="AW71">
-        <v>25.92668635845184</v>
+        <v>25.104587200284</v>
       </c>
       <c r="AX71">
-        <v>885.2735020026564</v>
+        <v>860.8514303967356</v>
       </c>
       <c r="AY71">
-        <v>4.723041579052805</v>
+        <v>4.486814143210649</v>
       </c>
       <c r="AZ71">
-        <v>223.8124471736551</v>
+        <v>220.8575356777907</v>
       </c>
       <c r="BA71">
-        <v>223.8124471736551</v>
+        <v>220.8575356777907</v>
       </c>
       <c r="BB71">
-        <v>223.8124471736551</v>
+        <v>220.8575356777907</v>
       </c>
       <c r="BC71">
-        <v>223.8124471736551</v>
+        <v>220.8575356777907</v>
       </c>
       <c r="BD71">
-        <v>223.8124471736551</v>
+        <v>220.8575356777907</v>
       </c>
       <c r="BE71">
-        <v>4.723041579052805</v>
+        <v>4.486814143210649</v>
       </c>
     </row>
     <row r="72" spans="1:57">
@@ -5720,73 +5720,73 @@
         <v>68</v>
       </c>
       <c r="AH72">
-        <v>13.98811280122027</v>
+        <v>12.12657052198425</v>
       </c>
       <c r="AI72">
-        <v>15.2970779588446</v>
+        <v>16.9015228160657</v>
       </c>
       <c r="AJ72">
-        <v>153.0186887697224</v>
+        <v>159.946241059103</v>
       </c>
       <c r="AK72">
-        <v>15.2970779588446</v>
+        <v>16.9015228160657</v>
       </c>
       <c r="AL72">
-        <v>153.0186887697224</v>
+        <v>159.946241059103</v>
       </c>
       <c r="AN72">
-        <v>3.391067505558021</v>
+        <v>3.432808256540448</v>
       </c>
       <c r="AO72">
-        <v>3.391067505558021</v>
+        <v>3.432808256540448</v>
       </c>
       <c r="AP72">
-        <v>36.30120203226805</v>
+        <v>38.0822760284692</v>
       </c>
       <c r="AQ72">
-        <v>1.918124681361951</v>
+        <v>1.902591010485776</v>
       </c>
       <c r="AR72">
-        <v>1.918124681361951</v>
+        <v>1.902591010485776</v>
       </c>
       <c r="AS72">
-        <v>89.16462504421361</v>
+        <v>94.14558300572448</v>
       </c>
       <c r="AT72">
-        <v>210.5832067055814</v>
+        <v>284.2840808640421</v>
       </c>
       <c r="AU72">
-        <v>210.5832067055814</v>
+        <v>284.2840808640421</v>
       </c>
       <c r="AV72">
-        <v>210.5832067055814</v>
+        <v>284.2840808640421</v>
       </c>
       <c r="AW72">
-        <v>5.622723040729761</v>
+        <v>5.659491407871246</v>
       </c>
       <c r="AX72">
-        <v>36.43868462974206</v>
+        <v>37.07372726369649</v>
       </c>
       <c r="AY72">
-        <v>0.2696506427740678</v>
+        <v>0.2551628283038735</v>
       </c>
       <c r="AZ72">
-        <v>61.94066436254979</v>
+        <v>63.77022078104318</v>
       </c>
       <c r="BA72">
-        <v>61.94066436254979</v>
+        <v>63.77022078104318</v>
       </c>
       <c r="BB72">
-        <v>61.94066436254979</v>
+        <v>63.77022078104318</v>
       </c>
       <c r="BC72">
-        <v>61.94066436254979</v>
+        <v>63.77022078104318</v>
       </c>
       <c r="BD72">
-        <v>61.94066436254979</v>
+        <v>63.77022078104318</v>
       </c>
       <c r="BE72">
-        <v>0.2696506427740678</v>
+        <v>0.2551628283038735</v>
       </c>
     </row>
     <row r="73" spans="1:57">
@@ -5794,73 +5794,73 @@
         <v>69</v>
       </c>
       <c r="AH73">
-        <v>20.77479004822672</v>
+        <v>20.19569584663957</v>
       </c>
       <c r="AI73">
-        <v>4.852747014700435</v>
+        <v>4.658376157283783</v>
       </c>
       <c r="AJ73">
-        <v>48.24235908871516</v>
+        <v>45.04365638662479</v>
       </c>
       <c r="AK73">
-        <v>4.852747014700435</v>
+        <v>4.658376157283783</v>
       </c>
       <c r="AL73">
-        <v>48.24235908871516</v>
+        <v>45.04365638662479</v>
       </c>
       <c r="AN73">
-        <v>4.100118934209458</v>
+        <v>3.658679197728634</v>
       </c>
       <c r="AO73">
-        <v>4.100118934209458</v>
+        <v>3.658679197728634</v>
       </c>
       <c r="AP73">
-        <v>5.887614787886851</v>
+        <v>5.007552876747213</v>
       </c>
       <c r="AQ73">
-        <v>1.975540813524276</v>
+        <v>1.805033399374224</v>
       </c>
       <c r="AR73">
-        <v>1.975540813524276</v>
+        <v>1.805033399374224</v>
       </c>
       <c r="AS73">
-        <v>94.09361228807829</v>
+        <v>86.93084141239524</v>
       </c>
       <c r="AT73">
-        <v>432.1870895471797</v>
+        <v>404.7909514588491</v>
       </c>
       <c r="AU73">
-        <v>432.1870895471797</v>
+        <v>404.7909514588491</v>
       </c>
       <c r="AV73">
-        <v>432.1870895471797</v>
+        <v>404.7909514588491</v>
       </c>
       <c r="AW73">
-        <v>7.274246802926064</v>
+        <v>6.744798259437085</v>
       </c>
       <c r="AX73">
-        <v>48.43849489577114</v>
+        <v>43.96498101418837</v>
       </c>
       <c r="AY73">
-        <v>2.568719942420721</v>
+        <v>2.483003831617534</v>
       </c>
       <c r="AZ73">
-        <v>96.82042559319736</v>
+        <v>91.36015177580715</v>
       </c>
       <c r="BA73">
-        <v>96.82042559319736</v>
+        <v>91.36015177580715</v>
       </c>
       <c r="BB73">
-        <v>96.82042559319736</v>
+        <v>91.36015177580715</v>
       </c>
       <c r="BC73">
-        <v>96.82042559319736</v>
+        <v>91.36015177580715</v>
       </c>
       <c r="BD73">
-        <v>96.82042559319736</v>
+        <v>91.36015177580715</v>
       </c>
       <c r="BE73">
-        <v>2.568719942420721</v>
+        <v>2.483003831617534</v>
       </c>
     </row>
     <row r="74" spans="1:57">
@@ -5868,73 +5868,73 @@
         <v>70</v>
       </c>
       <c r="AH74">
-        <v>6.972353674806655</v>
+        <v>7.307339250911028</v>
       </c>
       <c r="AI74">
-        <v>12.21744870962575</v>
+        <v>13.69840459926054</v>
       </c>
       <c r="AJ74">
-        <v>199.71937682949</v>
+        <v>199.3395090688811</v>
       </c>
       <c r="AK74">
-        <v>12.21744870962575</v>
+        <v>13.69840459926054</v>
       </c>
       <c r="AL74">
-        <v>199.71937682949</v>
+        <v>199.3395090688811</v>
       </c>
       <c r="AN74">
-        <v>18.19257926173508</v>
+        <v>18.56679355151951</v>
       </c>
       <c r="AO74">
-        <v>18.19257926173508</v>
+        <v>18.56679355151951</v>
       </c>
       <c r="AP74">
-        <v>18.15562672873959</v>
+        <v>21.40766636753455</v>
       </c>
       <c r="AQ74">
-        <v>11.11295016352087</v>
+        <v>11.34297313652933</v>
       </c>
       <c r="AR74">
-        <v>11.11295016352087</v>
+        <v>11.34297313652933</v>
       </c>
       <c r="AS74">
-        <v>263.5501914815977</v>
+        <v>256.3085316904262</v>
       </c>
       <c r="AT74">
-        <v>908.7285465851427</v>
+        <v>968.3056329841913</v>
       </c>
       <c r="AU74">
-        <v>908.7285465851427</v>
+        <v>968.3056329841913</v>
       </c>
       <c r="AV74">
-        <v>908.7285465851427</v>
+        <v>968.3056329841913</v>
       </c>
       <c r="AW74">
-        <v>15.00309596955776</v>
+        <v>15.95331169366837</v>
       </c>
       <c r="AX74">
-        <v>157.2740013517439</v>
+        <v>162.2239578679204</v>
       </c>
       <c r="AY74">
-        <v>10.54452222824097</v>
+        <v>10.75007495641708</v>
       </c>
       <c r="AZ74">
-        <v>341.338813333869</v>
+        <v>351.0435078027249</v>
       </c>
       <c r="BA74">
-        <v>341.338813333869</v>
+        <v>351.0435078027249</v>
       </c>
       <c r="BB74">
-        <v>341.338813333869</v>
+        <v>351.0435078027249</v>
       </c>
       <c r="BC74">
-        <v>341.338813333869</v>
+        <v>351.0435078027249</v>
       </c>
       <c r="BD74">
-        <v>341.338813333869</v>
+        <v>351.0435078027249</v>
       </c>
       <c r="BE74">
-        <v>10.54452222824097</v>
+        <v>10.75007495641708</v>
       </c>
     </row>
     <row r="75" spans="1:57">
@@ -5942,73 +5942,73 @@
         <v>71</v>
       </c>
       <c r="AH75">
-        <v>0.5680094407271827</v>
+        <v>0.601618711395422</v>
       </c>
       <c r="AI75">
-        <v>0.6389008355734405</v>
+        <v>0.9516931460180786</v>
       </c>
       <c r="AJ75">
-        <v>21.40426394213398</v>
+        <v>23.80405625421961</v>
       </c>
       <c r="AK75">
-        <v>0.6389008355734405</v>
+        <v>0.9516931460180786</v>
       </c>
       <c r="AL75">
-        <v>21.40426394213398</v>
+        <v>23.80405625421961</v>
       </c>
       <c r="AN75">
-        <v>3.499278473271989</v>
+        <v>3.727963994704187</v>
       </c>
       <c r="AO75">
-        <v>3.499278473271989</v>
+        <v>3.727963994704187</v>
       </c>
       <c r="AP75">
-        <v>2.967877806534525</v>
+        <v>3.160279473278206</v>
       </c>
       <c r="AQ75">
-        <v>2.793893166305497</v>
+        <v>2.963227289589122</v>
       </c>
       <c r="AR75">
-        <v>2.793893166305497</v>
+        <v>2.963227289589122</v>
       </c>
       <c r="AS75">
-        <v>14.40585431333166</v>
+        <v>12.93711299578426</v>
       </c>
       <c r="AT75">
-        <v>100.455687204795</v>
+        <v>87.0773120675143</v>
       </c>
       <c r="AU75">
-        <v>100.455687204795</v>
+        <v>87.0773120675143</v>
       </c>
       <c r="AV75">
-        <v>100.455687204795</v>
+        <v>87.0773120675143</v>
       </c>
       <c r="AW75">
-        <v>2.471739122271538</v>
+        <v>2.609629156813026</v>
       </c>
       <c r="AX75">
-        <v>3.190947880822932</v>
+        <v>3.462290843739174</v>
       </c>
       <c r="AY75">
-        <v>0.3704864161368459</v>
+        <v>0.3762618554476648</v>
       </c>
       <c r="AZ75">
-        <v>79.33680799412728</v>
+        <v>83.39902650240064</v>
       </c>
       <c r="BA75">
-        <v>79.33680799412728</v>
+        <v>83.39902650240064</v>
       </c>
       <c r="BB75">
-        <v>79.33680799412728</v>
+        <v>83.39902650240064</v>
       </c>
       <c r="BC75">
-        <v>79.33680799412728</v>
+        <v>83.39902650240064</v>
       </c>
       <c r="BD75">
-        <v>79.33680799412728</v>
+        <v>83.39902650240064</v>
       </c>
       <c r="BE75">
-        <v>0.3704864161368459</v>
+        <v>0.3762618554476648</v>
       </c>
     </row>
     <row r="76" spans="1:57">
@@ -6016,73 +6016,73 @@
         <v>72</v>
       </c>
       <c r="AH76">
-        <v>14.58600710416213</v>
+        <v>13.85764443734661</v>
       </c>
       <c r="AI76">
-        <v>20.80613398961723</v>
+        <v>19.95056011611596</v>
       </c>
       <c r="AJ76">
-        <v>203.2207749169506</v>
+        <v>188.1883556936681</v>
       </c>
       <c r="AK76">
-        <v>20.80613398961723</v>
+        <v>19.95056011611596</v>
       </c>
       <c r="AL76">
-        <v>203.2207749169506</v>
+        <v>188.1883556936681</v>
       </c>
       <c r="AN76">
-        <v>15.73506095610559</v>
+        <v>15.05556329432875</v>
       </c>
       <c r="AO76">
-        <v>15.73506095610559</v>
+        <v>15.05556329432875</v>
       </c>
       <c r="AP76">
-        <v>25.33586614327505</v>
+        <v>24.46613073630258</v>
       </c>
       <c r="AQ76">
-        <v>4.656144000031054</v>
+        <v>4.449329024087637</v>
       </c>
       <c r="AR76">
-        <v>4.656144000031054</v>
+        <v>4.449329024087637</v>
       </c>
       <c r="AS76">
-        <v>629.8837321466208</v>
+        <v>597.0477011181414</v>
       </c>
       <c r="AT76">
-        <v>2327.148932623268</v>
+        <v>2071.345427659303</v>
       </c>
       <c r="AU76">
-        <v>2327.148932623268</v>
+        <v>2071.345427659303</v>
       </c>
       <c r="AV76">
-        <v>2327.148932623268</v>
+        <v>2071.345427659303</v>
       </c>
       <c r="AW76">
-        <v>40.31813014149666</v>
+        <v>38.93565626442432</v>
       </c>
       <c r="AX76">
-        <v>221.5278009824455</v>
+        <v>208.2552911628038</v>
       </c>
       <c r="AY76">
-        <v>11.62228437572718</v>
+        <v>11.39214546427131</v>
       </c>
       <c r="AZ76">
-        <v>658.5692046878339</v>
+        <v>646.3229965324402</v>
       </c>
       <c r="BA76">
-        <v>658.5692046878339</v>
+        <v>646.3229965324402</v>
       </c>
       <c r="BB76">
-        <v>658.5692046878339</v>
+        <v>646.3229965324402</v>
       </c>
       <c r="BC76">
-        <v>658.5692046878339</v>
+        <v>646.3229965324402</v>
       </c>
       <c r="BD76">
-        <v>658.5692046878339</v>
+        <v>646.3229965324402</v>
       </c>
       <c r="BE76">
-        <v>11.62228437572718</v>
+        <v>11.39214546427131</v>
       </c>
     </row>
     <row r="77" spans="1:57">
@@ -6090,73 +6090,73 @@
         <v>73</v>
       </c>
       <c r="AH77">
-        <v>22.16415098886937</v>
+        <v>24.5903088150546</v>
       </c>
       <c r="AI77">
-        <v>49.84443322978914</v>
+        <v>52.28643382675946</v>
       </c>
       <c r="AJ77">
-        <v>674.1897927421331</v>
+        <v>694.5457258093916</v>
       </c>
       <c r="AK77">
-        <v>49.84443322978914</v>
+        <v>52.28643382675946</v>
       </c>
       <c r="AL77">
-        <v>674.1897927421331</v>
+        <v>694.5457258093916</v>
       </c>
       <c r="AN77">
-        <v>58.49801138035953</v>
+        <v>59.48494589842856</v>
       </c>
       <c r="AO77">
-        <v>58.49801138035953</v>
+        <v>59.48494589842856</v>
       </c>
       <c r="AP77">
-        <v>90.24182404957712</v>
+        <v>92.52750127643347</v>
       </c>
       <c r="AQ77">
-        <v>24.82541301250458</v>
+        <v>25.27276641130447</v>
       </c>
       <c r="AR77">
-        <v>24.82541301250458</v>
+        <v>25.27276641130447</v>
       </c>
       <c r="AS77">
-        <v>1220.66968123287</v>
+        <v>1224.262318660319</v>
       </c>
       <c r="AT77">
-        <v>3909.166663952172</v>
+        <v>4145.115404068531</v>
       </c>
       <c r="AU77">
-        <v>3909.166663952172</v>
+        <v>4145.115404068531</v>
       </c>
       <c r="AV77">
-        <v>3909.166663952172</v>
+        <v>4145.115404068531</v>
       </c>
       <c r="AW77">
-        <v>51.75319621562958</v>
+        <v>53.81576367616653</v>
       </c>
       <c r="AX77">
-        <v>509.3750439479947</v>
+        <v>526.0701887235045</v>
       </c>
       <c r="AY77">
-        <v>25.97905255854129</v>
+        <v>26.64478800415992</v>
       </c>
       <c r="AZ77">
-        <v>1172.28277120328</v>
+        <v>1204.293787675143</v>
       </c>
       <c r="BA77">
-        <v>1172.28277120328</v>
+        <v>1204.293787675143</v>
       </c>
       <c r="BB77">
-        <v>1172.28277120328</v>
+        <v>1204.293787675143</v>
       </c>
       <c r="BC77">
-        <v>1172.28277120328</v>
+        <v>1204.293787675143</v>
       </c>
       <c r="BD77">
-        <v>1172.28277120328</v>
+        <v>1204.293787675143</v>
       </c>
       <c r="BE77">
-        <v>25.97905255854129</v>
+        <v>26.64478800415992</v>
       </c>
     </row>
     <row r="78" spans="1:57">
@@ -6164,73 +6164,73 @@
         <v>74</v>
       </c>
       <c r="AH78">
-        <v>0.4406759691750631</v>
+        <v>0.4497678949945839</v>
       </c>
       <c r="AI78">
-        <v>7.213819674542174</v>
+        <v>9.127329872967676</v>
       </c>
       <c r="AJ78">
-        <v>74.40975860358914</v>
+        <v>80.82700926961144</v>
       </c>
       <c r="AK78">
-        <v>7.213819674542174</v>
+        <v>9.127329872967676</v>
       </c>
       <c r="AL78">
-        <v>74.40975860358914</v>
+        <v>80.82700926961144</v>
       </c>
       <c r="AN78">
-        <v>5.620547629725189</v>
+        <v>5.766370668038726</v>
       </c>
       <c r="AO78">
-        <v>5.620547629725189</v>
+        <v>5.766370668038726</v>
       </c>
       <c r="AP78">
-        <v>11.42237053900957</v>
+        <v>12.42110090942122</v>
       </c>
       <c r="AQ78">
-        <v>6.340353480260819</v>
+        <v>6.67573219994083</v>
       </c>
       <c r="AR78">
-        <v>6.340353480260819</v>
+        <v>6.67573219994083</v>
       </c>
       <c r="AS78">
-        <v>47.1778669777466</v>
+        <v>42.51490652150475</v>
       </c>
       <c r="AT78">
-        <v>121.1692079006415</v>
+        <v>151.1782363720797</v>
       </c>
       <c r="AU78">
-        <v>121.1692079006415</v>
+        <v>151.1782363720797</v>
       </c>
       <c r="AV78">
-        <v>121.1692079006415</v>
+        <v>151.1782363720797</v>
       </c>
       <c r="AW78">
-        <v>9.171287022531033</v>
+        <v>9.796898133307696</v>
       </c>
       <c r="AX78">
-        <v>30.8258233175613</v>
+        <v>31.67221261365339</v>
       </c>
       <c r="AY78">
-        <v>2.15244241643697</v>
+        <v>2.20512321665883</v>
       </c>
       <c r="AZ78">
-        <v>94.26668654054404</v>
+        <v>100.3765526088476</v>
       </c>
       <c r="BA78">
-        <v>94.26668654054404</v>
+        <v>100.3765526088476</v>
       </c>
       <c r="BB78">
-        <v>94.26668654054404</v>
+        <v>100.3765526088476</v>
       </c>
       <c r="BC78">
-        <v>94.26668654054404</v>
+        <v>100.3765526088476</v>
       </c>
       <c r="BD78">
-        <v>94.26668654054404</v>
+        <v>100.3765526088476</v>
       </c>
       <c r="BE78">
-        <v>2.15244241643697</v>
+        <v>2.20512321665883</v>
       </c>
     </row>
     <row r="79" spans="1:57">
@@ -6238,73 +6238,73 @@
         <v>75</v>
       </c>
       <c r="AH79">
-        <v>10.65145417792723</v>
+        <v>11.2832838165015</v>
       </c>
       <c r="AI79">
-        <v>4.660319383302704</v>
+        <v>4.088546174857766</v>
       </c>
       <c r="AJ79">
-        <v>39.81580099688144</v>
+        <v>37.01303481577663</v>
       </c>
       <c r="AK79">
-        <v>4.660319383302704</v>
+        <v>4.088546174857766</v>
       </c>
       <c r="AL79">
-        <v>39.81580099688144</v>
+        <v>37.01303481577663</v>
       </c>
       <c r="AN79">
-        <v>2.638983073509298</v>
+        <v>2.479228200144135</v>
       </c>
       <c r="AO79">
-        <v>2.638983073509298</v>
+        <v>2.479228200144135</v>
       </c>
       <c r="AP79">
-        <v>2.937615607588086</v>
+        <v>2.493765170674306</v>
       </c>
       <c r="AQ79">
-        <v>1.239205213543028</v>
+        <v>1.196790882037021</v>
       </c>
       <c r="AR79">
-        <v>1.239205213543028</v>
+        <v>1.196790882037021</v>
       </c>
       <c r="AS79">
-        <v>64.8387075754907</v>
+        <v>57.29072296076454</v>
       </c>
       <c r="AT79">
-        <v>415.808921625279</v>
+        <v>382.648740320392</v>
       </c>
       <c r="AU79">
-        <v>415.808921625279</v>
+        <v>382.648740320392</v>
       </c>
       <c r="AV79">
-        <v>415.808921625279</v>
+        <v>382.648740320392</v>
       </c>
       <c r="AW79">
-        <v>7.183363182842732</v>
+        <v>6.730584502965212</v>
       </c>
       <c r="AX79">
-        <v>100.2953584484756</v>
+        <v>95.32857898697256</v>
       </c>
       <c r="AY79">
-        <v>4.522884311899542</v>
+        <v>4.416727090328932</v>
       </c>
       <c r="AZ79">
-        <v>203.228815502882</v>
+        <v>201.1721370059848</v>
       </c>
       <c r="BA79">
-        <v>203.228815502882</v>
+        <v>201.1721370059848</v>
       </c>
       <c r="BB79">
-        <v>203.228815502882</v>
+        <v>201.1721370059848</v>
       </c>
       <c r="BC79">
-        <v>203.228815502882</v>
+        <v>201.1721370059848</v>
       </c>
       <c r="BD79">
-        <v>203.228815502882</v>
+        <v>201.1721370059848</v>
       </c>
       <c r="BE79">
-        <v>4.522884311899542</v>
+        <v>4.416727090328932</v>
       </c>
     </row>
     <row r="80" spans="1:57">
@@ -6312,73 +6312,73 @@
         <v>76</v>
       </c>
       <c r="AH80">
-        <v>13.45798746185377</v>
+        <v>12.11434977805242</v>
       </c>
       <c r="AI80">
-        <v>14.08343166541308</v>
+        <v>13.48438005382195</v>
       </c>
       <c r="AJ80">
-        <v>243.6396059985738</v>
+        <v>238.3949724503886</v>
       </c>
       <c r="AK80">
-        <v>14.08343166541308</v>
+        <v>13.48438005382195</v>
       </c>
       <c r="AL80">
-        <v>243.6396059985738</v>
+        <v>238.3949724503886</v>
       </c>
       <c r="AN80">
-        <v>21.23328398842365</v>
+        <v>21.09457629527897</v>
       </c>
       <c r="AO80">
-        <v>21.23328398842365</v>
+        <v>21.09457629527897</v>
       </c>
       <c r="AP80">
-        <v>29.97947199227288</v>
+        <v>29.99180235628039</v>
       </c>
       <c r="AQ80">
-        <v>10.14648030120879</v>
+        <v>10.00633736718446</v>
       </c>
       <c r="AR80">
-        <v>10.14648030120879</v>
+        <v>10.00633736718446</v>
       </c>
       <c r="AS80">
-        <v>456.9800567036122</v>
+        <v>453.513553744331</v>
       </c>
       <c r="AT80">
-        <v>2217.601935847849</v>
+        <v>2402.161853535325</v>
       </c>
       <c r="AU80">
-        <v>2217.601935847849</v>
+        <v>2402.161853535325</v>
       </c>
       <c r="AV80">
-        <v>2217.601935847849</v>
+        <v>2402.161853535325</v>
       </c>
       <c r="AW80">
-        <v>20.47749817073345</v>
+        <v>20.51861240714788</v>
       </c>
       <c r="AX80">
-        <v>158.8606877215207</v>
+        <v>153.9303804054856</v>
       </c>
       <c r="AY80">
-        <v>7.524771695435047</v>
+        <v>7.195476815402507</v>
       </c>
       <c r="AZ80">
-        <v>471.0361390480996</v>
+        <v>440.5391899815799</v>
       </c>
       <c r="BA80">
-        <v>471.0361390480996</v>
+        <v>440.5391899815799</v>
       </c>
       <c r="BB80">
-        <v>471.0361390480996</v>
+        <v>440.5391899815799</v>
       </c>
       <c r="BC80">
-        <v>471.0361390480996</v>
+        <v>440.5391899815799</v>
       </c>
       <c r="BD80">
-        <v>471.0361390480996</v>
+        <v>440.5391899815799</v>
       </c>
       <c r="BE80">
-        <v>7.524771695435047</v>
+        <v>7.195476815402507</v>
       </c>
     </row>
     <row r="81" spans="1:81">
@@ -6386,73 +6386,73 @@
         <v>77</v>
       </c>
       <c r="AH81">
-        <v>3.037352387174033</v>
+        <v>2.714177616508678</v>
       </c>
       <c r="AI81">
-        <v>2.217408262763638</v>
+        <v>2.50873473623069</v>
       </c>
       <c r="AJ81">
-        <v>52.46461887568468</v>
+        <v>50.32512200158322</v>
       </c>
       <c r="AK81">
-        <v>2.217408262763638</v>
+        <v>2.50873473623069</v>
       </c>
       <c r="AL81">
-        <v>52.46461887568468</v>
+        <v>50.32512200158322</v>
       </c>
       <c r="AN81">
-        <v>2.566478029908613</v>
+        <v>2.694804817461409</v>
       </c>
       <c r="AO81">
-        <v>2.566478029908613</v>
+        <v>2.694804817461409</v>
       </c>
       <c r="AP81">
-        <v>6.34865314183291</v>
+        <v>5.961855987883173</v>
       </c>
       <c r="AQ81">
-        <v>3.550646647298708</v>
+        <v>3.61652621650137</v>
       </c>
       <c r="AR81">
-        <v>3.550646647298708</v>
+        <v>3.61652621650137</v>
       </c>
       <c r="AS81">
-        <v>35.47821828959975</v>
+        <v>37.5595741965808</v>
       </c>
       <c r="AT81">
-        <v>304.7823744788766</v>
+        <v>301.6063246752508</v>
       </c>
       <c r="AU81">
-        <v>304.7823744788766</v>
+        <v>301.6063246752508</v>
       </c>
       <c r="AV81">
-        <v>304.7823744788766</v>
+        <v>301.6063246752508</v>
       </c>
       <c r="AW81">
-        <v>5.122214941680432</v>
+        <v>5.515517091006041</v>
       </c>
       <c r="AX81">
-        <v>35.88583554206416</v>
+        <v>37.27662544269115</v>
       </c>
       <c r="AY81">
-        <v>2.002981155142188</v>
+        <v>1.983568638414144</v>
       </c>
       <c r="AZ81">
-        <v>80.71584402132035</v>
+        <v>81.64394999697805</v>
       </c>
       <c r="BA81">
-        <v>80.71584402132035</v>
+        <v>81.64394999697805</v>
       </c>
       <c r="BB81">
-        <v>80.71584402132035</v>
+        <v>81.64394999697805</v>
       </c>
       <c r="BC81">
-        <v>80.71584402132035</v>
+        <v>81.64394999697805</v>
       </c>
       <c r="BD81">
-        <v>80.71584402132035</v>
+        <v>81.64394999697805</v>
       </c>
       <c r="BE81">
-        <v>2.002981155142188</v>
+        <v>1.983568638414144</v>
       </c>
     </row>
     <row r="82" spans="1:81">

</xml_diff>

<commit_message>
awaiting requested output format
</commit_message>
<xml_diff>
--- a/excel_files/output.xlsx
+++ b/excel_files/output.xlsx
@@ -4837,61 +4837,61 @@
         <v>56</v>
       </c>
       <c r="BK58">
-        <v>7078.174746093063</v>
+        <v>6990.049284296037</v>
       </c>
       <c r="BL58">
-        <v>1444.393869164158</v>
+        <v>1340.191604392026</v>
       </c>
       <c r="BM58">
-        <v>12838.60618591949</v>
+        <v>13331.23923523152</v>
       </c>
       <c r="BN58">
-        <v>25756.04642876922</v>
+        <v>25705.07287315651</v>
       </c>
       <c r="BO58">
-        <v>1995.628295730427</v>
+        <v>1949.597887802064</v>
       </c>
       <c r="BP58">
-        <v>5869.649075423349</v>
+        <v>6164.985557787995</v>
       </c>
       <c r="BQ58">
-        <v>15978.87289030425</v>
+        <v>16151.1897315123</v>
       </c>
       <c r="BR58">
-        <v>1723.667646666086</v>
+        <v>1470.757508594189</v>
       </c>
       <c r="BS58">
-        <v>1949.314980610249</v>
+        <v>2080.611127017555</v>
       </c>
       <c r="BT58">
-        <v>5630.730755461873</v>
+        <v>5397.408730016446</v>
       </c>
       <c r="BU58">
-        <v>764.6444049755133</v>
+        <v>779.0691758155526</v>
       </c>
       <c r="BV58">
-        <v>10806.28559654408</v>
+        <v>11718.02515430384</v>
       </c>
       <c r="BW58">
-        <v>22094.55055163287</v>
+        <v>21149.79115015452</v>
       </c>
       <c r="BX58">
-        <v>1261.475488687794</v>
+        <v>1125.352923839777</v>
       </c>
       <c r="BY58">
-        <v>2425.322495755267</v>
+        <v>2555.231727340843</v>
       </c>
       <c r="BZ58">
-        <v>10659.60169516933</v>
+        <v>10280.99735213215</v>
       </c>
       <c r="CA58">
-        <v>1524.323987165695</v>
+        <v>1529.402883787179</v>
       </c>
       <c r="CC58">
         <v>112199.01</v>
       </c>
       <c r="CF58">
-        <v>1231.931639694078</v>
+        <v>1314.246116743768</v>
       </c>
     </row>
     <row r="59" spans="1:84">
@@ -5128,73 +5128,73 @@
         <v>82</v>
       </c>
       <c r="AH64">
-        <v>10.32749597553164</v>
+        <v>9.414114025598392</v>
       </c>
       <c r="AI64">
-        <v>4.572988519864158</v>
+        <v>4.98343871824909</v>
       </c>
       <c r="AJ64">
-        <v>181.3535974402819</v>
+        <v>200.4209536320157</v>
       </c>
       <c r="AK64">
-        <v>4.572988519864158</v>
+        <v>4.98343871824909</v>
       </c>
       <c r="AL64">
-        <v>181.3535974402819</v>
+        <v>200.4209536320157</v>
       </c>
       <c r="AN64">
-        <v>3.242894353428856</v>
+        <v>3.583830243987031</v>
       </c>
       <c r="AO64">
-        <v>3.242894353428856</v>
+        <v>3.583830243987031</v>
       </c>
       <c r="AP64">
-        <v>10.59236898211762</v>
+        <v>11.83001546522602</v>
       </c>
       <c r="AQ64">
-        <v>0.8428759983042254</v>
+        <v>0.882314035994932</v>
       </c>
       <c r="AR64">
-        <v>0.8428759983042254</v>
+        <v>0.882314035994932</v>
       </c>
       <c r="AS64">
-        <v>67.1392593125347</v>
+        <v>73.19743904368953</v>
       </c>
       <c r="AT64">
-        <v>187.1088795390912</v>
+        <v>192.0036300258339</v>
       </c>
       <c r="AU64">
-        <v>187.1088795390912</v>
+        <v>192.0036300258339</v>
       </c>
       <c r="AV64">
-        <v>187.1088795390912</v>
+        <v>192.0036300258339</v>
       </c>
       <c r="AW64">
-        <v>7.32389857172966</v>
+        <v>8.166333993524313</v>
       </c>
       <c r="AX64">
-        <v>21.63126105456613</v>
+        <v>22.61657591545954</v>
       </c>
       <c r="AY64">
-        <v>0.576311818435788</v>
+        <v>0.6143333348818123</v>
       </c>
       <c r="AZ64">
-        <v>34.48267618393898</v>
+        <v>38.40820165850223</v>
       </c>
       <c r="BA64">
-        <v>34.48267618393898</v>
+        <v>38.40820165850223</v>
       </c>
       <c r="BB64">
-        <v>34.48267618393898</v>
+        <v>38.40820165850223</v>
       </c>
       <c r="BC64">
-        <v>34.48267618393898</v>
+        <v>38.40820165850223</v>
       </c>
       <c r="BD64">
-        <v>34.48267618393898</v>
+        <v>38.40820165850223</v>
       </c>
       <c r="BE64">
-        <v>0.576311818435788</v>
+        <v>0.6143333348818123</v>
       </c>
     </row>
     <row r="65" spans="1:57">
@@ -5202,73 +5202,73 @@
         <v>61</v>
       </c>
       <c r="AH65">
-        <v>55.62435575969518</v>
+        <v>59.33229717329145</v>
       </c>
       <c r="AI65">
-        <v>51.37581306248904</v>
+        <v>52.88727739527822</v>
       </c>
       <c r="AJ65">
-        <v>2374.258369275034</v>
+        <v>2386.627410095036</v>
       </c>
       <c r="AK65">
-        <v>51.37581306248904</v>
+        <v>52.88727739527822</v>
       </c>
       <c r="AL65">
-        <v>2374.258369275034</v>
+        <v>2386.627410095036</v>
       </c>
       <c r="AN65">
-        <v>17.37251496220007</v>
+        <v>16.82216917671263</v>
       </c>
       <c r="AO65">
-        <v>17.37251496220007</v>
+        <v>16.82216917671263</v>
       </c>
       <c r="AP65">
-        <v>76.32228273190559</v>
+        <v>75.89979358144105</v>
       </c>
       <c r="AQ65">
-        <v>10.02416591662914</v>
+        <v>9.907512448914348</v>
       </c>
       <c r="AR65">
-        <v>10.02416591662914</v>
+        <v>9.907512448914348</v>
       </c>
       <c r="AS65">
-        <v>189.7119347106106</v>
+        <v>168.617042367179</v>
       </c>
       <c r="AT65">
-        <v>383.2473745921999</v>
+        <v>337.3299611688592</v>
       </c>
       <c r="AU65">
-        <v>383.2473745921999</v>
+        <v>337.3299611688592</v>
       </c>
       <c r="AV65">
-        <v>383.2473745921999</v>
+        <v>337.3299611688592</v>
       </c>
       <c r="AW65">
-        <v>16.16081960052252</v>
+        <v>15.90577829927206</v>
       </c>
       <c r="AX65">
-        <v>159.3026870578528</v>
+        <v>164.5034938763827</v>
       </c>
       <c r="AY65">
-        <v>2.813445122912526</v>
+        <v>2.83422336127609</v>
       </c>
       <c r="AZ65">
-        <v>103.9243851554692</v>
+        <v>111.1287621074915</v>
       </c>
       <c r="BA65">
-        <v>103.9243851554692</v>
+        <v>111.1287621074915</v>
       </c>
       <c r="BB65">
-        <v>103.9243851554692</v>
+        <v>111.1287621074915</v>
       </c>
       <c r="BC65">
-        <v>103.9243851554692</v>
+        <v>111.1287621074915</v>
       </c>
       <c r="BD65">
-        <v>103.9243851554692</v>
+        <v>111.1287621074915</v>
       </c>
       <c r="BE65">
-        <v>2.813445122912526</v>
+        <v>2.83422336127609</v>
       </c>
     </row>
     <row r="66" spans="1:57">
@@ -5276,73 +5276,73 @@
         <v>62</v>
       </c>
       <c r="AH66">
-        <v>7.047710597058758</v>
+        <v>7.205654163155705</v>
       </c>
       <c r="AI66">
-        <v>3.990203469153494</v>
+        <v>4.216897656582296</v>
       </c>
       <c r="AJ66">
-        <v>458.6134734524042</v>
+        <v>424.28795445811</v>
       </c>
       <c r="AK66">
-        <v>3.990203469153494</v>
+        <v>4.216897656582296</v>
       </c>
       <c r="AL66">
-        <v>458.6134734524042</v>
+        <v>424.28795445811</v>
       </c>
       <c r="AN66">
-        <v>3.954541075909511</v>
+        <v>3.524966271901503</v>
       </c>
       <c r="AO66">
-        <v>3.954541075909511</v>
+        <v>3.524966271901503</v>
       </c>
       <c r="AP66">
-        <v>15.17512013768777</v>
+        <v>14.83037091043778</v>
       </c>
       <c r="AQ66">
-        <v>2.719587604282424</v>
+        <v>2.587943928549066</v>
       </c>
       <c r="AR66">
-        <v>2.719587604282424</v>
+        <v>2.587943928549066</v>
       </c>
       <c r="AS66">
-        <v>15.26135000328533</v>
+        <v>15.87995030975901</v>
       </c>
       <c r="AT66">
-        <v>104.1169870545808</v>
+        <v>95.40936142164284</v>
       </c>
       <c r="AU66">
-        <v>104.1169870545808</v>
+        <v>95.40936142164284</v>
       </c>
       <c r="AV66">
-        <v>104.1169870545808</v>
+        <v>95.40936142164284</v>
       </c>
       <c r="AW66">
-        <v>4.574907561019063</v>
+        <v>4.508362703770399</v>
       </c>
       <c r="AX66">
-        <v>22.23482795781456</v>
+        <v>20.73699029148556</v>
       </c>
       <c r="AY66">
-        <v>0.7343764872662722</v>
+        <v>0.6809700198937206</v>
       </c>
       <c r="AZ66">
-        <v>25.54492551310361</v>
+        <v>24.04094541568309</v>
       </c>
       <c r="BA66">
-        <v>25.54492551310361</v>
+        <v>24.04094541568309</v>
       </c>
       <c r="BB66">
-        <v>25.54492551310361</v>
+        <v>24.04094541568309</v>
       </c>
       <c r="BC66">
-        <v>25.54492551310361</v>
+        <v>24.04094541568309</v>
       </c>
       <c r="BD66">
-        <v>25.54492551310361</v>
+        <v>24.04094541568309</v>
       </c>
       <c r="BE66">
-        <v>0.7343764872662722</v>
+        <v>0.6809700198937206</v>
       </c>
     </row>
     <row r="67" spans="1:57">
@@ -5350,73 +5350,73 @@
         <v>63</v>
       </c>
       <c r="AH67">
-        <v>88.13898866191506</v>
+        <v>85.96996595606208</v>
       </c>
       <c r="AI67">
-        <v>46.80938113369048</v>
+        <v>45.81034803465009</v>
       </c>
       <c r="AJ67">
-        <v>1055.319351939931</v>
+        <v>1067.650717165209</v>
       </c>
       <c r="AK67">
-        <v>46.80938113369048</v>
+        <v>45.81034803465009</v>
       </c>
       <c r="AL67">
-        <v>1055.319351939931</v>
+        <v>1067.650717165209</v>
       </c>
       <c r="AN67">
-        <v>20.47571496848017</v>
+        <v>21.2452943026647</v>
       </c>
       <c r="AO67">
-        <v>20.47571496848017</v>
+        <v>21.2452943026647</v>
       </c>
       <c r="AP67">
-        <v>64.813621731475</v>
+        <v>67.45605026192963</v>
       </c>
       <c r="AQ67">
-        <v>3.584853507205844</v>
+        <v>3.648380930209532</v>
       </c>
       <c r="AR67">
-        <v>3.584853507205844</v>
+        <v>3.648380930209532</v>
       </c>
       <c r="AS67">
-        <v>983.8413402225077</v>
+        <v>1017.25321948424</v>
       </c>
       <c r="AT67">
-        <v>2134.991636324525</v>
+        <v>2296.914724432677</v>
       </c>
       <c r="AU67">
-        <v>2134.991636324525</v>
+        <v>2296.914724432677</v>
       </c>
       <c r="AV67">
-        <v>2134.991636324525</v>
+        <v>2296.914724432677</v>
       </c>
       <c r="AW67">
-        <v>56.55622662901879</v>
+        <v>57.67828812599182</v>
       </c>
       <c r="AX67">
-        <v>256.5261487729848</v>
+        <v>253.528219165653</v>
       </c>
       <c r="AY67">
-        <v>6.381567758470773</v>
+        <v>6.298046703189611</v>
       </c>
       <c r="AZ67">
-        <v>543.7226424624921</v>
+        <v>533.8607489335537</v>
       </c>
       <c r="BA67">
-        <v>543.7226424624921</v>
+        <v>533.8607489335537</v>
       </c>
       <c r="BB67">
-        <v>543.7226424624921</v>
+        <v>533.8607489335537</v>
       </c>
       <c r="BC67">
-        <v>543.7226424624921</v>
+        <v>533.8607489335537</v>
       </c>
       <c r="BD67">
-        <v>543.7226424624921</v>
+        <v>533.8607489335537</v>
       </c>
       <c r="BE67">
-        <v>6.381567758470773</v>
+        <v>6.298046703189611</v>
       </c>
     </row>
     <row r="68" spans="1:57">
@@ -5424,73 +5424,73 @@
         <v>64</v>
       </c>
       <c r="AH68">
-        <v>219.239612736702</v>
+        <v>210.7794315168262</v>
       </c>
       <c r="AI68">
-        <v>307.289012221992</v>
+        <v>300.8081789076329</v>
       </c>
       <c r="AJ68">
-        <v>4580.026900641024</v>
+        <v>4553.744405761063</v>
       </c>
       <c r="AK68">
-        <v>307.289012221992</v>
+        <v>300.8081789076329</v>
       </c>
       <c r="AL68">
-        <v>4580.026900641024</v>
+        <v>4553.744405761063</v>
       </c>
       <c r="AN68">
-        <v>71.96046021983028</v>
+        <v>71.71276636935771</v>
       </c>
       <c r="AO68">
-        <v>71.96046021983028</v>
+        <v>71.71276636935771</v>
       </c>
       <c r="AP68">
-        <v>427.6999570736289</v>
+        <v>425.0448387694359</v>
       </c>
       <c r="AQ68">
-        <v>24.70265532545745</v>
+        <v>24.91756613589823</v>
       </c>
       <c r="AR68">
-        <v>24.70265532545745</v>
+        <v>24.91756613589823</v>
       </c>
       <c r="AS68">
-        <v>1274.942523638755</v>
+        <v>1199.389830690175</v>
       </c>
       <c r="AT68">
-        <v>3465.241693329811</v>
+        <v>3500.822733426095</v>
       </c>
       <c r="AU68">
-        <v>3465.241693329811</v>
+        <v>3500.822733426095</v>
       </c>
       <c r="AV68">
-        <v>3465.241693329811</v>
+        <v>3500.822733426095</v>
       </c>
       <c r="AW68">
-        <v>55.81736481785774</v>
+        <v>55.08900470733643</v>
       </c>
       <c r="AX68">
-        <v>815.0322411715983</v>
+        <v>787.1122351065278</v>
       </c>
       <c r="AY68">
-        <v>7.278745202422141</v>
+        <v>7.304603953659534</v>
       </c>
       <c r="AZ68">
-        <v>517.0148204239607</v>
+        <v>521.6428579665424</v>
       </c>
       <c r="BA68">
-        <v>517.0148204239607</v>
+        <v>521.6428579665424</v>
       </c>
       <c r="BB68">
-        <v>517.0148204239607</v>
+        <v>521.6428579665424</v>
       </c>
       <c r="BC68">
-        <v>517.0148204239607</v>
+        <v>521.6428579665424</v>
       </c>
       <c r="BD68">
-        <v>517.0148204239607</v>
+        <v>521.6428579665424</v>
       </c>
       <c r="BE68">
-        <v>7.278745202422141</v>
+        <v>7.304603953659534</v>
       </c>
     </row>
     <row r="69" spans="1:57">
@@ -5498,73 +5498,73 @@
         <v>65</v>
       </c>
       <c r="AH69">
-        <v>18.53883464202285</v>
+        <v>17.85041145477444</v>
       </c>
       <c r="AI69">
-        <v>29.33736850079149</v>
+        <v>28.15027438197285</v>
       </c>
       <c r="AJ69">
-        <v>418.786363815777</v>
+        <v>377.6822184351739</v>
       </c>
       <c r="AK69">
-        <v>29.33736850079149</v>
+        <v>28.15027438197285</v>
       </c>
       <c r="AL69">
-        <v>418.786363815777</v>
+        <v>377.6822184351739</v>
       </c>
       <c r="AN69">
-        <v>4.858426191443577</v>
+        <v>4.714462637193501</v>
       </c>
       <c r="AO69">
-        <v>4.858426191443577</v>
+        <v>4.714462637193501</v>
       </c>
       <c r="AP69">
-        <v>50.61843925260008</v>
+        <v>49.16584968741984</v>
       </c>
       <c r="AQ69">
-        <v>2.979895184142515</v>
+        <v>2.893772782757878</v>
       </c>
       <c r="AR69">
-        <v>2.979895184142515</v>
+        <v>2.893772782757878</v>
       </c>
       <c r="AS69">
-        <v>36.33592108886689</v>
+        <v>33.3963167022774</v>
       </c>
       <c r="AT69">
-        <v>240.4236348219589</v>
+        <v>255.6969061620534</v>
       </c>
       <c r="AU69">
-        <v>240.4236348219589</v>
+        <v>255.6969061620534</v>
       </c>
       <c r="AV69">
-        <v>240.4236348219589</v>
+        <v>255.6969061620534</v>
       </c>
       <c r="AW69">
-        <v>5.169273956120015</v>
+        <v>5.374387093633413</v>
       </c>
       <c r="AX69">
-        <v>27.46067404816858</v>
+        <v>25.69650055831298</v>
       </c>
       <c r="AY69">
-        <v>0.2682642942527309</v>
+        <v>0.2742241334868595</v>
       </c>
       <c r="AZ69">
-        <v>44.75472246079148</v>
+        <v>44.71875981566311</v>
       </c>
       <c r="BA69">
-        <v>44.75472246079148</v>
+        <v>44.71875981566311</v>
       </c>
       <c r="BB69">
-        <v>44.75472246079148</v>
+        <v>44.71875981566311</v>
       </c>
       <c r="BC69">
-        <v>44.75472246079148</v>
+        <v>44.71875981566311</v>
       </c>
       <c r="BD69">
-        <v>44.75472246079148</v>
+        <v>44.71875981566311</v>
       </c>
       <c r="BE69">
-        <v>0.2682642942527309</v>
+        <v>0.2742241334868595</v>
       </c>
     </row>
     <row r="70" spans="1:57">
@@ -5572,73 +5572,73 @@
         <v>66</v>
       </c>
       <c r="AH70">
-        <v>19.97223727237433</v>
+        <v>22.72248552095145</v>
       </c>
       <c r="AI70">
-        <v>25.96263036634773</v>
+        <v>26.40249624270946</v>
       </c>
       <c r="AJ70">
-        <v>526.1549890216626</v>
+        <v>551.2811292873323</v>
       </c>
       <c r="AK70">
-        <v>25.96263036634773</v>
+        <v>26.40249624270946</v>
       </c>
       <c r="AL70">
-        <v>526.1549890216626</v>
+        <v>551.2811292873323</v>
       </c>
       <c r="AN70">
-        <v>4.432074601035565</v>
+        <v>4.544429623456672</v>
       </c>
       <c r="AO70">
-        <v>4.432074601035565</v>
+        <v>4.544429623456672</v>
       </c>
       <c r="AP70">
-        <v>14.37950947392732</v>
+        <v>15.6135156785883</v>
       </c>
       <c r="AQ70">
-        <v>1.066733890632168</v>
+        <v>1.124677603738382</v>
       </c>
       <c r="AR70">
-        <v>1.066733890632168</v>
+        <v>1.124677603738382</v>
       </c>
       <c r="AS70">
-        <v>208.6571391646564</v>
+        <v>224.3877803584561</v>
       </c>
       <c r="AT70">
-        <v>1132.170541267768</v>
+        <v>1211.574020833299</v>
       </c>
       <c r="AU70">
-        <v>1132.170541267768</v>
+        <v>1211.574020833299</v>
       </c>
       <c r="AV70">
-        <v>1132.170541267768</v>
+        <v>1211.574020833299</v>
       </c>
       <c r="AW70">
-        <v>13.81265972405672</v>
+        <v>13.75366018712521</v>
       </c>
       <c r="AX70">
-        <v>150.4025145620108</v>
+        <v>151.1198314923793</v>
       </c>
       <c r="AY70">
-        <v>5.01814355880022</v>
+        <v>4.972760506421327</v>
       </c>
       <c r="AZ70">
-        <v>188.1288497092128</v>
+        <v>185.2030471046567</v>
       </c>
       <c r="BA70">
-        <v>188.1288497092128</v>
+        <v>185.2030471046567</v>
       </c>
       <c r="BB70">
-        <v>188.1288497092128</v>
+        <v>185.2030471046567</v>
       </c>
       <c r="BC70">
-        <v>188.1288497092128</v>
+        <v>185.2030471046567</v>
       </c>
       <c r="BD70">
-        <v>188.1288497092128</v>
+        <v>185.2030471046567</v>
       </c>
       <c r="BE70">
-        <v>5.01814355880022</v>
+        <v>4.972760506421327</v>
       </c>
     </row>
     <row r="71" spans="1:57">
@@ -5646,73 +5646,73 @@
         <v>67</v>
       </c>
       <c r="AH71">
-        <v>82.58001702383162</v>
+        <v>86.79474751248956</v>
       </c>
       <c r="AI71">
-        <v>127.9566214829683</v>
+        <v>139.8593661420047</v>
       </c>
       <c r="AJ71">
-        <v>1489.914490683451</v>
+        <v>1530.035279196426</v>
       </c>
       <c r="AK71">
-        <v>127.9566214829683</v>
+        <v>139.8593661420047</v>
       </c>
       <c r="AL71">
-        <v>1489.914490683451</v>
+        <v>1530.035279196426</v>
       </c>
       <c r="AN71">
-        <v>27.35663459844887</v>
+        <v>27.99167295109481</v>
       </c>
       <c r="AO71">
-        <v>27.35663459844887</v>
+        <v>27.99167295109481</v>
       </c>
       <c r="AP71">
-        <v>182.8487649159133</v>
+        <v>188.5514367929101</v>
       </c>
       <c r="AQ71">
-        <v>9.322926331870258</v>
+        <v>9.954080538451672</v>
       </c>
       <c r="AR71">
-        <v>9.322926331870258</v>
+        <v>9.954080538451672</v>
       </c>
       <c r="AS71">
-        <v>908.189632204175</v>
+        <v>898.22598473683</v>
       </c>
       <c r="AT71">
-        <v>3165.645268564821</v>
+        <v>3174.076085808873</v>
       </c>
       <c r="AU71">
-        <v>3165.645268564821</v>
+        <v>3174.076085808873</v>
       </c>
       <c r="AV71">
-        <v>3165.645268564821</v>
+        <v>3174.076085808873</v>
       </c>
       <c r="AW71">
-        <v>25.104587200284</v>
+        <v>25.92668635845184</v>
       </c>
       <c r="AX71">
-        <v>860.8514303967356</v>
+        <v>885.2735020026564</v>
       </c>
       <c r="AY71">
-        <v>4.486814143210649</v>
+        <v>4.723041579052805</v>
       </c>
       <c r="AZ71">
-        <v>220.8575356777907</v>
+        <v>223.8124471736551</v>
       </c>
       <c r="BA71">
-        <v>220.8575356777907</v>
+        <v>223.8124471736551</v>
       </c>
       <c r="BB71">
-        <v>220.8575356777907</v>
+        <v>223.8124471736551</v>
       </c>
       <c r="BC71">
-        <v>220.8575356777907</v>
+        <v>223.8124471736551</v>
       </c>
       <c r="BD71">
-        <v>220.8575356777907</v>
+        <v>223.8124471736551</v>
       </c>
       <c r="BE71">
-        <v>4.486814143210649</v>
+        <v>4.723041579052805</v>
       </c>
     </row>
     <row r="72" spans="1:57">
@@ -5720,73 +5720,73 @@
         <v>68</v>
       </c>
       <c r="AH72">
-        <v>12.12657052198425</v>
+        <v>13.98811280122027</v>
       </c>
       <c r="AI72">
-        <v>16.9015228160657</v>
+        <v>15.2970779588446</v>
       </c>
       <c r="AJ72">
-        <v>159.946241059103</v>
+        <v>153.0186887697224</v>
       </c>
       <c r="AK72">
-        <v>16.9015228160657</v>
+        <v>15.2970779588446</v>
       </c>
       <c r="AL72">
-        <v>159.946241059103</v>
+        <v>153.0186887697224</v>
       </c>
       <c r="AN72">
-        <v>3.432808256540448</v>
+        <v>3.391067505558021</v>
       </c>
       <c r="AO72">
-        <v>3.432808256540448</v>
+        <v>3.391067505558021</v>
       </c>
       <c r="AP72">
-        <v>38.0822760284692</v>
+        <v>36.30120203226805</v>
       </c>
       <c r="AQ72">
-        <v>1.902591010485776</v>
+        <v>1.918124681361951</v>
       </c>
       <c r="AR72">
-        <v>1.902591010485776</v>
+        <v>1.918124681361951</v>
       </c>
       <c r="AS72">
-        <v>94.14558300572448</v>
+        <v>89.16462504421361</v>
       </c>
       <c r="AT72">
-        <v>284.2840808640421</v>
+        <v>210.5832067055814</v>
       </c>
       <c r="AU72">
-        <v>284.2840808640421</v>
+        <v>210.5832067055814</v>
       </c>
       <c r="AV72">
-        <v>284.2840808640421</v>
+        <v>210.5832067055814</v>
       </c>
       <c r="AW72">
-        <v>5.659491407871246</v>
+        <v>5.622723040729761</v>
       </c>
       <c r="AX72">
-        <v>37.07372726369649</v>
+        <v>36.43868462974206</v>
       </c>
       <c r="AY72">
-        <v>0.2551628283038735</v>
+        <v>0.2696506427740678</v>
       </c>
       <c r="AZ72">
-        <v>63.77022078104318</v>
+        <v>61.94066436254979</v>
       </c>
       <c r="BA72">
-        <v>63.77022078104318</v>
+        <v>61.94066436254979</v>
       </c>
       <c r="BB72">
-        <v>63.77022078104318</v>
+        <v>61.94066436254979</v>
       </c>
       <c r="BC72">
-        <v>63.77022078104318</v>
+        <v>61.94066436254979</v>
       </c>
       <c r="BD72">
-        <v>63.77022078104318</v>
+        <v>61.94066436254979</v>
       </c>
       <c r="BE72">
-        <v>0.2551628283038735</v>
+        <v>0.2696506427740678</v>
       </c>
     </row>
     <row r="73" spans="1:57">
@@ -5794,73 +5794,73 @@
         <v>69</v>
       </c>
       <c r="AH73">
-        <v>20.19569584663957</v>
+        <v>20.77479004822672</v>
       </c>
       <c r="AI73">
-        <v>4.658376157283783</v>
+        <v>4.852747014700435</v>
       </c>
       <c r="AJ73">
-        <v>45.04365638662479</v>
+        <v>48.24235908871516</v>
       </c>
       <c r="AK73">
-        <v>4.658376157283783</v>
+        <v>4.852747014700435</v>
       </c>
       <c r="AL73">
-        <v>45.04365638662479</v>
+        <v>48.24235908871516</v>
       </c>
       <c r="AN73">
-        <v>3.658679197728634</v>
+        <v>4.100118934209458</v>
       </c>
       <c r="AO73">
-        <v>3.658679197728634</v>
+        <v>4.100118934209458</v>
       </c>
       <c r="AP73">
-        <v>5.007552876747213</v>
+        <v>5.887614787886851</v>
       </c>
       <c r="AQ73">
-        <v>1.805033399374224</v>
+        <v>1.975540813524276</v>
       </c>
       <c r="AR73">
-        <v>1.805033399374224</v>
+        <v>1.975540813524276</v>
       </c>
       <c r="AS73">
-        <v>86.93084141239524</v>
+        <v>94.09361228807829</v>
       </c>
       <c r="AT73">
-        <v>404.7909514588491</v>
+        <v>432.1870895471797</v>
       </c>
       <c r="AU73">
-        <v>404.7909514588491</v>
+        <v>432.1870895471797</v>
       </c>
       <c r="AV73">
-        <v>404.7909514588491</v>
+        <v>432.1870895471797</v>
       </c>
       <c r="AW73">
-        <v>6.744798259437085</v>
+        <v>7.274246802926064</v>
       </c>
       <c r="AX73">
-        <v>43.96498101418837</v>
+        <v>48.43849489577114</v>
       </c>
       <c r="AY73">
-        <v>2.483003831617534</v>
+        <v>2.568719942420721</v>
       </c>
       <c r="AZ73">
-        <v>91.36015177580715</v>
+        <v>96.82042559319736</v>
       </c>
       <c r="BA73">
-        <v>91.36015177580715</v>
+        <v>96.82042559319736</v>
       </c>
       <c r="BB73">
-        <v>91.36015177580715</v>
+        <v>96.82042559319736</v>
       </c>
       <c r="BC73">
-        <v>91.36015177580715</v>
+        <v>96.82042559319736</v>
       </c>
       <c r="BD73">
-        <v>91.36015177580715</v>
+        <v>96.82042559319736</v>
       </c>
       <c r="BE73">
-        <v>2.483003831617534</v>
+        <v>2.568719942420721</v>
       </c>
     </row>
     <row r="74" spans="1:57">
@@ -5868,73 +5868,73 @@
         <v>70</v>
       </c>
       <c r="AH74">
-        <v>7.307339250911028</v>
+        <v>6.972353674806655</v>
       </c>
       <c r="AI74">
-        <v>13.69840459926054</v>
+        <v>12.21744870962575</v>
       </c>
       <c r="AJ74">
-        <v>199.3395090688811</v>
+        <v>199.71937682949</v>
       </c>
       <c r="AK74">
-        <v>13.69840459926054</v>
+        <v>12.21744870962575</v>
       </c>
       <c r="AL74">
-        <v>199.3395090688811</v>
+        <v>199.71937682949</v>
       </c>
       <c r="AN74">
-        <v>18.56679355151951</v>
+        <v>18.19257926173508</v>
       </c>
       <c r="AO74">
-        <v>18.56679355151951</v>
+        <v>18.19257926173508</v>
       </c>
       <c r="AP74">
-        <v>21.40766636753455</v>
+        <v>18.15562672873959</v>
       </c>
       <c r="AQ74">
-        <v>11.34297313652933</v>
+        <v>11.11295016352087</v>
       </c>
       <c r="AR74">
-        <v>11.34297313652933</v>
+        <v>11.11295016352087</v>
       </c>
       <c r="AS74">
-        <v>256.3085316904262</v>
+        <v>263.5501914815977</v>
       </c>
       <c r="AT74">
-        <v>968.3056329841913</v>
+        <v>908.7285465851427</v>
       </c>
       <c r="AU74">
-        <v>968.3056329841913</v>
+        <v>908.7285465851427</v>
       </c>
       <c r="AV74">
-        <v>968.3056329841913</v>
+        <v>908.7285465851427</v>
       </c>
       <c r="AW74">
-        <v>15.95331169366837</v>
+        <v>15.00309596955776</v>
       </c>
       <c r="AX74">
-        <v>162.2239578679204</v>
+        <v>157.2740013517439</v>
       </c>
       <c r="AY74">
-        <v>10.75007495641708</v>
+        <v>10.54452222824097</v>
       </c>
       <c r="AZ74">
-        <v>351.0435078027249</v>
+        <v>341.338813333869</v>
       </c>
       <c r="BA74">
-        <v>351.0435078027249</v>
+        <v>341.338813333869</v>
       </c>
       <c r="BB74">
-        <v>351.0435078027249</v>
+        <v>341.338813333869</v>
       </c>
       <c r="BC74">
-        <v>351.0435078027249</v>
+        <v>341.338813333869</v>
       </c>
       <c r="BD74">
-        <v>351.0435078027249</v>
+        <v>341.338813333869</v>
       </c>
       <c r="BE74">
-        <v>10.75007495641708</v>
+        <v>10.54452222824097</v>
       </c>
     </row>
     <row r="75" spans="1:57">
@@ -5942,73 +5942,73 @@
         <v>71</v>
       </c>
       <c r="AH75">
-        <v>0.601618711395422</v>
+        <v>0.5680094407271827</v>
       </c>
       <c r="AI75">
-        <v>0.9516931460180786</v>
+        <v>0.6389008355734405</v>
       </c>
       <c r="AJ75">
-        <v>23.80405625421961</v>
+        <v>21.40426394213398</v>
       </c>
       <c r="AK75">
-        <v>0.9516931460180786</v>
+        <v>0.6389008355734405</v>
       </c>
       <c r="AL75">
-        <v>23.80405625421961</v>
+        <v>21.40426394213398</v>
       </c>
       <c r="AN75">
-        <v>3.727963994704187</v>
+        <v>3.499278473271989</v>
       </c>
       <c r="AO75">
-        <v>3.727963994704187</v>
+        <v>3.499278473271989</v>
       </c>
       <c r="AP75">
-        <v>3.160279473278206</v>
+        <v>2.967877806534525</v>
       </c>
       <c r="AQ75">
-        <v>2.963227289589122</v>
+        <v>2.793893166305497</v>
       </c>
       <c r="AR75">
-        <v>2.963227289589122</v>
+        <v>2.793893166305497</v>
       </c>
       <c r="AS75">
-        <v>12.93711299578426</v>
+        <v>14.40585431333166</v>
       </c>
       <c r="AT75">
-        <v>87.0773120675143</v>
+        <v>100.455687204795</v>
       </c>
       <c r="AU75">
-        <v>87.0773120675143</v>
+        <v>100.455687204795</v>
       </c>
       <c r="AV75">
-        <v>87.0773120675143</v>
+        <v>100.455687204795</v>
       </c>
       <c r="AW75">
-        <v>2.609629156813026</v>
+        <v>2.471739122271538</v>
       </c>
       <c r="AX75">
-        <v>3.462290843739174</v>
+        <v>3.190947880822932</v>
       </c>
       <c r="AY75">
-        <v>0.3762618554476648</v>
+        <v>0.3704864161368459</v>
       </c>
       <c r="AZ75">
-        <v>83.39902650240064</v>
+        <v>79.33680799412728</v>
       </c>
       <c r="BA75">
-        <v>83.39902650240064</v>
+        <v>79.33680799412728</v>
       </c>
       <c r="BB75">
-        <v>83.39902650240064</v>
+        <v>79.33680799412728</v>
       </c>
       <c r="BC75">
-        <v>83.39902650240064</v>
+        <v>79.33680799412728</v>
       </c>
       <c r="BD75">
-        <v>83.39902650240064</v>
+        <v>79.33680799412728</v>
       </c>
       <c r="BE75">
-        <v>0.3762618554476648</v>
+        <v>0.3704864161368459</v>
       </c>
     </row>
     <row r="76" spans="1:57">
@@ -6016,73 +6016,73 @@
         <v>72</v>
       </c>
       <c r="AH76">
-        <v>13.85764443734661</v>
+        <v>14.58600710416213</v>
       </c>
       <c r="AI76">
-        <v>19.95056011611596</v>
+        <v>20.80613398961723</v>
       </c>
       <c r="AJ76">
-        <v>188.1883556936681</v>
+        <v>203.2207749169506</v>
       </c>
       <c r="AK76">
-        <v>19.95056011611596</v>
+        <v>20.80613398961723</v>
       </c>
       <c r="AL76">
-        <v>188.1883556936681</v>
+        <v>203.2207749169506</v>
       </c>
       <c r="AN76">
-        <v>15.05556329432875</v>
+        <v>15.73506095610559</v>
       </c>
       <c r="AO76">
-        <v>15.05556329432875</v>
+        <v>15.73506095610559</v>
       </c>
       <c r="AP76">
-        <v>24.46613073630258</v>
+        <v>25.33586614327505</v>
       </c>
       <c r="AQ76">
-        <v>4.449329024087637</v>
+        <v>4.656144000031054</v>
       </c>
       <c r="AR76">
-        <v>4.449329024087637</v>
+        <v>4.656144000031054</v>
       </c>
       <c r="AS76">
-        <v>597.0477011181414</v>
+        <v>629.8837321466208</v>
       </c>
       <c r="AT76">
-        <v>2071.345427659303</v>
+        <v>2327.148932623268</v>
       </c>
       <c r="AU76">
-        <v>2071.345427659303</v>
+        <v>2327.148932623268</v>
       </c>
       <c r="AV76">
-        <v>2071.345427659303</v>
+        <v>2327.148932623268</v>
       </c>
       <c r="AW76">
-        <v>38.93565626442432</v>
+        <v>40.31813014149666</v>
       </c>
       <c r="AX76">
-        <v>208.2552911628038</v>
+        <v>221.5278009824455</v>
       </c>
       <c r="AY76">
-        <v>11.39214546427131</v>
+        <v>11.62228437572718</v>
       </c>
       <c r="AZ76">
-        <v>646.3229965324402</v>
+        <v>658.5692046878339</v>
       </c>
       <c r="BA76">
-        <v>646.3229965324402</v>
+        <v>658.5692046878339</v>
       </c>
       <c r="BB76">
-        <v>646.3229965324402</v>
+        <v>658.5692046878339</v>
       </c>
       <c r="BC76">
-        <v>646.3229965324402</v>
+        <v>658.5692046878339</v>
       </c>
       <c r="BD76">
-        <v>646.3229965324402</v>
+        <v>658.5692046878339</v>
       </c>
       <c r="BE76">
-        <v>11.39214546427131</v>
+        <v>11.62228437572718</v>
       </c>
     </row>
     <row r="77" spans="1:57">
@@ -6090,73 +6090,73 @@
         <v>73</v>
       </c>
       <c r="AH77">
-        <v>24.5903088150546</v>
+        <v>22.16415098886937</v>
       </c>
       <c r="AI77">
-        <v>52.28643382675946</v>
+        <v>49.84443322978914</v>
       </c>
       <c r="AJ77">
-        <v>694.5457258093916</v>
+        <v>674.1897927421331</v>
       </c>
       <c r="AK77">
-        <v>52.28643382675946</v>
+        <v>49.84443322978914</v>
       </c>
       <c r="AL77">
-        <v>694.5457258093916</v>
+        <v>674.1897927421331</v>
       </c>
       <c r="AN77">
-        <v>59.48494589842856</v>
+        <v>58.49801138035953</v>
       </c>
       <c r="AO77">
-        <v>59.48494589842856</v>
+        <v>58.49801138035953</v>
       </c>
       <c r="AP77">
-        <v>92.52750127643347</v>
+        <v>90.24182404957712</v>
       </c>
       <c r="AQ77">
-        <v>25.27276641130447</v>
+        <v>24.82541301250458</v>
       </c>
       <c r="AR77">
-        <v>25.27276641130447</v>
+        <v>24.82541301250458</v>
       </c>
       <c r="AS77">
-        <v>1224.262318660319</v>
+        <v>1220.66968123287</v>
       </c>
       <c r="AT77">
-        <v>4145.115404068531</v>
+        <v>3909.166663952172</v>
       </c>
       <c r="AU77">
-        <v>4145.115404068531</v>
+        <v>3909.166663952172</v>
       </c>
       <c r="AV77">
-        <v>4145.115404068531</v>
+        <v>3909.166663952172</v>
       </c>
       <c r="AW77">
-        <v>53.81576367616653</v>
+        <v>51.75319621562958</v>
       </c>
       <c r="AX77">
-        <v>526.0701887235045</v>
+        <v>509.3750439479947</v>
       </c>
       <c r="AY77">
-        <v>26.64478800415992</v>
+        <v>25.97905255854129</v>
       </c>
       <c r="AZ77">
-        <v>1204.293787675143</v>
+        <v>1172.28277120328</v>
       </c>
       <c r="BA77">
-        <v>1204.293787675143</v>
+        <v>1172.28277120328</v>
       </c>
       <c r="BB77">
-        <v>1204.293787675143</v>
+        <v>1172.28277120328</v>
       </c>
       <c r="BC77">
-        <v>1204.293787675143</v>
+        <v>1172.28277120328</v>
       </c>
       <c r="BD77">
-        <v>1204.293787675143</v>
+        <v>1172.28277120328</v>
       </c>
       <c r="BE77">
-        <v>26.64478800415992</v>
+        <v>25.97905255854129</v>
       </c>
     </row>
     <row r="78" spans="1:57">
@@ -6164,73 +6164,73 @@
         <v>74</v>
       </c>
       <c r="AH78">
-        <v>0.4497678949945839</v>
+        <v>0.4406759691750631</v>
       </c>
       <c r="AI78">
-        <v>9.127329872967676</v>
+        <v>7.213819674542174</v>
       </c>
       <c r="AJ78">
-        <v>80.82700926961144</v>
+        <v>74.40975860358914</v>
       </c>
       <c r="AK78">
-        <v>9.127329872967676</v>
+        <v>7.213819674542174</v>
       </c>
       <c r="AL78">
-        <v>80.82700926961144</v>
+        <v>74.40975860358914</v>
       </c>
       <c r="AN78">
-        <v>5.766370668038726</v>
+        <v>5.620547629725189</v>
       </c>
       <c r="AO78">
-        <v>5.766370668038726</v>
+        <v>5.620547629725189</v>
       </c>
       <c r="AP78">
-        <v>12.42110090942122</v>
+        <v>11.42237053900957</v>
       </c>
       <c r="AQ78">
-        <v>6.67573219994083</v>
+        <v>6.340353480260819</v>
       </c>
       <c r="AR78">
-        <v>6.67573219994083</v>
+        <v>6.340353480260819</v>
       </c>
       <c r="AS78">
-        <v>42.51490652150475</v>
+        <v>47.1778669777466</v>
       </c>
       <c r="AT78">
-        <v>151.1782363720797</v>
+        <v>121.1692079006415</v>
       </c>
       <c r="AU78">
-        <v>151.1782363720797</v>
+        <v>121.1692079006415</v>
       </c>
       <c r="AV78">
-        <v>151.1782363720797</v>
+        <v>121.1692079006415</v>
       </c>
       <c r="AW78">
-        <v>9.796898133307696</v>
+        <v>9.171287022531033</v>
       </c>
       <c r="AX78">
-        <v>31.67221261365339</v>
+        <v>30.8258233175613</v>
       </c>
       <c r="AY78">
-        <v>2.20512321665883</v>
+        <v>2.15244241643697</v>
       </c>
       <c r="AZ78">
-        <v>100.3765526088476</v>
+        <v>94.26668654054404</v>
       </c>
       <c r="BA78">
-        <v>100.3765526088476</v>
+        <v>94.26668654054404</v>
       </c>
       <c r="BB78">
-        <v>100.3765526088476</v>
+        <v>94.26668654054404</v>
       </c>
       <c r="BC78">
-        <v>100.3765526088476</v>
+        <v>94.26668654054404</v>
       </c>
       <c r="BD78">
-        <v>100.3765526088476</v>
+        <v>94.26668654054404</v>
       </c>
       <c r="BE78">
-        <v>2.20512321665883</v>
+        <v>2.15244241643697</v>
       </c>
     </row>
     <row r="79" spans="1:57">
@@ -6238,73 +6238,73 @@
         <v>75</v>
       </c>
       <c r="AH79">
-        <v>11.2832838165015</v>
+        <v>10.65145417792723</v>
       </c>
       <c r="AI79">
-        <v>4.088546174857766</v>
+        <v>4.660319383302704</v>
       </c>
       <c r="AJ79">
-        <v>37.01303481577663</v>
+        <v>39.81580099688144</v>
       </c>
       <c r="AK79">
-        <v>4.088546174857766</v>
+        <v>4.660319383302704</v>
       </c>
       <c r="AL79">
-        <v>37.01303481577663</v>
+        <v>39.81580099688144</v>
       </c>
       <c r="AN79">
-        <v>2.479228200144135</v>
+        <v>2.638983073509298</v>
       </c>
       <c r="AO79">
-        <v>2.479228200144135</v>
+        <v>2.638983073509298</v>
       </c>
       <c r="AP79">
-        <v>2.493765170674306</v>
+        <v>2.937615607588086</v>
       </c>
       <c r="AQ79">
-        <v>1.196790882037021</v>
+        <v>1.239205213543028</v>
       </c>
       <c r="AR79">
-        <v>1.196790882037021</v>
+        <v>1.239205213543028</v>
       </c>
       <c r="AS79">
-        <v>57.29072296076454</v>
+        <v>64.8387075754907</v>
       </c>
       <c r="AT79">
-        <v>382.648740320392</v>
+        <v>415.808921625279</v>
       </c>
       <c r="AU79">
-        <v>382.648740320392</v>
+        <v>415.808921625279</v>
       </c>
       <c r="AV79">
-        <v>382.648740320392</v>
+        <v>415.808921625279</v>
       </c>
       <c r="AW79">
-        <v>6.730584502965212</v>
+        <v>7.183363182842732</v>
       </c>
       <c r="AX79">
-        <v>95.32857898697256</v>
+        <v>100.2953584484756</v>
       </c>
       <c r="AY79">
-        <v>4.416727090328932</v>
+        <v>4.522884311899542</v>
       </c>
       <c r="AZ79">
-        <v>201.1721370059848</v>
+        <v>203.228815502882</v>
       </c>
       <c r="BA79">
-        <v>201.1721370059848</v>
+        <v>203.228815502882</v>
       </c>
       <c r="BB79">
-        <v>201.1721370059848</v>
+        <v>203.228815502882</v>
       </c>
       <c r="BC79">
-        <v>201.1721370059848</v>
+        <v>203.228815502882</v>
       </c>
       <c r="BD79">
-        <v>201.1721370059848</v>
+        <v>203.228815502882</v>
       </c>
       <c r="BE79">
-        <v>4.416727090328932</v>
+        <v>4.522884311899542</v>
       </c>
     </row>
     <row r="80" spans="1:57">
@@ -6312,73 +6312,73 @@
         <v>76</v>
       </c>
       <c r="AH80">
-        <v>12.11434977805242</v>
+        <v>13.45798746185377</v>
       </c>
       <c r="AI80">
-        <v>13.48438005382195</v>
+        <v>14.08343166541308</v>
       </c>
       <c r="AJ80">
-        <v>238.3949724503886</v>
+        <v>243.6396059985738</v>
       </c>
       <c r="AK80">
-        <v>13.48438005382195</v>
+        <v>14.08343166541308</v>
       </c>
       <c r="AL80">
-        <v>238.3949724503886</v>
+        <v>243.6396059985738</v>
       </c>
       <c r="AN80">
-        <v>21.09457629527897</v>
+        <v>21.23328398842365</v>
       </c>
       <c r="AO80">
-        <v>21.09457629527897</v>
+        <v>21.23328398842365</v>
       </c>
       <c r="AP80">
-        <v>29.99180235628039</v>
+        <v>29.97947199227288</v>
       </c>
       <c r="AQ80">
-        <v>10.00633736718446</v>
+        <v>10.14648030120879</v>
       </c>
       <c r="AR80">
-        <v>10.00633736718446</v>
+        <v>10.14648030120879</v>
       </c>
       <c r="AS80">
-        <v>453.513553744331</v>
+        <v>456.9800567036122</v>
       </c>
       <c r="AT80">
-        <v>2402.161853535325</v>
+        <v>2217.601935847849</v>
       </c>
       <c r="AU80">
-        <v>2402.161853535325</v>
+        <v>2217.601935847849</v>
       </c>
       <c r="AV80">
-        <v>2402.161853535325</v>
+        <v>2217.601935847849</v>
       </c>
       <c r="AW80">
-        <v>20.51861240714788</v>
+        <v>20.47749817073345</v>
       </c>
       <c r="AX80">
-        <v>153.9303804054856</v>
+        <v>158.8606877215207</v>
       </c>
       <c r="AY80">
-        <v>7.195476815402507</v>
+        <v>7.524771695435047</v>
       </c>
       <c r="AZ80">
-        <v>440.5391899815799</v>
+        <v>471.0361390480996</v>
       </c>
       <c r="BA80">
-        <v>440.5391899815799</v>
+        <v>471.0361390480996</v>
       </c>
       <c r="BB80">
-        <v>440.5391899815799</v>
+        <v>471.0361390480996</v>
       </c>
       <c r="BC80">
-        <v>440.5391899815799</v>
+        <v>471.0361390480996</v>
       </c>
       <c r="BD80">
-        <v>440.5391899815799</v>
+        <v>471.0361390480996</v>
       </c>
       <c r="BE80">
-        <v>7.195476815402507</v>
+        <v>7.524771695435047</v>
       </c>
     </row>
     <row r="81" spans="1:81">
@@ -6386,73 +6386,73 @@
         <v>77</v>
       </c>
       <c r="AH81">
-        <v>2.714177616508678</v>
+        <v>3.037352387174033</v>
       </c>
       <c r="AI81">
-        <v>2.50873473623069</v>
+        <v>2.217408262763638</v>
       </c>
       <c r="AJ81">
-        <v>50.32512200158322</v>
+        <v>52.46461887568468</v>
       </c>
       <c r="AK81">
-        <v>2.50873473623069</v>
+        <v>2.217408262763638</v>
       </c>
       <c r="AL81">
-        <v>50.32512200158322</v>
+        <v>52.46461887568468</v>
       </c>
       <c r="AN81">
-        <v>2.694804817461409</v>
+        <v>2.566478029908613</v>
       </c>
       <c r="AO81">
-        <v>2.694804817461409</v>
+        <v>2.566478029908613</v>
       </c>
       <c r="AP81">
-        <v>5.961855987883173</v>
+        <v>6.34865314183291</v>
       </c>
       <c r="AQ81">
-        <v>3.61652621650137</v>
+        <v>3.550646647298708</v>
       </c>
       <c r="AR81">
-        <v>3.61652621650137</v>
+        <v>3.550646647298708</v>
       </c>
       <c r="AS81">
-        <v>37.5595741965808</v>
+        <v>35.47821828959975</v>
       </c>
       <c r="AT81">
-        <v>301.6063246752508</v>
+        <v>304.7823744788766</v>
       </c>
       <c r="AU81">
-        <v>301.6063246752508</v>
+        <v>304.7823744788766</v>
       </c>
       <c r="AV81">
-        <v>301.6063246752508</v>
+        <v>304.7823744788766</v>
       </c>
       <c r="AW81">
-        <v>5.515517091006041</v>
+        <v>5.122214941680432</v>
       </c>
       <c r="AX81">
-        <v>37.27662544269115</v>
+        <v>35.88583554206416</v>
       </c>
       <c r="AY81">
-        <v>1.983568638414144</v>
+        <v>2.002981155142188</v>
       </c>
       <c r="AZ81">
-        <v>81.64394999697805</v>
+        <v>80.71584402132035</v>
       </c>
       <c r="BA81">
-        <v>81.64394999697805</v>
+        <v>80.71584402132035</v>
       </c>
       <c r="BB81">
-        <v>81.64394999697805</v>
+        <v>80.71584402132035</v>
       </c>
       <c r="BC81">
-        <v>81.64394999697805</v>
+        <v>80.71584402132035</v>
       </c>
       <c r="BD81">
-        <v>81.64394999697805</v>
+        <v>80.71584402132035</v>
       </c>
       <c r="BE81">
-        <v>1.983568638414144</v>
+        <v>2.002981155142188</v>
       </c>
     </row>
     <row r="82" spans="1:81">

</xml_diff>

<commit_message>
now removes old Labour rows
</commit_message>
<xml_diff>
--- a/excel_files/output.xlsx
+++ b/excel_files/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5544" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5472" uniqueCount="85">
   <si>
     <t>AT</t>
   </si>
@@ -259,9 +259,6 @@
     <t>Labour 233</t>
   </si>
   <si>
-    <t>Labour</t>
-  </si>
-  <si>
     <t>Capital</t>
   </si>
   <si>
@@ -269,6 +266,9 @@
   </si>
   <si>
     <t>tax_com</t>
+  </si>
+  <si>
+    <t>Labour</t>
   </si>
 </sst>
 </file>
@@ -600,7 +600,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1848"/>
+  <dimension ref="A1:D1824"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -17750,7 +17750,7 @@
         <v>57</v>
       </c>
       <c r="C1225" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D1225">
         <v>131530.1</v>
@@ -17764,7 +17764,7 @@
         <v>57</v>
       </c>
       <c r="C1226" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D1226">
         <v>112199.01</v>
@@ -17792,7 +17792,7 @@
         <v>58</v>
       </c>
       <c r="C1228" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D1228">
         <v>4774.3</v>
@@ -17806,7 +17806,7 @@
         <v>58</v>
       </c>
       <c r="C1229" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D1229">
         <v>9930.33</v>
@@ -24781,7 +24781,7 @@
         <v>33</v>
       </c>
       <c r="D1727">
-        <v>606.71</v>
+        <v>5167.79</v>
       </c>
     </row>
     <row r="1728" spans="1:4">
@@ -24795,7 +24795,7 @@
         <v>34</v>
       </c>
       <c r="D1728">
-        <v>2.48</v>
+        <v>7.13</v>
       </c>
     </row>
     <row r="1729" spans="1:4">
@@ -24809,7 +24809,7 @@
         <v>35</v>
       </c>
       <c r="D1729">
-        <v>288.04</v>
+        <v>673.79</v>
       </c>
     </row>
     <row r="1730" spans="1:4">
@@ -24823,7 +24823,7 @@
         <v>36</v>
       </c>
       <c r="D1730">
-        <v>1467.42</v>
+        <v>1611.53</v>
       </c>
     </row>
     <row r="1731" spans="1:4">
@@ -24837,7 +24837,7 @@
         <v>37</v>
       </c>
       <c r="D1731">
-        <v>25315.67</v>
+        <v>19997.65</v>
       </c>
     </row>
     <row r="1732" spans="1:4">
@@ -24851,7 +24851,7 @@
         <v>38</v>
       </c>
       <c r="D1732">
-        <v>496.89</v>
+        <v>723.73</v>
       </c>
     </row>
     <row r="1733" spans="1:4">
@@ -24865,7 +24865,7 @@
         <v>39</v>
       </c>
       <c r="D1733">
-        <v>115.12</v>
+        <v>67.78</v>
       </c>
     </row>
     <row r="1734" spans="1:4">
@@ -24879,7 +24879,7 @@
         <v>40</v>
       </c>
       <c r="D1734">
-        <v>464.11</v>
+        <v>703.41</v>
       </c>
     </row>
     <row r="1735" spans="1:4">
@@ -24893,7 +24893,7 @@
         <v>41</v>
       </c>
       <c r="D1735">
-        <v>1077.97</v>
+        <v>2397.43</v>
       </c>
     </row>
     <row r="1736" spans="1:4">
@@ -24907,7 +24907,7 @@
         <v>42</v>
       </c>
       <c r="D1736">
-        <v>238.76</v>
+        <v>79.59999999999999</v>
       </c>
     </row>
     <row r="1737" spans="1:4">
@@ -24921,7 +24921,7 @@
         <v>43</v>
       </c>
       <c r="D1737">
-        <v>10.19</v>
+        <v>6.37</v>
       </c>
     </row>
     <row r="1738" spans="1:4">
@@ -24935,7 +24935,7 @@
         <v>44</v>
       </c>
       <c r="D1738">
-        <v>6546.59</v>
+        <v>5650.28</v>
       </c>
     </row>
     <row r="1739" spans="1:4">
@@ -24949,7 +24949,7 @@
         <v>45</v>
       </c>
       <c r="D1739">
-        <v>9171.24</v>
+        <v>7547.66</v>
       </c>
     </row>
     <row r="1740" spans="1:4">
@@ -24963,7 +24963,7 @@
         <v>46</v>
       </c>
       <c r="D1740">
-        <v>16888.18</v>
+        <v>13791.83</v>
       </c>
     </row>
     <row r="1741" spans="1:4">
@@ -24977,7 +24977,7 @@
         <v>47</v>
       </c>
       <c r="D1741">
-        <v>39974.96</v>
+        <v>47294.49</v>
       </c>
     </row>
     <row r="1742" spans="1:4">
@@ -24991,7 +24991,7 @@
         <v>48</v>
       </c>
       <c r="D1742">
-        <v>350.8</v>
+        <v>941.97</v>
       </c>
     </row>
     <row r="1743" spans="1:4">
@@ -25005,7 +25005,7 @@
         <v>49</v>
       </c>
       <c r="D1743">
-        <v>3612.7</v>
+        <v>1072.71</v>
       </c>
     </row>
     <row r="1744" spans="1:4">
@@ -25019,7 +25019,7 @@
         <v>50</v>
       </c>
       <c r="D1744">
-        <v>172.44</v>
+        <v>208.05</v>
       </c>
     </row>
     <row r="1745" spans="1:4">
@@ -25033,7 +25033,7 @@
         <v>51</v>
       </c>
       <c r="D1745">
-        <v>1.93</v>
+        <v>2.61</v>
       </c>
     </row>
     <row r="1746" spans="1:4">
@@ -25047,7 +25047,7 @@
         <v>52</v>
       </c>
       <c r="D1746">
-        <v>14.36</v>
+        <v>20.59</v>
       </c>
     </row>
     <row r="1747" spans="1:4">
@@ -25061,7 +25061,7 @@
         <v>53</v>
       </c>
       <c r="D1747">
-        <v>507.79</v>
+        <v>397.37</v>
       </c>
     </row>
     <row r="1748" spans="1:4">
@@ -25075,7 +25075,7 @@
         <v>54</v>
       </c>
       <c r="D1748">
-        <v>23024.77</v>
+        <v>2884.17</v>
       </c>
     </row>
     <row r="1749" spans="1:4">
@@ -25089,7 +25089,7 @@
         <v>55</v>
       </c>
       <c r="D1749">
-        <v>1162.91</v>
+        <v>936.51</v>
       </c>
     </row>
     <row r="1750" spans="1:4">
@@ -25103,7 +25103,7 @@
         <v>56</v>
       </c>
       <c r="D1750">
-        <v>18.08</v>
+        <v>14.56</v>
       </c>
     </row>
     <row r="1751" spans="1:4">
@@ -25117,7 +25117,7 @@
         <v>33</v>
       </c>
       <c r="D1751">
-        <v>5167.79</v>
+        <v>7.28</v>
       </c>
     </row>
     <row r="1752" spans="1:4">
@@ -25128,10 +25128,10 @@
         <v>82</v>
       </c>
       <c r="C1752" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D1752">
-        <v>7.13</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="1753" spans="1:4">
@@ -25142,10 +25142,10 @@
         <v>82</v>
       </c>
       <c r="C1753" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D1753">
-        <v>673.79</v>
+        <v>50.76</v>
       </c>
     </row>
     <row r="1754" spans="1:4">
@@ -25156,10 +25156,10 @@
         <v>82</v>
       </c>
       <c r="C1754" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D1754">
-        <v>1611.53</v>
+        <v>660.9299999999999</v>
       </c>
     </row>
     <row r="1755" spans="1:4">
@@ -25170,10 +25170,10 @@
         <v>82</v>
       </c>
       <c r="C1755" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D1755">
-        <v>19997.65</v>
+        <v>15.33</v>
       </c>
     </row>
     <row r="1756" spans="1:4">
@@ -25184,10 +25184,10 @@
         <v>82</v>
       </c>
       <c r="C1756" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D1756">
-        <v>723.73</v>
+        <v>7.13</v>
       </c>
     </row>
     <row r="1757" spans="1:4">
@@ -25198,10 +25198,10 @@
         <v>82</v>
       </c>
       <c r="C1757" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D1757">
-        <v>67.78</v>
+        <v>30.73</v>
       </c>
     </row>
     <row r="1758" spans="1:4">
@@ -25212,10 +25212,10 @@
         <v>82</v>
       </c>
       <c r="C1758" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D1758">
-        <v>703.41</v>
+        <v>96.58</v>
       </c>
     </row>
     <row r="1759" spans="1:4">
@@ -25226,10 +25226,10 @@
         <v>82</v>
       </c>
       <c r="C1759" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D1759">
-        <v>2397.43</v>
+        <v>13.3</v>
       </c>
     </row>
     <row r="1760" spans="1:4">
@@ -25240,10 +25240,10 @@
         <v>82</v>
       </c>
       <c r="C1760" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D1760">
-        <v>79.59999999999999</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="1761" spans="1:4">
@@ -25254,10 +25254,10 @@
         <v>82</v>
       </c>
       <c r="C1761" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D1761">
-        <v>6.37</v>
+        <v>268.63</v>
       </c>
     </row>
     <row r="1762" spans="1:4">
@@ -25268,10 +25268,10 @@
         <v>82</v>
       </c>
       <c r="C1762" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D1762">
-        <v>5650.28</v>
+        <v>397.03</v>
       </c>
     </row>
     <row r="1763" spans="1:4">
@@ -25282,10 +25282,10 @@
         <v>82</v>
       </c>
       <c r="C1763" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D1763">
-        <v>7547.66</v>
+        <v>664.72</v>
       </c>
     </row>
     <row r="1764" spans="1:4">
@@ -25296,10 +25296,10 @@
         <v>82</v>
       </c>
       <c r="C1764" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D1764">
-        <v>13791.83</v>
+        <v>1652.9</v>
       </c>
     </row>
     <row r="1765" spans="1:4">
@@ -25310,10 +25310,10 @@
         <v>82</v>
       </c>
       <c r="C1765" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D1765">
-        <v>47294.49</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="1766" spans="1:4">
@@ -25324,10 +25324,10 @@
         <v>82</v>
       </c>
       <c r="C1766" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D1766">
-        <v>941.97</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="1767" spans="1:4">
@@ -25338,10 +25338,10 @@
         <v>82</v>
       </c>
       <c r="C1767" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D1767">
-        <v>1072.71</v>
+        <v>27.2</v>
       </c>
     </row>
     <row r="1768" spans="1:4">
@@ -25352,10 +25352,10 @@
         <v>82</v>
       </c>
       <c r="C1768" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D1768">
-        <v>208.05</v>
+        <v>820.11</v>
       </c>
     </row>
     <row r="1769" spans="1:4">
@@ -25366,10 +25366,10 @@
         <v>82</v>
       </c>
       <c r="C1769" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D1769">
-        <v>2.61</v>
+        <v>59.18</v>
       </c>
     </row>
     <row r="1770" spans="1:4">
@@ -25380,10 +25380,10 @@
         <v>82</v>
       </c>
       <c r="C1770" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D1770">
-        <v>20.59</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="1771" spans="1:4">
@@ -25391,13 +25391,13 @@
         <v>0</v>
       </c>
       <c r="B1771" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C1771" t="s">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="D1771">
-        <v>397.37</v>
+        <v>227.52</v>
       </c>
     </row>
     <row r="1772" spans="1:4">
@@ -25405,13 +25405,13 @@
         <v>0</v>
       </c>
       <c r="B1772" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C1772" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
       <c r="D1772">
-        <v>2884.17</v>
+        <v>74.33</v>
       </c>
     </row>
     <row r="1773" spans="1:4">
@@ -25419,13 +25419,13 @@
         <v>0</v>
       </c>
       <c r="B1773" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C1773" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="D1773">
-        <v>936.51</v>
+        <v>2319.47</v>
       </c>
     </row>
     <row r="1774" spans="1:4">
@@ -25433,13 +25433,13 @@
         <v>0</v>
       </c>
       <c r="B1774" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C1774" t="s">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="D1774">
-        <v>14.56</v>
+        <v>186.97</v>
       </c>
     </row>
     <row r="1775" spans="1:4">
@@ -25450,10 +25450,10 @@
         <v>83</v>
       </c>
       <c r="C1775" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="D1775">
-        <v>7.28</v>
+        <v>5.96</v>
       </c>
     </row>
     <row r="1776" spans="1:4">
@@ -25464,10 +25464,10 @@
         <v>83</v>
       </c>
       <c r="C1776" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="D1776">
-        <v>0.16</v>
+        <v>109.87</v>
       </c>
     </row>
     <row r="1777" spans="1:4">
@@ -25478,10 +25478,10 @@
         <v>83</v>
       </c>
       <c r="C1777" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="D1777">
-        <v>50.76</v>
+        <v>99.19</v>
       </c>
     </row>
     <row r="1778" spans="1:4">
@@ -25492,10 +25492,10 @@
         <v>83</v>
       </c>
       <c r="C1778" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="D1778">
-        <v>660.9299999999999</v>
+        <v>558.99</v>
       </c>
     </row>
     <row r="1779" spans="1:4">
@@ -25506,10 +25506,10 @@
         <v>83</v>
       </c>
       <c r="C1779" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="D1779">
-        <v>15.33</v>
+        <v>41.54</v>
       </c>
     </row>
     <row r="1780" spans="1:4">
@@ -25520,10 +25520,10 @@
         <v>83</v>
       </c>
       <c r="C1780" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="D1780">
-        <v>7.13</v>
+        <v>433.29</v>
       </c>
     </row>
     <row r="1781" spans="1:4">
@@ -25534,10 +25534,10 @@
         <v>83</v>
       </c>
       <c r="C1781" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="D1781">
-        <v>30.73</v>
+        <v>580.78</v>
       </c>
     </row>
     <row r="1782" spans="1:4">
@@ -25548,10 +25548,10 @@
         <v>83</v>
       </c>
       <c r="C1782" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="D1782">
-        <v>96.58</v>
+        <v>765.54</v>
       </c>
     </row>
     <row r="1783" spans="1:4">
@@ -25562,10 +25562,10 @@
         <v>83</v>
       </c>
       <c r="C1783" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="D1783">
-        <v>13.3</v>
+        <v>3251.01</v>
       </c>
     </row>
     <row r="1784" spans="1:4">
@@ -25576,10 +25576,10 @@
         <v>83</v>
       </c>
       <c r="C1784" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D1784">
-        <v>0.71</v>
+        <v>53.1</v>
       </c>
     </row>
     <row r="1785" spans="1:4">
@@ -25590,10 +25590,10 @@
         <v>83</v>
       </c>
       <c r="C1785" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="D1785">
-        <v>268.63</v>
+        <v>216.04</v>
       </c>
     </row>
     <row r="1786" spans="1:4">
@@ -25604,10 +25604,10 @@
         <v>83</v>
       </c>
       <c r="C1786" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="D1786">
-        <v>397.03</v>
+        <v>5.88</v>
       </c>
     </row>
     <row r="1787" spans="1:4">
@@ -25618,10 +25618,10 @@
         <v>83</v>
       </c>
       <c r="C1787" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="D1787">
-        <v>664.72</v>
+        <v>76.8</v>
       </c>
     </row>
     <row r="1788" spans="1:4">
@@ -25632,10 +25632,10 @@
         <v>83</v>
       </c>
       <c r="C1788" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="D1788">
-        <v>1652.9</v>
+        <v>174.74</v>
       </c>
     </row>
     <row r="1789" spans="1:4">
@@ -25646,10 +25646,10 @@
         <v>83</v>
       </c>
       <c r="C1789" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="D1789">
-        <v>0.09</v>
+        <v>21.43</v>
       </c>
     </row>
     <row r="1790" spans="1:4">
@@ -25660,10 +25660,10 @@
         <v>83</v>
       </c>
       <c r="C1790" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="D1790">
-        <v>0.63</v>
+        <v>42.26</v>
       </c>
     </row>
     <row r="1791" spans="1:4">
@@ -25674,10 +25674,10 @@
         <v>83</v>
       </c>
       <c r="C1791" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="D1791">
-        <v>27.2</v>
+        <v>51.85</v>
       </c>
     </row>
     <row r="1792" spans="1:4">
@@ -25688,10 +25688,10 @@
         <v>83</v>
       </c>
       <c r="C1792" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="D1792">
-        <v>820.11</v>
+        <v>19.07</v>
       </c>
     </row>
     <row r="1793" spans="1:4">
@@ -25702,10 +25702,10 @@
         <v>83</v>
       </c>
       <c r="C1793" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="D1793">
-        <v>59.18</v>
+        <v>19.84</v>
       </c>
     </row>
     <row r="1794" spans="1:4">
@@ -25716,10 +25716,10 @@
         <v>83</v>
       </c>
       <c r="C1794" t="s">
-        <v>56</v>
+        <v>24</v>
       </c>
       <c r="D1794">
-        <v>0.91</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="1795" spans="1:4">
@@ -25727,13 +25727,13 @@
         <v>0</v>
       </c>
       <c r="B1795" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C1795" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="D1795">
-        <v>227.52</v>
+        <v>117.44</v>
       </c>
     </row>
     <row r="1796" spans="1:4">
@@ -25741,13 +25741,13 @@
         <v>0</v>
       </c>
       <c r="B1796" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C1796" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="D1796">
-        <v>74.33</v>
+        <v>12.27</v>
       </c>
     </row>
     <row r="1797" spans="1:4">
@@ -25755,13 +25755,13 @@
         <v>0</v>
       </c>
       <c r="B1797" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C1797" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="D1797">
-        <v>2319.47</v>
+        <v>4.69</v>
       </c>
     </row>
     <row r="1798" spans="1:4">
@@ -25769,13 +25769,13 @@
         <v>0</v>
       </c>
       <c r="B1798" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C1798" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="D1798">
-        <v>186.97</v>
+        <v>330.19</v>
       </c>
     </row>
     <row r="1799" spans="1:4">
@@ -25783,13 +25783,13 @@
         <v>0</v>
       </c>
       <c r="B1799" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C1799" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="D1799">
-        <v>5.96</v>
+        <v>33.42</v>
       </c>
     </row>
     <row r="1800" spans="1:4">
@@ -25797,13 +25797,13 @@
         <v>0</v>
       </c>
       <c r="B1800" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C1800" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D1800">
-        <v>109.87</v>
+        <v>4.14</v>
       </c>
     </row>
     <row r="1801" spans="1:4">
@@ -25811,13 +25811,13 @@
         <v>0</v>
       </c>
       <c r="B1801" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C1801" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="D1801">
-        <v>99.19</v>
+        <v>92.26000000000001</v>
       </c>
     </row>
     <row r="1802" spans="1:4">
@@ -25825,13 +25825,13 @@
         <v>0</v>
       </c>
       <c r="B1802" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C1802" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="D1802">
-        <v>558.99</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1803" spans="1:4">
@@ -25839,13 +25839,13 @@
         <v>0</v>
       </c>
       <c r="B1803" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C1803" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="D1803">
-        <v>41.54</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1804" spans="1:4">
@@ -25853,13 +25853,13 @@
         <v>0</v>
       </c>
       <c r="B1804" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C1804" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="D1804">
-        <v>433.29</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1805" spans="1:4">
@@ -25867,13 +25867,13 @@
         <v>0</v>
       </c>
       <c r="B1805" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C1805" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="D1805">
-        <v>580.78</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1806" spans="1:4">
@@ -25881,13 +25881,13 @@
         <v>0</v>
       </c>
       <c r="B1806" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C1806" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="D1806">
-        <v>765.54</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1807" spans="1:4">
@@ -25895,13 +25895,13 @@
         <v>0</v>
       </c>
       <c r="B1807" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C1807" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="D1807">
-        <v>3251.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1808" spans="1:4">
@@ -25909,13 +25909,13 @@
         <v>0</v>
       </c>
       <c r="B1808" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C1808" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="D1808">
-        <v>53.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1809" spans="1:4">
@@ -25923,13 +25923,13 @@
         <v>0</v>
       </c>
       <c r="B1809" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C1809" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="D1809">
-        <v>216.04</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1810" spans="1:4">
@@ -25937,13 +25937,13 @@
         <v>0</v>
       </c>
       <c r="B1810" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C1810" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="D1810">
-        <v>5.88</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1811" spans="1:4">
@@ -25951,13 +25951,13 @@
         <v>0</v>
       </c>
       <c r="B1811" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C1811" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="D1811">
-        <v>76.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1812" spans="1:4">
@@ -25965,13 +25965,13 @@
         <v>0</v>
       </c>
       <c r="B1812" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C1812" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="D1812">
-        <v>174.74</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1813" spans="1:4">
@@ -25979,13 +25979,13 @@
         <v>0</v>
       </c>
       <c r="B1813" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C1813" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="D1813">
-        <v>21.43</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1814" spans="1:4">
@@ -25993,13 +25993,13 @@
         <v>0</v>
       </c>
       <c r="B1814" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C1814" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="D1814">
-        <v>42.26</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1815" spans="1:4">
@@ -26007,13 +26007,13 @@
         <v>0</v>
       </c>
       <c r="B1815" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C1815" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="D1815">
-        <v>51.85</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1816" spans="1:4">
@@ -26021,13 +26021,13 @@
         <v>0</v>
       </c>
       <c r="B1816" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C1816" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="D1816">
-        <v>19.07</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1817" spans="1:4">
@@ -26035,13 +26035,13 @@
         <v>0</v>
       </c>
       <c r="B1817" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C1817" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="D1817">
-        <v>19.84</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1818" spans="1:4">
@@ -26049,13 +26049,13 @@
         <v>0</v>
       </c>
       <c r="B1818" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C1818" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="D1818">
-        <v>0.44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1819" spans="1:4">
@@ -26063,13 +26063,13 @@
         <v>0</v>
       </c>
       <c r="B1819" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C1819" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="D1819">
-        <v>117.44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1820" spans="1:4">
@@ -26077,13 +26077,13 @@
         <v>0</v>
       </c>
       <c r="B1820" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C1820" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="D1820">
-        <v>12.27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1821" spans="1:4">
@@ -26091,13 +26091,13 @@
         <v>0</v>
       </c>
       <c r="B1821" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C1821" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="D1821">
-        <v>4.69</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1822" spans="1:4">
@@ -26105,13 +26105,13 @@
         <v>0</v>
       </c>
       <c r="B1822" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C1822" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="D1822">
-        <v>330.19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1823" spans="1:4">
@@ -26119,13 +26119,13 @@
         <v>0</v>
       </c>
       <c r="B1823" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C1823" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="D1823">
-        <v>33.42</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1824" spans="1:4">
@@ -26133,348 +26133,12 @@
         <v>0</v>
       </c>
       <c r="B1824" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C1824" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
       <c r="D1824">
-        <v>4.14</v>
-      </c>
-    </row>
-    <row r="1825" spans="1:4">
-      <c r="A1825" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1825" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1825" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1825">
-        <v>92.26000000000001</v>
-      </c>
-    </row>
-    <row r="1826" spans="1:4">
-      <c r="A1826" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1826" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1826" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1826">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1827" spans="1:4">
-      <c r="A1827" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1827" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1827" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1827">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1828" spans="1:4">
-      <c r="A1828" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1828" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1828" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1828">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1829" spans="1:4">
-      <c r="A1829" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1829" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1829" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1829">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1830" spans="1:4">
-      <c r="A1830" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1830" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1830" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1830">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1831" spans="1:4">
-      <c r="A1831" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1831" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1831" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1831">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1832" spans="1:4">
-      <c r="A1832" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1832" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1832" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1832">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1833" spans="1:4">
-      <c r="A1833" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1833" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1833" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1833">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1834" spans="1:4">
-      <c r="A1834" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1834" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1834" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1834">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1835" spans="1:4">
-      <c r="A1835" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1835" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1835" t="s">
-        <v>46</v>
-      </c>
-      <c r="D1835">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1836" spans="1:4">
-      <c r="A1836" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1836" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1836" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1836">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1837" spans="1:4">
-      <c r="A1837" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1837" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1837" t="s">
-        <v>48</v>
-      </c>
-      <c r="D1837">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1838" spans="1:4">
-      <c r="A1838" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1838" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1838" t="s">
-        <v>49</v>
-      </c>
-      <c r="D1838">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1839" spans="1:4">
-      <c r="A1839" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1839" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1839" t="s">
-        <v>53</v>
-      </c>
-      <c r="D1839">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1840" spans="1:4">
-      <c r="A1840" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1840" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1840" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1840">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1841" spans="1:4">
-      <c r="A1841" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1841" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1841" t="s">
-        <v>56</v>
-      </c>
-      <c r="D1841">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1842" spans="1:4">
-      <c r="A1842" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1842" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1842" t="s">
-        <v>57</v>
-      </c>
-      <c r="D1842">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1843" spans="1:4">
-      <c r="A1843" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1843" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1843" t="s">
-        <v>58</v>
-      </c>
-      <c r="D1843">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1844" spans="1:4">
-      <c r="A1844" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1844" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1844" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1844">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1845" spans="1:4">
-      <c r="A1845" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1845" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1845" t="s">
-        <v>60</v>
-      </c>
-      <c r="D1845">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1846" spans="1:4">
-      <c r="A1846" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1846" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1846" t="s">
-        <v>61</v>
-      </c>
-      <c r="D1846">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1847" spans="1:4">
-      <c r="A1847" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1847" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1847" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1847">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1848" spans="1:4">
-      <c r="A1848" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1848" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1848" t="s">
-        <v>82</v>
-      </c>
-      <c r="D1848">
         <v>0</v>
       </c>
     </row>

</xml_diff>